<commit_message>
corretto il meccanismo che genera Terminologia_glossario
</commit_message>
<xml_diff>
--- a/static/saved_dataframes/Elab1.xlsx
+++ b/static/saved_dataframes/Elab1.xlsx
@@ -362,7 +362,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AE78"/>
+  <dimension ref="A1:AE77"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2957,7 +2957,7 @@
         <v>2000001</v>
       </c>
       <c r="D26" t="n">
-        <v>3000025</v>
+        <v>3000026</v>
       </c>
       <c r="E26" t="n">
         <v>4000019</v>
@@ -2966,7 +2966,7 @@
         <v>5000001</v>
       </c>
       <c r="G26" t="n">
-        <v>6000025</v>
+        <v>6000026</v>
       </c>
       <c r="H26" t="n">
         <v>7000024</v>
@@ -3058,16 +3058,16 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>1000026</v>
+        <v>1000025</v>
       </c>
       <c r="C27" t="n">
         <v>2000001</v>
       </c>
       <c r="D27" t="n">
-        <v>3000026</v>
+        <v>3000025</v>
       </c>
       <c r="E27" t="n">
-        <v>4000026</v>
+        <v>4000025</v>
       </c>
       <c r="F27" t="n">
         <v>5000001</v>
@@ -3079,16 +3079,16 @@
         <v>7000001</v>
       </c>
       <c r="I27" t="n">
-        <v>8000026</v>
+        <v>8000025</v>
       </c>
       <c r="J27" t="n">
         <v>9000003</v>
       </c>
       <c r="K27" t="n">
-        <v>10000026</v>
+        <v>10000025</v>
       </c>
       <c r="L27" t="n">
-        <v>11000026</v>
+        <v>11000025</v>
       </c>
       <c r="M27" t="n">
         <v>12000001</v>
@@ -3104,7 +3104,7 @@
       </c>
       <c r="Q27" t="inlineStr">
         <is>
-          <t>Evento NBC - settore B</t>
+          <t>Emergenza Di Tipo B</t>
         </is>
       </c>
       <c r="R27" t="inlineStr"/>
@@ -3894,13 +3894,13 @@
         <v>33</v>
       </c>
       <c r="B35" t="n">
-        <v>1000039</v>
+        <v>1000034</v>
       </c>
       <c r="C35" t="n">
         <v>2000001</v>
       </c>
       <c r="D35" t="n">
-        <v>3000039</v>
+        <v>3000034</v>
       </c>
       <c r="E35" t="n">
         <v>4000001</v>
@@ -3915,22 +3915,22 @@
         <v>7000001</v>
       </c>
       <c r="I35" t="n">
-        <v>8000039</v>
+        <v>8000034</v>
       </c>
       <c r="J35" t="n">
         <v>9000003</v>
       </c>
       <c r="K35" t="n">
-        <v>10000035</v>
+        <v>10000034</v>
       </c>
       <c r="L35" t="n">
-        <v>11000039</v>
+        <v>11000034</v>
       </c>
       <c r="M35" t="n">
         <v>12000001</v>
       </c>
       <c r="N35" t="n">
-        <v>13000035</v>
+        <v>13000034</v>
       </c>
       <c r="O35" t="n">
         <v>14000034</v>
@@ -3989,13 +3989,13 @@
         <v>34</v>
       </c>
       <c r="B36" t="n">
-        <v>1000035</v>
+        <v>1000037</v>
       </c>
       <c r="C36" t="n">
         <v>2000001</v>
       </c>
       <c r="D36" t="n">
-        <v>3000035</v>
+        <v>3000037</v>
       </c>
       <c r="E36" t="n">
         <v>4000001</v>
@@ -4010,22 +4010,22 @@
         <v>7000001</v>
       </c>
       <c r="I36" t="n">
-        <v>8000035</v>
+        <v>8000037</v>
       </c>
       <c r="J36" t="n">
         <v>9000003</v>
       </c>
       <c r="K36" t="n">
-        <v>10000035</v>
+        <v>10000034</v>
       </c>
       <c r="L36" t="n">
-        <v>11000035</v>
+        <v>11000037</v>
       </c>
       <c r="M36" t="n">
         <v>12000001</v>
       </c>
       <c r="N36" t="n">
-        <v>13000035</v>
+        <v>13000034</v>
       </c>
       <c r="O36" t="n">
         <v>14000034</v>
@@ -4084,13 +4084,13 @@
         <v>35</v>
       </c>
       <c r="B37" t="n">
-        <v>1000036</v>
+        <v>1000038</v>
       </c>
       <c r="C37" t="n">
         <v>2000001</v>
       </c>
       <c r="D37" t="n">
-        <v>3000036</v>
+        <v>3000038</v>
       </c>
       <c r="E37" t="n">
         <v>4000001</v>
@@ -4105,22 +4105,22 @@
         <v>7000001</v>
       </c>
       <c r="I37" t="n">
-        <v>8000036</v>
+        <v>8000038</v>
       </c>
       <c r="J37" t="n">
         <v>9000003</v>
       </c>
       <c r="K37" t="n">
-        <v>10000036</v>
+        <v>10000038</v>
       </c>
       <c r="L37" t="n">
-        <v>11000036</v>
+        <v>11000038</v>
       </c>
       <c r="M37" t="n">
         <v>12000001</v>
       </c>
       <c r="N37" t="n">
-        <v>13000036</v>
+        <v>13000038</v>
       </c>
       <c r="O37" t="n">
         <v>14000034</v>
@@ -4184,13 +4184,13 @@
         <v>36</v>
       </c>
       <c r="B38" t="n">
-        <v>1000034</v>
+        <v>1000036</v>
       </c>
       <c r="C38" t="n">
         <v>2000001</v>
       </c>
       <c r="D38" t="n">
-        <v>3000034</v>
+        <v>3000036</v>
       </c>
       <c r="E38" t="n">
         <v>4000001</v>
@@ -4208,7 +4208,7 @@
         <v>8000032</v>
       </c>
       <c r="J38" t="n">
-        <v>9000034</v>
+        <v>9000003</v>
       </c>
       <c r="K38" t="n">
         <v>10000032</v>
@@ -4220,7 +4220,7 @@
         <v>12000001</v>
       </c>
       <c r="N38" t="n">
-        <v>13000034</v>
+        <v>13000036</v>
       </c>
       <c r="O38" t="n">
         <v>14000034</v>
@@ -4230,13 +4230,13 @@
       </c>
       <c r="Q38" t="inlineStr">
         <is>
-          <t>Vigili del fuoco</t>
+          <t>Nucleo Unitario di Valutazione e Risposta Emergenze transfrontaliere</t>
         </is>
       </c>
       <c r="R38" t="inlineStr"/>
       <c r="S38" t="inlineStr">
         <is>
-          <t>Struttura operativa della protezione civile.</t>
+          <t>team transfrontaliero di coordinamento costituito congiuntamente da personale qualificato, formato e attrezzato, della protezione civile lombarda e ticinese. Esso ha il compito, durante le emergenze nei territori di confine, di operare insieme sia per la valutazione dell’evento in corso e per i reciproci possibili riflessi sui rispettivi territori, sia quali “ufficiali di collegamento” per collegare le rispettive sale operative di ambo i lati del confine, consentendo una efficiente ed efficace relazione operativa. Il NUVRE viene introdotto dal progetto Gestisco 2018-2021.</t>
         </is>
       </c>
       <c r="T38" t="inlineStr"/>
@@ -4244,16 +4244,12 @@
       <c r="V38" t="inlineStr"/>
       <c r="W38" t="inlineStr"/>
       <c r="X38" t="inlineStr"/>
-      <c r="Y38" t="inlineStr">
-        <is>
-          <t>Alberto Bruno, Funzionario della protezione civile di regione lombardia</t>
-        </is>
-      </c>
+      <c r="Y38" t="inlineStr"/>
       <c r="Z38" t="inlineStr"/>
       <c r="AA38" t="inlineStr"/>
       <c r="AB38" t="inlineStr"/>
       <c r="AC38" s="2" t="n">
-        <v>43804</v>
+        <v>43774</v>
       </c>
       <c r="AD38" t="inlineStr">
         <is>
@@ -4271,13 +4267,13 @@
         <v>37</v>
       </c>
       <c r="B39" t="n">
-        <v>1000037</v>
+        <v>1000035</v>
       </c>
       <c r="C39" t="n">
         <v>2000001</v>
       </c>
       <c r="D39" t="n">
-        <v>3000037</v>
+        <v>3000035</v>
       </c>
       <c r="E39" t="n">
         <v>4000001</v>
@@ -4295,7 +4291,7 @@
         <v>8000032</v>
       </c>
       <c r="J39" t="n">
-        <v>9000003</v>
+        <v>9000035</v>
       </c>
       <c r="K39" t="n">
         <v>10000032</v>
@@ -4307,7 +4303,7 @@
         <v>12000001</v>
       </c>
       <c r="N39" t="n">
-        <v>13000037</v>
+        <v>13000035</v>
       </c>
       <c r="O39" t="n">
         <v>14000034</v>
@@ -4317,13 +4313,13 @@
       </c>
       <c r="Q39" t="inlineStr">
         <is>
-          <t>Nucleo Unitario di Valutazione e Risposta Emergenze transfrontaliere</t>
+          <t>Vigili del fuoco</t>
         </is>
       </c>
       <c r="R39" t="inlineStr"/>
       <c r="S39" t="inlineStr">
         <is>
-          <t>team transfrontaliero di coordinamento costituito congiuntamente da personale qualificato, formato e attrezzato, della protezione civile lombarda e ticinese. Esso ha il compito, durante le emergenze nei territori di confine, di operare insieme sia per la valutazione dell’evento in corso e per i reciproci possibili riflessi sui rispettivi territori, sia quali “ufficiali di collegamento” per collegare le rispettive sale operative di ambo i lati del confine, consentendo una efficiente ed efficace relazione operativa. Il NUVRE viene introdotto dal progetto Gestisco 2018-2021.</t>
+          <t>Struttura operativa della protezione civile.</t>
         </is>
       </c>
       <c r="T39" t="inlineStr"/>
@@ -4331,12 +4327,16 @@
       <c r="V39" t="inlineStr"/>
       <c r="W39" t="inlineStr"/>
       <c r="X39" t="inlineStr"/>
-      <c r="Y39" t="inlineStr"/>
+      <c r="Y39" t="inlineStr">
+        <is>
+          <t>Alberto Bruno, Funzionario della protezione civile di regione lombardia</t>
+        </is>
+      </c>
       <c r="Z39" t="inlineStr"/>
       <c r="AA39" t="inlineStr"/>
       <c r="AB39" t="inlineStr"/>
       <c r="AC39" s="2" t="n">
-        <v>43774</v>
+        <v>43804</v>
       </c>
       <c r="AD39" t="inlineStr">
         <is>
@@ -4354,16 +4354,16 @@
         <v>38</v>
       </c>
       <c r="B40" t="n">
-        <v>1000038</v>
+        <v>1000039</v>
       </c>
       <c r="C40" t="n">
         <v>2000001</v>
       </c>
       <c r="D40" t="n">
-        <v>3000038</v>
+        <v>3000039</v>
       </c>
       <c r="E40" t="n">
-        <v>4000001</v>
+        <v>4000019</v>
       </c>
       <c r="F40" t="n">
         <v>5000001</v>
@@ -4375,51 +4375,71 @@
         <v>7000001</v>
       </c>
       <c r="I40" t="n">
-        <v>8000032</v>
+        <v>8000015</v>
       </c>
       <c r="J40" t="n">
         <v>9000003</v>
       </c>
       <c r="K40" t="n">
-        <v>10000032</v>
+        <v>10000025</v>
       </c>
       <c r="L40" t="n">
-        <v>11000032</v>
+        <v>11000039</v>
       </c>
       <c r="M40" t="n">
         <v>12000001</v>
       </c>
       <c r="N40" t="n">
-        <v>13000034</v>
+        <v>13000039</v>
       </c>
       <c r="O40" t="n">
-        <v>14000034</v>
+        <v>14000039</v>
       </c>
       <c r="P40" t="n">
         <v>15000001</v>
       </c>
-      <c r="Q40" t="inlineStr"/>
+      <c r="Q40" t="inlineStr">
+        <is>
+          <t>Centrale nazionale d'allarme</t>
+        </is>
+      </c>
       <c r="R40" t="inlineStr"/>
       <c r="S40" t="inlineStr">
         <is>
-          <t>Componente della protezione civile, costituiscono corpo civico</t>
-        </is>
-      </c>
-      <c r="T40" t="inlineStr"/>
+          <t>La CENAL, una divisione dell'Ufficio federale della protezione della popolazione (UFPP), è l'organo federale competente per gli eventi straordinari. Il compito principale della CENAL è quello di tracciare il quadro della situazione prioritaria per la protezione della popolazione. A tal fine, sia nella quotidianità che in caso d'evento scambia informazioni con le autorità competenti dei Cantoni, diversi uffici federali, i gestori delle reti di telecomunicazione, dell'energia e dei trasporti, organizzazioni internazionali e con i centri d'analisi della situazione dei Paesi limitrofi. In caso d'evento, funge da primo punto di contatto per i Cantoni in relazione a tutte le questioni inerenti alla protezione della popolazione. In caso di eventi maggiori, la CENAL informa lo stato maggiore federale Protezione della popolazione e l'assiste nel suo lavoro.</t>
+        </is>
+      </c>
+      <c r="T40" t="inlineStr">
+        <is>
+          <t>Competenza di protezione civile</t>
+        </is>
+      </c>
       <c r="U40" t="inlineStr"/>
       <c r="V40" t="inlineStr"/>
       <c r="W40" t="inlineStr"/>
-      <c r="X40" t="inlineStr"/>
+      <c r="X40" t="inlineStr">
+        <is>
+          <t>Benvenuti sul sito web della Centrale nazionale d'allarme CENAL</t>
+        </is>
+      </c>
       <c r="Y40" t="inlineStr"/>
-      <c r="Z40" t="inlineStr"/>
-      <c r="AA40" t="inlineStr"/>
+      <c r="Z40" t="inlineStr">
+        <is>
+          <t>Confederazione Elvetica</t>
+        </is>
+      </c>
+      <c r="AA40" t="inlineStr">
+        <is>
+          <t>https://www.naz.ch/index_it.html</t>
+        </is>
+      </c>
       <c r="AB40" t="inlineStr"/>
       <c r="AC40" s="2" t="n">
-        <v>43804</v>
+        <v>43656</v>
       </c>
       <c r="AD40" t="inlineStr">
         <is>
-          <t>ITCH00000</t>
+          <t>ITCH00001</t>
         </is>
       </c>
       <c r="AE40" t="inlineStr">
@@ -4454,13 +4474,13 @@
         <v>7000001</v>
       </c>
       <c r="I41" t="n">
-        <v>8000015</v>
+        <v>8000040</v>
       </c>
       <c r="J41" t="n">
         <v>9000003</v>
       </c>
       <c r="K41" t="n">
-        <v>10000026</v>
+        <v>10000025</v>
       </c>
       <c r="L41" t="n">
         <v>11000040</v>
@@ -4469,7 +4489,7 @@
         <v>12000001</v>
       </c>
       <c r="N41" t="n">
-        <v>13000040</v>
+        <v>13000039</v>
       </c>
       <c r="O41" t="n">
         <v>14000040</v>
@@ -4479,110 +4499,11 @@
       </c>
       <c r="Q41" t="inlineStr">
         <is>
-          <t>Centrale nazionale d'allarme</t>
+          <t>Stato maggiore federale Protezione della popolazione</t>
         </is>
       </c>
       <c r="R41" t="inlineStr"/>
       <c r="S41" t="inlineStr">
-        <is>
-          <t>La CENAL, una divisione dell'Ufficio federale della protezione della popolazione (UFPP), è l'organo federale competente per gli eventi straordinari. Il compito principale della CENAL è quello di tracciare il quadro della situazione prioritaria per la protezione della popolazione. A tal fine, sia nella quotidianità che in caso d'evento scambia informazioni con le autorità competenti dei Cantoni, diversi uffici federali, i gestori delle reti di telecomunicazione, dell'energia e dei trasporti, organizzazioni internazionali e con i centri d'analisi della situazione dei Paesi limitrofi. In caso d'evento, funge da primo punto di contatto per i Cantoni in relazione a tutte le questioni inerenti alla protezione della popolazione. In caso di eventi maggiori, la CENAL informa lo stato maggiore federale Protezione della popolazione e l'assiste nel suo lavoro.</t>
-        </is>
-      </c>
-      <c r="T41" t="inlineStr">
-        <is>
-          <t>Competenza di protezione civile</t>
-        </is>
-      </c>
-      <c r="U41" t="inlineStr"/>
-      <c r="V41" t="inlineStr"/>
-      <c r="W41" t="inlineStr"/>
-      <c r="X41" t="inlineStr">
-        <is>
-          <t>Benvenuti sul sito web della Centrale nazionale d'allarme CENAL</t>
-        </is>
-      </c>
-      <c r="Y41" t="inlineStr"/>
-      <c r="Z41" t="inlineStr">
-        <is>
-          <t>Confederazione Elvetica</t>
-        </is>
-      </c>
-      <c r="AA41" t="inlineStr">
-        <is>
-          <t>https://www.naz.ch/index_it.html</t>
-        </is>
-      </c>
-      <c r="AB41" t="inlineStr"/>
-      <c r="AC41" s="2" t="n">
-        <v>43656</v>
-      </c>
-      <c r="AD41" t="inlineStr">
-        <is>
-          <t>ITCH00001</t>
-        </is>
-      </c>
-      <c r="AE41" t="inlineStr">
-        <is>
-          <t>show</t>
-        </is>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" s="1" t="n">
-        <v>40</v>
-      </c>
-      <c r="B42" t="n">
-        <v>1000041</v>
-      </c>
-      <c r="C42" t="n">
-        <v>2000001</v>
-      </c>
-      <c r="D42" t="n">
-        <v>3000041</v>
-      </c>
-      <c r="E42" t="n">
-        <v>4000019</v>
-      </c>
-      <c r="F42" t="n">
-        <v>5000001</v>
-      </c>
-      <c r="G42" t="n">
-        <v>6000001</v>
-      </c>
-      <c r="H42" t="n">
-        <v>7000001</v>
-      </c>
-      <c r="I42" t="n">
-        <v>8000041</v>
-      </c>
-      <c r="J42" t="n">
-        <v>9000003</v>
-      </c>
-      <c r="K42" t="n">
-        <v>10000026</v>
-      </c>
-      <c r="L42" t="n">
-        <v>11000041</v>
-      </c>
-      <c r="M42" t="n">
-        <v>12000001</v>
-      </c>
-      <c r="N42" t="n">
-        <v>13000040</v>
-      </c>
-      <c r="O42" t="n">
-        <v>14000041</v>
-      </c>
-      <c r="P42" t="n">
-        <v>15000001</v>
-      </c>
-      <c r="Q42" t="inlineStr">
-        <is>
-          <t>Stato maggiore federale Protezione della popolazione</t>
-        </is>
-      </c>
-      <c r="R42" t="inlineStr"/>
-      <c r="S42" t="inlineStr">
         <is>
           <t>Nel caso in cui si delinea o si è verificato un evento di portata nazionale rilevante per la protezione della popolazione, lo SMFP assume i compiti seguenti (art. 4, cpv. 2 OSMFP):
 - assicura lo scambio di informazioni e il coordinamento con altri stati maggiori e organi della Confederazione e dei Cantoni, con i gestori di infrastrutture critiche e con i competenti organi all'estero;
@@ -4593,37 +4514,152 @@
 Lo SMFP si compone di una conferenza dei direttori, un elemento di pianificazione formato da esperti degli organi competenti e un elemento d'intervento e di supporto.</t>
         </is>
       </c>
+      <c r="T41" t="inlineStr">
+        <is>
+          <t>Competenza di protezione civile</t>
+        </is>
+      </c>
+      <c r="U41" t="inlineStr"/>
+      <c r="V41" t="inlineStr"/>
+      <c r="W41" t="inlineStr"/>
+      <c r="X41" t="inlineStr">
+        <is>
+          <t>Elemento d'intervento e di supporto dello Stato maggiore federale Protezione della popolazione</t>
+        </is>
+      </c>
+      <c r="Y41" t="inlineStr"/>
+      <c r="Z41" t="inlineStr">
+        <is>
+          <t>Confederazione Elvetica</t>
+        </is>
+      </c>
+      <c r="AA41" t="inlineStr">
+        <is>
+          <t>https://www.naz.ch/it/naz/eo.html</t>
+        </is>
+      </c>
+      <c r="AB41" t="inlineStr"/>
+      <c r="AC41" s="2" t="n">
+        <v>43656</v>
+      </c>
+      <c r="AD41" t="inlineStr">
+        <is>
+          <t>ITCH00002</t>
+        </is>
+      </c>
+      <c r="AE41" t="inlineStr">
+        <is>
+          <t>show</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="B42" t="n">
+        <v>1000041</v>
+      </c>
+      <c r="C42" t="n">
+        <v>2000001</v>
+      </c>
+      <c r="D42" t="n">
+        <v>3000042</v>
+      </c>
+      <c r="E42" t="n">
+        <v>4000019</v>
+      </c>
+      <c r="F42" t="n">
+        <v>5000001</v>
+      </c>
+      <c r="G42" t="n">
+        <v>6000002</v>
+      </c>
+      <c r="H42" t="n">
+        <v>7000009</v>
+      </c>
+      <c r="I42" t="n">
+        <v>8000019</v>
+      </c>
+      <c r="J42" t="n">
+        <v>9000019</v>
+      </c>
+      <c r="K42" t="n">
+        <v>10000019</v>
+      </c>
+      <c r="L42" t="n">
+        <v>11000019</v>
+      </c>
+      <c r="M42" t="n">
+        <v>12000041</v>
+      </c>
+      <c r="N42" t="n">
+        <v>13000039</v>
+      </c>
+      <c r="O42" t="n">
+        <v>14000041</v>
+      </c>
+      <c r="P42" t="n">
+        <v>15000001</v>
+      </c>
+      <c r="Q42" t="inlineStr">
+        <is>
+          <t>Protezione civile</t>
+        </is>
+      </c>
+      <c r="R42" t="inlineStr"/>
+      <c r="S42" t="inlineStr">
+        <is>
+          <t>Il Servizio nazionale della protezione civile, di seguito Servizio nazionale, definito di pubblica utilita', e' il sistema che esercita la funzione di protezione civile costituita dall'insieme delle competenze e delle attivita' volte a tutelare la vita, l'integrita' fisica, i beni, gli insediamenti, gli animali e l'ambiente dai danni o dal pericolo di danni derivanti da eventi calamitosi di origine naturale o derivanti dall'attivita' dell'uomo.</t>
+        </is>
+      </c>
       <c r="T42" t="inlineStr">
         <is>
           <t>Competenza di protezione civile</t>
         </is>
       </c>
       <c r="U42" t="inlineStr"/>
-      <c r="V42" t="inlineStr"/>
-      <c r="W42" t="inlineStr"/>
+      <c r="V42" t="inlineStr">
+        <is>
+          <t>Art 1, comma 1</t>
+        </is>
+      </c>
+      <c r="W42" t="inlineStr">
+        <is>
+          <t>https://www.gazzettaufficiale.it/atto/serie_generale/caricaArticolo?art.progressivo=0&amp;art.idArticolo=1&amp;art.versione=1&amp;art.codiceRedazionale=18G00011&amp;art.dataPubblicazioneGazzetta=2018-01-22&amp;art.idGruppo=1&amp;art.idSottoArticolo1=10&amp;art.idSottoArticolo=1&amp;art.flagTipoArticolo=0</t>
+        </is>
+      </c>
       <c r="X42" t="inlineStr">
         <is>
-          <t>Elemento d'intervento e di supporto dello Stato maggiore federale Protezione della popolazione</t>
-        </is>
-      </c>
-      <c r="Y42" t="inlineStr"/>
+          <t>Decreto Legislativo 2 Gennaio 2018, N. 1, Codice Della Protezione Civile. (18G00011)</t>
+        </is>
+      </c>
+      <c r="Y42" t="inlineStr">
+        <is>
+          <t>Presidenza Del Consiglio Dei Ministri</t>
+        </is>
+      </c>
       <c r="Z42" t="inlineStr">
         <is>
-          <t>Confederazione Elvetica</t>
+          <t>Gazzetta Ufficiale</t>
         </is>
       </c>
       <c r="AA42" t="inlineStr">
         <is>
-          <t>https://www.naz.ch/it/naz/eo.html</t>
-        </is>
-      </c>
-      <c r="AB42" t="inlineStr"/>
+          <t>http://www.gazzettaufficiale.it/eli/id/2018/1/22/18G00011/sg</t>
+        </is>
+      </c>
+      <c r="AB42" t="inlineStr">
+        <is>
+          <t>Definizioni riorganizzate da Tommaso Sansone, Politecnico di Milano.</t>
+        </is>
+      </c>
       <c r="AC42" s="2" t="n">
         <v>43656</v>
       </c>
       <c r="AD42" t="inlineStr">
         <is>
-          <t>ITCH00002</t>
+          <t>ITCH00003</t>
         </is>
       </c>
       <c r="AE42" t="inlineStr">
@@ -4637,13 +4673,13 @@
         <v>41</v>
       </c>
       <c r="B43" t="n">
-        <v>1000042</v>
+        <v>1000041</v>
       </c>
       <c r="C43" t="n">
         <v>2000001</v>
       </c>
       <c r="D43" t="n">
-        <v>3000043</v>
+        <v>3000041</v>
       </c>
       <c r="E43" t="n">
         <v>4000019</v>
@@ -4652,31 +4688,31 @@
         <v>5000001</v>
       </c>
       <c r="G43" t="n">
-        <v>6000002</v>
+        <v>6000041</v>
       </c>
       <c r="H43" t="n">
-        <v>7000009</v>
+        <v>7000001</v>
       </c>
       <c r="I43" t="n">
-        <v>8000019</v>
+        <v>8000041</v>
       </c>
       <c r="J43" t="n">
-        <v>9000019</v>
+        <v>9000003</v>
       </c>
       <c r="K43" t="n">
-        <v>10000019</v>
+        <v>10000041</v>
       </c>
       <c r="L43" t="n">
-        <v>11000019</v>
+        <v>11000041</v>
       </c>
       <c r="M43" t="n">
-        <v>12000042</v>
+        <v>12000041</v>
       </c>
       <c r="N43" t="n">
-        <v>13000040</v>
+        <v>13000039</v>
       </c>
       <c r="O43" t="n">
-        <v>14000042</v>
+        <v>14000041</v>
       </c>
       <c r="P43" t="n">
         <v>15000001</v>
@@ -4689,7 +4725,7 @@
       <c r="R43" t="inlineStr"/>
       <c r="S43" t="inlineStr">
         <is>
-          <t>Il Servizio nazionale della protezione civile, di seguito Servizio nazionale, definito di pubblica utilita', e' il sistema che esercita la funzione di protezione civile costituita dall'insieme delle competenze e delle attivita' volte a tutelare la vita, l'integrita' fisica, i beni, gli insediamenti, gli animali e l'ambiente dai danni o dal pericolo di danni derivanti da eventi calamitosi di origine naturale o derivanti dall'attivita' dell'uomo.</t>
+          <t>La protezione civile protegge la popolazione, assiste le persone in cerca di protezione, protegge i beni culturali, sostiene gli organi di condotta e le altre organizzazioni partner nonché svolge lavori di ripristino e di pubblica utilità. Essa è un’organizzazione civile che opera singolarmente o in maniera coordinata, come organizzazione partner, all'interno della struttura svizzera di di protezione della popolazione.</t>
         </is>
       </c>
       <c r="T43" t="inlineStr">
@@ -4700,32 +4736,24 @@
       <c r="U43" t="inlineStr"/>
       <c r="V43" t="inlineStr">
         <is>
-          <t>Art 1, comma 1</t>
-        </is>
-      </c>
-      <c r="W43" t="inlineStr">
-        <is>
-          <t>https://www.gazzettaufficiale.it/atto/serie_generale/caricaArticolo?art.progressivo=0&amp;art.idArticolo=1&amp;art.versione=1&amp;art.codiceRedazionale=18G00011&amp;art.dataPubblicazioneGazzetta=2018-01-22&amp;art.idGruppo=1&amp;art.idSottoArticolo1=10&amp;art.idSottoArticolo=1&amp;art.flagTipoArticolo=0</t>
-        </is>
-      </c>
+          <t>Art. 1</t>
+        </is>
+      </c>
+      <c r="W43" t="inlineStr"/>
       <c r="X43" t="inlineStr">
         <is>
-          <t>Decreto Legislativo 2 Gennaio 2018, N. 1, Codice Della Protezione Civile. (18G00011)</t>
-        </is>
-      </c>
-      <c r="Y43" t="inlineStr">
-        <is>
-          <t>Presidenza Del Consiglio Dei Ministri</t>
-        </is>
-      </c>
+          <t>Legge sulla protezione civile del 26 febbraio 2007</t>
+        </is>
+      </c>
+      <c r="Y43" t="inlineStr"/>
       <c r="Z43" t="inlineStr">
         <is>
-          <t>Gazzetta Ufficiale</t>
+          <t>Repubblica e Cantone Ticino</t>
         </is>
       </c>
       <c r="AA43" t="inlineStr">
         <is>
-          <t>http://www.gazzettaufficiale.it/eli/id/2018/1/22/18G00011/sg</t>
+          <t>https://m3.ti.ch/CAN/RLeggi/public/index.php/raccolta-leggi/legge/num/44</t>
         </is>
       </c>
       <c r="AB43" t="inlineStr">
@@ -4752,13 +4780,13 @@
         <v>42</v>
       </c>
       <c r="B44" t="n">
-        <v>1000042</v>
+        <v>1000043</v>
       </c>
       <c r="C44" t="n">
         <v>2000001</v>
       </c>
       <c r="D44" t="n">
-        <v>3000042</v>
+        <v>3000043</v>
       </c>
       <c r="E44" t="n">
         <v>4000019</v>
@@ -4767,149 +4795,42 @@
         <v>5000001</v>
       </c>
       <c r="G44" t="n">
-        <v>6000042</v>
+        <v>6000001</v>
       </c>
       <c r="H44" t="n">
         <v>7000001</v>
       </c>
       <c r="I44" t="n">
-        <v>8000042</v>
+        <v>8000043</v>
       </c>
       <c r="J44" t="n">
         <v>9000003</v>
       </c>
       <c r="K44" t="n">
-        <v>10000042</v>
+        <v>10000025</v>
       </c>
       <c r="L44" t="n">
-        <v>11000042</v>
+        <v>11000043</v>
       </c>
       <c r="M44" t="n">
-        <v>12000042</v>
+        <v>12000001</v>
       </c>
       <c r="N44" t="n">
-        <v>13000040</v>
+        <v>13000039</v>
       </c>
       <c r="O44" t="n">
-        <v>14000042</v>
+        <v>14000043</v>
       </c>
       <c r="P44" t="n">
         <v>15000001</v>
       </c>
       <c r="Q44" t="inlineStr">
         <is>
-          <t>Protezione civile</t>
+          <t>Comando della protezione civile</t>
         </is>
       </c>
       <c r="R44" t="inlineStr"/>
       <c r="S44" t="inlineStr">
-        <is>
-          <t>La protezione civile protegge la popolazione, assiste le persone in cerca di protezione, protegge i beni culturali, sostiene gli organi di condotta e le altre organizzazioni partner nonché svolge lavori di ripristino e di pubblica utilità. Essa è un’organizzazione civile che opera singolarmente o in maniera coordinata, come organizzazione partner, all'interno della struttura svizzera di di protezione della popolazione.</t>
-        </is>
-      </c>
-      <c r="T44" t="inlineStr">
-        <is>
-          <t>Competenza di protezione civile</t>
-        </is>
-      </c>
-      <c r="U44" t="inlineStr"/>
-      <c r="V44" t="inlineStr">
-        <is>
-          <t>Art. 1</t>
-        </is>
-      </c>
-      <c r="W44" t="inlineStr"/>
-      <c r="X44" t="inlineStr">
-        <is>
-          <t>Legge sulla protezione civile del 26 febbraio 2007</t>
-        </is>
-      </c>
-      <c r="Y44" t="inlineStr"/>
-      <c r="Z44" t="inlineStr">
-        <is>
-          <t>Repubblica e Cantone Ticino</t>
-        </is>
-      </c>
-      <c r="AA44" t="inlineStr">
-        <is>
-          <t>https://m3.ti.ch/CAN/RLeggi/public/index.php/raccolta-leggi/legge/num/44</t>
-        </is>
-      </c>
-      <c r="AB44" t="inlineStr">
-        <is>
-          <t>Definizioni riorganizzate da Tommaso Sansone, Politecnico di Milano.</t>
-        </is>
-      </c>
-      <c r="AC44" s="2" t="n">
-        <v>43656</v>
-      </c>
-      <c r="AD44" t="inlineStr">
-        <is>
-          <t>ITCH00003</t>
-        </is>
-      </c>
-      <c r="AE44" t="inlineStr">
-        <is>
-          <t>show</t>
-        </is>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" s="1" t="n">
-        <v>43</v>
-      </c>
-      <c r="B45" t="n">
-        <v>1000044</v>
-      </c>
-      <c r="C45" t="n">
-        <v>2000001</v>
-      </c>
-      <c r="D45" t="n">
-        <v>3000044</v>
-      </c>
-      <c r="E45" t="n">
-        <v>4000019</v>
-      </c>
-      <c r="F45" t="n">
-        <v>5000001</v>
-      </c>
-      <c r="G45" t="n">
-        <v>6000001</v>
-      </c>
-      <c r="H45" t="n">
-        <v>7000001</v>
-      </c>
-      <c r="I45" t="n">
-        <v>8000044</v>
-      </c>
-      <c r="J45" t="n">
-        <v>9000003</v>
-      </c>
-      <c r="K45" t="n">
-        <v>10000026</v>
-      </c>
-      <c r="L45" t="n">
-        <v>11000044</v>
-      </c>
-      <c r="M45" t="n">
-        <v>12000001</v>
-      </c>
-      <c r="N45" t="n">
-        <v>13000040</v>
-      </c>
-      <c r="O45" t="n">
-        <v>14000044</v>
-      </c>
-      <c r="P45" t="n">
-        <v>15000001</v>
-      </c>
-      <c r="Q45" t="inlineStr">
-        <is>
-          <t>Comando della protezione civile</t>
-        </is>
-      </c>
-      <c r="R45" t="inlineStr"/>
-      <c r="S45" t="inlineStr">
         <is>
           <t>Il comando della protezione civile è l’organo che dirige la protezione civile, ed è generalmente costituito dal comandante della protezione civile e dai suoi sostituti. I suoi compiti fondamentali sono i seguenti:
 - condurre gli interventi
@@ -4919,17 +4840,120 @@
 - rappresentare le questioni della protezione civile presso le autorità, le organizzazioni partner, gli organi di condotta e la popolazione</t>
         </is>
       </c>
+      <c r="T44" t="inlineStr">
+        <is>
+          <t>Competenza di protezione civile</t>
+        </is>
+      </c>
+      <c r="U44" t="inlineStr"/>
+      <c r="V44" t="inlineStr"/>
+      <c r="W44" t="inlineStr"/>
+      <c r="X44" t="inlineStr">
+        <is>
+          <t>Il comando della protezione civile</t>
+        </is>
+      </c>
+      <c r="Y44" t="inlineStr"/>
+      <c r="Z44" t="inlineStr">
+        <is>
+          <t>Confederazione Elvetica</t>
+        </is>
+      </c>
+      <c r="AA44" t="inlineStr">
+        <is>
+          <t>https://www.babs.admin.ch/it/zs/org/kdo.html</t>
+        </is>
+      </c>
+      <c r="AB44" t="inlineStr"/>
+      <c r="AC44" s="2" t="n">
+        <v>43656</v>
+      </c>
+      <c r="AD44" t="inlineStr">
+        <is>
+          <t>ITCH00004</t>
+        </is>
+      </c>
+      <c r="AE44" t="inlineStr">
+        <is>
+          <t>show</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="B45" t="n">
+        <v>1000044</v>
+      </c>
+      <c r="C45" t="n">
+        <v>2000001</v>
+      </c>
+      <c r="D45" t="n">
+        <v>3000044</v>
+      </c>
+      <c r="E45" t="n">
+        <v>4000019</v>
+      </c>
+      <c r="F45" t="n">
+        <v>5000001</v>
+      </c>
+      <c r="G45" t="n">
+        <v>6000044</v>
+      </c>
+      <c r="H45" t="n">
+        <v>7000001</v>
+      </c>
+      <c r="I45" t="n">
+        <v>8000044</v>
+      </c>
+      <c r="J45" t="n">
+        <v>9000003</v>
+      </c>
+      <c r="K45" t="n">
+        <v>10000025</v>
+      </c>
+      <c r="L45" t="n">
+        <v>11000044</v>
+      </c>
+      <c r="M45" t="n">
+        <v>12000001</v>
+      </c>
+      <c r="N45" t="n">
+        <v>13000044</v>
+      </c>
+      <c r="O45" t="n">
+        <v>14000044</v>
+      </c>
+      <c r="P45" t="n">
+        <v>15000001</v>
+      </c>
+      <c r="Q45" t="inlineStr">
+        <is>
+          <t>Impianto di protezione per la protezione della popolazione</t>
+        </is>
+      </c>
+      <c r="R45" t="inlineStr"/>
+      <c r="S45" t="inlineStr">
+        <is>
+          <t>Si definiscono impianti di protezione i posti di comando, gli impianti d'apprestamento, i centri sanitari protetti e gli ospedali protetti. Essi vengono utilizzati soprattutto per garantire la condotta e l’operatività dei mezzi della protezione della popolazione.</t>
+        </is>
+      </c>
       <c r="T45" t="inlineStr">
         <is>
           <t>Competenza di protezione civile</t>
         </is>
       </c>
       <c r="U45" t="inlineStr"/>
-      <c r="V45" t="inlineStr"/>
+      <c r="V45" t="inlineStr">
+        <is>
+          <t>Impianti di protezione per la protezione della popolazione</t>
+        </is>
+      </c>
       <c r="W45" t="inlineStr"/>
       <c r="X45" t="inlineStr">
         <is>
-          <t>Il comando della protezione civile</t>
+          <t>Costruzioni di protezione</t>
         </is>
       </c>
       <c r="Y45" t="inlineStr"/>
@@ -4940,16 +4964,16 @@
       </c>
       <c r="AA45" t="inlineStr">
         <is>
-          <t>https://www.babs.admin.ch/it/zs/org/kdo.html</t>
+          <t>https://www.babs.admin.ch/it/aufgabenbabs/schutzbauten.html</t>
         </is>
       </c>
       <c r="AB45" t="inlineStr"/>
       <c r="AC45" s="2" t="n">
-        <v>43656</v>
+        <v>43657</v>
       </c>
       <c r="AD45" t="inlineStr">
         <is>
-          <t>ITCH00004</t>
+          <t>ITCH00005</t>
         </is>
       </c>
       <c r="AE45" t="inlineStr">
@@ -4984,22 +5008,22 @@
         <v>7000001</v>
       </c>
       <c r="I46" t="n">
-        <v>8000045</v>
+        <v>8000025</v>
       </c>
       <c r="J46" t="n">
         <v>9000003</v>
       </c>
       <c r="K46" t="n">
-        <v>10000026</v>
+        <v>10000025</v>
       </c>
       <c r="L46" t="n">
-        <v>11000045</v>
+        <v>11000025</v>
       </c>
       <c r="M46" t="n">
         <v>12000001</v>
       </c>
       <c r="N46" t="n">
-        <v>13000045</v>
+        <v>13000044</v>
       </c>
       <c r="O46" t="n">
         <v>14000045</v>
@@ -5009,13 +5033,16 @@
       </c>
       <c r="Q46" t="inlineStr">
         <is>
-          <t>Impianto di protezione per la protezione della popolazione</t>
+          <t>Evento NBC</t>
         </is>
       </c>
       <c r="R46" t="inlineStr"/>
       <c r="S46" t="inlineStr">
         <is>
-          <t>Si definiscono impianti di protezione i posti di comando, gli impianti d'apprestamento, i centri sanitari protetti e gli ospedali protetti. Essi vengono utilizzati soprattutto per garantire la condotta e l’operatività dei mezzi della protezione della popolazione.</t>
+          <t>Per evento NBC s'intende l'emissione illecita di sostanze nucleari (atomiche e radiologiche, N), biologiche (B) o chimiche (C). L'emissione può essere accidentale (incidente) o intenzionale (atto criminale o terroristico). Si distinguono i seguenti settori:
+- settore N: emissione di radiazioni ionizzanti e radioattività;
+- settore B: emissione di organismi patogeni (che causano malattie) o dei loro prodotti metabolici;
+- settore C: emissione di gas, liquidi o solidi tossici.</t>
         </is>
       </c>
       <c r="T46" t="inlineStr">
@@ -5026,13 +5053,13 @@
       <c r="U46" t="inlineStr"/>
       <c r="V46" t="inlineStr">
         <is>
-          <t>Impianti di protezione per la protezione della popolazione</t>
+          <t>Definizione di „evento NBC“: emissione di sostanze pericolose</t>
         </is>
       </c>
       <c r="W46" t="inlineStr"/>
       <c r="X46" t="inlineStr">
         <is>
-          <t>Costruzioni di protezione</t>
+          <t>La Protezione NBC</t>
         </is>
       </c>
       <c r="Y46" t="inlineStr"/>
@@ -5043,7 +5070,7 @@
       </c>
       <c r="AA46" t="inlineStr">
         <is>
-          <t>https://www.babs.admin.ch/it/aufgabenbabs/schutzbauten.html</t>
+          <t>https://www.babs.admin.ch/it/aufgabenbabs/abcschutz.html</t>
         </is>
       </c>
       <c r="AB46" t="inlineStr"/>
@@ -5052,7 +5079,7 @@
       </c>
       <c r="AD46" t="inlineStr">
         <is>
-          <t>ITCH00005</t>
+          <t>ITCH00006</t>
         </is>
       </c>
       <c r="AE46" t="inlineStr">
@@ -5075,7 +5102,7 @@
         <v>3000046</v>
       </c>
       <c r="E47" t="n">
-        <v>4000019</v>
+        <v>4000033</v>
       </c>
       <c r="F47" t="n">
         <v>5000001</v>
@@ -5087,22 +5114,22 @@
         <v>7000001</v>
       </c>
       <c r="I47" t="n">
-        <v>8000026</v>
+        <v>8000046</v>
       </c>
       <c r="J47" t="n">
-        <v>9000003</v>
+        <v>9000046</v>
       </c>
       <c r="K47" t="n">
-        <v>10000026</v>
+        <v>10000046</v>
       </c>
       <c r="L47" t="n">
-        <v>11000026</v>
+        <v>11000046</v>
       </c>
       <c r="M47" t="n">
         <v>12000001</v>
       </c>
       <c r="N47" t="n">
-        <v>13000045</v>
+        <v>13000046</v>
       </c>
       <c r="O47" t="n">
         <v>14000046</v>
@@ -5112,53 +5139,54 @@
       </c>
       <c r="Q47" t="inlineStr">
         <is>
-          <t>Evento NBC</t>
+          <t>Suscettibilità da Frana</t>
         </is>
       </c>
       <c r="R47" t="inlineStr"/>
       <c r="S47" t="inlineStr">
         <is>
-          <t>Per evento NBC s'intende l'emissione illecita di sostanze nucleari (atomiche e radiologiche, N), biologiche (B) o chimiche (C). L'emissione può essere accidentale (incidente) o intenzionale (atto criminale o terroristico). Si distinguono i seguenti settori:
-- settore N: emissione di radiazioni ionizzanti e radioattività;
-- settore B: emissione di organismi patogeni (che causano malattie) o dei loro prodotti metabolici;
-- settore C: emissione di gas, liquidi o solidi tossici.</t>
+          <t>La suscettibilità da frana è la probabilità che una frana avvenga in un territorio, sulla base delle condizioni locali. E’ una misura del grado in cui un territorio potrà essere interessato da frane, ossia una stima di “dove” le frane potranno accadere. La suscettibilità non considera la ricorrenza temporale, né la dimensione delle frane. In termini matematici, la suscettibilità da frana è comunemente espressa come la probabilità d’occorrenza spaziale di un dissesto, dato un insieme di condizioni territoriali e ambientali.</t>
         </is>
       </c>
       <c r="T47" t="inlineStr">
         <is>
-          <t>Competenza di protezione civile</t>
+          <t>Geologia e sismologia</t>
         </is>
       </c>
       <c r="U47" t="inlineStr"/>
       <c r="V47" t="inlineStr">
         <is>
-          <t>Definizione di „evento NBC“: emissione di sostanze pericolose</t>
+          <t>primo paragrafo</t>
         </is>
       </c>
       <c r="W47" t="inlineStr"/>
       <c r="X47" t="inlineStr">
         <is>
-          <t>La Protezione NBC</t>
-        </is>
-      </c>
-      <c r="Y47" t="inlineStr"/>
+          <t>Modelli e carte di suscettibilità da frana</t>
+        </is>
+      </c>
+      <c r="Y47" t="inlineStr">
+        <is>
+          <t>IRPI</t>
+        </is>
+      </c>
       <c r="Z47" t="inlineStr">
         <is>
-          <t>Confederazione Elvetica</t>
+          <t>IRPI CNR</t>
         </is>
       </c>
       <c r="AA47" t="inlineStr">
         <is>
-          <t>https://www.babs.admin.ch/it/aufgabenbabs/abcschutz.html</t>
+          <t>http://www.irpi.cnr.it/focus/suscettibilita-da-frana/</t>
         </is>
       </c>
       <c r="AB47" t="inlineStr"/>
       <c r="AC47" s="2" t="n">
-        <v>43657</v>
+        <v>43731</v>
       </c>
       <c r="AD47" t="inlineStr">
         <is>
-          <t>ITCH00006</t>
+          <t>ITCH00007</t>
         </is>
       </c>
       <c r="AE47" t="inlineStr">
@@ -5181,7 +5209,7 @@
         <v>3000047</v>
       </c>
       <c r="E48" t="n">
-        <v>4000033</v>
+        <v>4000047</v>
       </c>
       <c r="F48" t="n">
         <v>5000001</v>
@@ -5196,16 +5224,16 @@
         <v>8000047</v>
       </c>
       <c r="J48" t="n">
-        <v>9000047</v>
+        <v>9000003</v>
       </c>
       <c r="K48" t="n">
-        <v>10000047</v>
+        <v>10000025</v>
       </c>
       <c r="L48" t="n">
         <v>11000047</v>
       </c>
       <c r="M48" t="n">
-        <v>12000001</v>
+        <v>12000047</v>
       </c>
       <c r="N48" t="n">
         <v>13000047</v>
@@ -5218,54 +5246,54 @@
       </c>
       <c r="Q48" t="inlineStr">
         <is>
-          <t>Suscettibilità da Frana</t>
+          <t>Pompieri</t>
         </is>
       </c>
       <c r="R48" t="inlineStr"/>
       <c r="S48" t="inlineStr">
         <is>
-          <t>La suscettibilità da frana è la probabilità che una frana avvenga in un territorio, sulla base delle condizioni locali. E’ una misura del grado in cui un territorio potrà essere interessato da frane, ossia una stima di “dove” le frane potranno accadere. La suscettibilità non considera la ricorrenza temporale, né la dimensione delle frane. In termini matematici, la suscettibilità da frana è comunemente espressa come la probabilità d’occorrenza spaziale di un dissesto, dato un insieme di condizioni territoriali e ambientali.</t>
+          <t>I pompieri sono responsabili di salvataggio e lotta contro i sinistri in generale, compresa la lotta antincendio e contro i sinistri ordinari. Intervengono anche in caso d’emissioni tossiche, fuoriuscite di carburanti e contaminazioni radioattive. Sono un mezzo di primo intervento.</t>
         </is>
       </c>
       <c r="T48" t="inlineStr">
         <is>
-          <t>Geologia e sismologia</t>
+          <t>Competenza di soccorso tecnico urgente; Competenza della Protezione Civile</t>
         </is>
       </c>
       <c r="U48" t="inlineStr"/>
       <c r="V48" t="inlineStr">
         <is>
-          <t>primo paragrafo</t>
+          <t>Art. 3</t>
         </is>
       </c>
       <c r="W48" t="inlineStr"/>
       <c r="X48" t="inlineStr">
         <is>
-          <t>Modelli e carte di suscettibilità da frana</t>
-        </is>
-      </c>
-      <c r="Y48" t="inlineStr">
-        <is>
-          <t>IRPI</t>
-        </is>
-      </c>
+          <t>Legge federale sulla protezione della popolazione e sulla protezione civile del 4 ottobre 2002</t>
+        </is>
+      </c>
+      <c r="Y48" t="inlineStr"/>
       <c r="Z48" t="inlineStr">
         <is>
-          <t>IRPI CNR</t>
+          <t>Confederazione Elvetica</t>
         </is>
       </c>
       <c r="AA48" t="inlineStr">
         <is>
-          <t>http://www.irpi.cnr.it/focus/suscettibilita-da-frana/</t>
-        </is>
-      </c>
-      <c r="AB48" t="inlineStr"/>
+          <t>https://www.admin.ch/opc/it/classified-compilation/20011872/201701010000/520.1.pdf</t>
+        </is>
+      </c>
+      <c r="AB48" t="inlineStr">
+        <is>
+          <t>Per il lato italiano, definizione tratta dall'art 10 del codice di protezione civile del 2-1-2018, rielaborata da Tommaso Sansone.</t>
+        </is>
+      </c>
       <c r="AC48" s="2" t="n">
-        <v>43731</v>
+        <v>43766</v>
       </c>
       <c r="AD48" t="inlineStr">
         <is>
-          <t>ITCH00007</t>
+          <t>ITCH00009</t>
         </is>
       </c>
       <c r="AE48" t="inlineStr">
@@ -5279,7 +5307,7 @@
         <v>47</v>
       </c>
       <c r="B49" t="n">
-        <v>1000048</v>
+        <v>1000035</v>
       </c>
       <c r="C49" t="n">
         <v>2000001</v>
@@ -5288,7 +5316,7 @@
         <v>3000048</v>
       </c>
       <c r="E49" t="n">
-        <v>4000048</v>
+        <v>4000047</v>
       </c>
       <c r="F49" t="n">
         <v>5000001</v>
@@ -5297,41 +5325,41 @@
         <v>6000048</v>
       </c>
       <c r="H49" t="n">
-        <v>7000001</v>
+        <v>7000048</v>
       </c>
       <c r="I49" t="n">
-        <v>8000048</v>
+        <v>8000019</v>
       </c>
       <c r="J49" t="n">
-        <v>9000003</v>
+        <v>9000019</v>
       </c>
       <c r="K49" t="n">
-        <v>10000026</v>
+        <v>10000019</v>
       </c>
       <c r="L49" t="n">
         <v>11000048</v>
       </c>
       <c r="M49" t="n">
-        <v>12000048</v>
+        <v>12000047</v>
       </c>
       <c r="N49" t="n">
-        <v>13000048</v>
+        <v>13000047</v>
       </c>
       <c r="O49" t="n">
-        <v>14000048</v>
+        <v>14000047</v>
       </c>
       <c r="P49" t="n">
         <v>15000001</v>
       </c>
       <c r="Q49" t="inlineStr">
         <is>
-          <t>Pompieri</t>
+          <t>Vigili del fuoco</t>
         </is>
       </c>
       <c r="R49" t="inlineStr"/>
       <c r="S49" t="inlineStr">
         <is>
-          <t>I pompieri sono responsabili di salvataggio e lotta contro i sinistri in generale, compresa la lotta antincendio e contro i sinistri ordinari. Intervengono anche in caso d’emissioni tossiche, fuoriuscite di carburanti e contaminazioni radioattive. Sono un mezzo di primo intervento.</t>
+          <t>In occasione degli eventi calamitosi, il Corpo nazionale dei vigili del fuoco opera gli interventi di soccorso tecnico indifferibili e urgenti: di ricerca e salvataggio delle persone e – ai fini della salvaguardia della pubblica incolumità – anche di messa in sicurezza dei luoghi, delle strutture e degli impianti.</t>
         </is>
       </c>
       <c r="T49" t="inlineStr">
@@ -5342,24 +5370,32 @@
       <c r="U49" t="inlineStr"/>
       <c r="V49" t="inlineStr">
         <is>
-          <t>Art. 3</t>
-        </is>
-      </c>
-      <c r="W49" t="inlineStr"/>
+          <t>Art. 10</t>
+        </is>
+      </c>
+      <c r="W49" t="inlineStr">
+        <is>
+          <t>https://www.gazzettaufficiale.it/atto/serie_generale/caricaArticolo?art.progressivo=0&amp;art.idArticolo=10&amp;art.versione=1&amp;art.codiceRedazionale=18G00011&amp;art.dataPubblicazioneGazzetta=2018-01-22&amp;art.idGruppo=3&amp;art.idSottoArticolo1=10&amp;art.idSottoArticolo=1&amp;art.flagTipoArticolo=0#art</t>
+        </is>
+      </c>
       <c r="X49" t="inlineStr">
         <is>
-          <t>Legge federale sulla protezione della popolazione e sulla protezione civile del 4 ottobre 2002</t>
-        </is>
-      </c>
-      <c r="Y49" t="inlineStr"/>
+          <t>Decreto Legislativo 2 Gennaio 2018, N. 1, Codice Della Protezione Civile. (18G00011)</t>
+        </is>
+      </c>
+      <c r="Y49" t="inlineStr">
+        <is>
+          <t>Presidenza Del Consiglio Dei Ministri</t>
+        </is>
+      </c>
       <c r="Z49" t="inlineStr">
         <is>
-          <t>Confederazione Elvetica</t>
+          <t>Gazzetta Ufficiale</t>
         </is>
       </c>
       <c r="AA49" t="inlineStr">
         <is>
-          <t>https://www.admin.ch/opc/it/classified-compilation/20011872/201701010000/520.1.pdf</t>
+          <t>https://www.gazzettaufficiale.it/eli/id/2018/1/22/18G00011/sg</t>
         </is>
       </c>
       <c r="AB49" t="inlineStr">
@@ -5386,100 +5422,96 @@
         <v>48</v>
       </c>
       <c r="B50" t="n">
-        <v>1000034</v>
+        <v>1000050</v>
       </c>
       <c r="C50" t="n">
         <v>2000001</v>
       </c>
       <c r="D50" t="n">
-        <v>3000049</v>
+        <v>3000050</v>
       </c>
       <c r="E50" t="n">
-        <v>4000048</v>
+        <v>4000001</v>
       </c>
       <c r="F50" t="n">
-        <v>5000001</v>
+        <v>5000050</v>
       </c>
       <c r="G50" t="n">
-        <v>6000049</v>
+        <v>6000047</v>
       </c>
       <c r="H50" t="n">
-        <v>7000049</v>
+        <v>7000001</v>
       </c>
       <c r="I50" t="n">
-        <v>8000019</v>
+        <v>8000047</v>
       </c>
       <c r="J50" t="n">
-        <v>9000019</v>
+        <v>9000050</v>
       </c>
       <c r="K50" t="n">
-        <v>10000019</v>
+        <v>10000050</v>
       </c>
       <c r="L50" t="n">
-        <v>11000049</v>
+        <v>11000047</v>
       </c>
       <c r="M50" t="n">
-        <v>12000048</v>
+        <v>12000049</v>
       </c>
       <c r="N50" t="n">
-        <v>13000048</v>
+        <v>13000047</v>
       </c>
       <c r="O50" t="n">
-        <v>14000048</v>
+        <v>14000049</v>
       </c>
       <c r="P50" t="n">
         <v>15000001</v>
       </c>
       <c r="Q50" t="inlineStr">
         <is>
-          <t>Vigili del fuoco</t>
+          <t>Organizzazione partner</t>
         </is>
       </c>
       <c r="R50" t="inlineStr"/>
       <c r="S50" t="inlineStr">
         <is>
-          <t>In occasione degli eventi calamitosi, il Corpo nazionale dei vigili del fuoco opera gli interventi di soccorso tecnico indifferibili e urgenti: di ricerca e salvataggio delle persone e – ai fini della salvaguardia della pubblica incolumità – anche di messa in sicurezza dei luoghi, delle strutture e degli impianti.</t>
-        </is>
-      </c>
-      <c r="T50" t="inlineStr">
-        <is>
-          <t>Competenza di soccorso tecnico urgente; Competenza della Protezione Civile</t>
-        </is>
-      </c>
-      <c r="U50" t="inlineStr"/>
+          <t>Sono organizzazioni partner quelle che collaborano alla protezione della popolazione: Polizia, pompieri, servizi della sanità pubblica, servizi tecnici, protezione civile.</t>
+        </is>
+      </c>
+      <c r="T50" t="inlineStr"/>
+      <c r="U50" t="inlineStr">
+        <is>
+          <t>confederazione elvetica</t>
+        </is>
+      </c>
       <c r="V50" t="inlineStr">
         <is>
-          <t>Art. 10</t>
-        </is>
-      </c>
-      <c r="W50" t="inlineStr">
-        <is>
-          <t>https://www.gazzettaufficiale.it/atto/serie_generale/caricaArticolo?art.progressivo=0&amp;art.idArticolo=10&amp;art.versione=1&amp;art.codiceRedazionale=18G00011&amp;art.dataPubblicazioneGazzetta=2018-01-22&amp;art.idGruppo=3&amp;art.idSottoArticolo1=10&amp;art.idSottoArticolo=1&amp;art.flagTipoArticolo=0#art</t>
-        </is>
-      </c>
+          <t>Art. 3</t>
+        </is>
+      </c>
+      <c r="W50" t="inlineStr"/>
       <c r="X50" t="inlineStr">
         <is>
-          <t>Decreto Legislativo 2 Gennaio 2018, N. 1, Codice Della Protezione Civile. (18G00011)</t>
+          <t>Legge federale sulla protezione della popolazione e sulla protezione civile del 4 ottobre 2002</t>
         </is>
       </c>
       <c r="Y50" t="inlineStr">
         <is>
-          <t>Presidenza Del Consiglio Dei Ministri</t>
+          <t>Confederazion elvetica</t>
         </is>
       </c>
       <c r="Z50" t="inlineStr">
         <is>
-          <t>Gazzetta Ufficiale</t>
+          <t>Confederazione elvetica</t>
         </is>
       </c>
       <c r="AA50" t="inlineStr">
         <is>
-          <t>https://www.gazzettaufficiale.it/eli/id/2018/1/22/18G00011/sg</t>
+          <t>https://www.admin.ch/opc/it/classified-compilation/20011872/201701010000/520.1.pdf</t>
         </is>
       </c>
       <c r="AB50" t="inlineStr">
         <is>
-          <t>Per il lato italiano, definizione tratta dall'art 10 del codice di protezione civile del 2-1-2018, rielaborata da Tommaso Sansone.</t>
+          <t>strutture operative in italia e organizzazioni partner in svizzera hanno la stessa connotazione all'interno di un sistema di protezione della popolazione.</t>
         </is>
       </c>
       <c r="AC50" s="2" t="n">
@@ -5487,7 +5519,7 @@
       </c>
       <c r="AD50" t="inlineStr">
         <is>
-          <t>ITCH00009</t>
+          <t>ITCH00010</t>
         </is>
       </c>
       <c r="AE50" t="inlineStr">
@@ -5501,91 +5533,95 @@
         <v>49</v>
       </c>
       <c r="B51" t="n">
-        <v>1000050</v>
+        <v>1000049</v>
       </c>
       <c r="C51" t="n">
         <v>2000001</v>
       </c>
       <c r="D51" t="n">
-        <v>3000050</v>
+        <v>3000049</v>
       </c>
       <c r="E51" t="n">
-        <v>4000001</v>
+        <v>4000002</v>
       </c>
       <c r="F51" t="n">
-        <v>5000050</v>
+        <v>5000001</v>
       </c>
       <c r="G51" t="n">
-        <v>6000048</v>
+        <v>6000049</v>
       </c>
       <c r="H51" t="n">
-        <v>7000001</v>
+        <v>7000049</v>
       </c>
       <c r="I51" t="n">
-        <v>8000048</v>
+        <v>8000019</v>
       </c>
       <c r="J51" t="n">
-        <v>9000050</v>
+        <v>9000019</v>
       </c>
       <c r="K51" t="n">
-        <v>10000040</v>
+        <v>10000019</v>
       </c>
       <c r="L51" t="n">
         <v>11000048</v>
       </c>
       <c r="M51" t="n">
-        <v>12000050</v>
+        <v>12000049</v>
       </c>
       <c r="N51" t="n">
-        <v>13000048</v>
+        <v>13000047</v>
       </c>
       <c r="O51" t="n">
-        <v>14000050</v>
+        <v>14000049</v>
       </c>
       <c r="P51" t="n">
         <v>15000001</v>
       </c>
       <c r="Q51" t="inlineStr">
         <is>
-          <t>Organizzazione partner</t>
+          <t>Struttura operativa</t>
         </is>
       </c>
       <c r="R51" t="inlineStr"/>
       <c r="S51" t="inlineStr">
         <is>
-          <t>Sono organizzazioni partner quelle che collaborano alla protezione della popolazione: Polizia, pompieri, servizi della sanità pubblica, servizi tecnici, protezione civile.</t>
-        </is>
-      </c>
-      <c r="T51" t="inlineStr"/>
-      <c r="U51" t="inlineStr">
-        <is>
-          <t>confederazione elvetica</t>
-        </is>
-      </c>
+          <t>Oltre al Corpo nazionale dei vigili del fuoco, che opera quale componente fondamentale del Servizio nazionale della protezione civile, sono strutture operative nazionali: a) le Forze armate; b) le Forze di polizia; c) gli enti e istituti di ricerca di rilievo nazionale con finalità di protezione civile, anche organizzati come centri di competenza, l'Istituto nazionale di geofisica e vulcanologia e il Consiglio nazionale delle ricerche; d) le strutture del Servizio sanitario nazionale; e) il volontariato organizzato di protezione civile iscritto nell'elenco nazionale del volontariato di protezione civile, l'Associazione della Croce rossa italiana e il Corpo nazionale del soccorso alpino e speleologico; f) il Sistema nazionale per la protezione dell'ambiente; g) le strutture preposte alla gestione dei servizi meteorologici a livello nazionale.</t>
+        </is>
+      </c>
+      <c r="T51" t="inlineStr">
+        <is>
+          <t>Competenza della Protezione Civile</t>
+        </is>
+      </c>
+      <c r="U51" t="inlineStr"/>
       <c r="V51" t="inlineStr">
         <is>
-          <t>Art. 3</t>
-        </is>
-      </c>
-      <c r="W51" t="inlineStr"/>
+          <t>Art. 13</t>
+        </is>
+      </c>
+      <c r="W51" t="inlineStr">
+        <is>
+          <t>https://www.gazzettaufficiale.it/atto/serie_generale/caricaArticolo?art.progressivo=0&amp;art.idArticolo=13&amp;art.versione=1&amp;art.codiceRedazionale=18G00011&amp;art.dataPubblicazioneGazzetta=2018-01-22&amp;art.idGruppo=3&amp;art.idSottoArticolo1=10&amp;art.idSottoArticolo=1&amp;art.flagTipoArticolo=0#art</t>
+        </is>
+      </c>
       <c r="X51" t="inlineStr">
         <is>
-          <t>Legge federale sulla protezione della popolazione e sulla protezione civile del 4 ottobre 2002</t>
+          <t>Decreto Legislativo 2 Gennaio 2018, N. 1, Codice Della Protezione Civile. (18G00011)</t>
         </is>
       </c>
       <c r="Y51" t="inlineStr">
         <is>
-          <t>Confederazion elvetica</t>
+          <t>Presidenza Del Consiglio Dei Ministri</t>
         </is>
       </c>
       <c r="Z51" t="inlineStr">
         <is>
-          <t>Confederazione elvetica</t>
+          <t>Gazzetta Ufficiale</t>
         </is>
       </c>
       <c r="AA51" t="inlineStr">
         <is>
-          <t>https://www.admin.ch/opc/it/classified-compilation/20011872/201701010000/520.1.pdf</t>
+          <t>https://www.gazzettaufficiale.it/eli/id/2018/1/22/18G00011/sg</t>
         </is>
       </c>
       <c r="AB51" t="inlineStr">
@@ -5621,7 +5657,7 @@
         <v>3000051</v>
       </c>
       <c r="E52" t="n">
-        <v>4000002</v>
+        <v>4000001</v>
       </c>
       <c r="F52" t="n">
         <v>5000001</v>
@@ -5630,90 +5666,75 @@
         <v>6000051</v>
       </c>
       <c r="H52" t="n">
-        <v>7000051</v>
+        <v>7000001</v>
       </c>
       <c r="I52" t="n">
-        <v>8000019</v>
+        <v>8000047</v>
       </c>
       <c r="J52" t="n">
-        <v>9000019</v>
+        <v>9000003</v>
       </c>
       <c r="K52" t="n">
-        <v>10000019</v>
+        <v>10000025</v>
       </c>
       <c r="L52" t="n">
-        <v>11000049</v>
+        <v>11000047</v>
       </c>
       <c r="M52" t="n">
-        <v>12000050</v>
+        <v>12000001</v>
       </c>
       <c r="N52" t="n">
-        <v>13000048</v>
+        <v>13000047</v>
       </c>
       <c r="O52" t="n">
-        <v>14000050</v>
+        <v>14000051</v>
       </c>
       <c r="P52" t="n">
         <v>15000001</v>
       </c>
       <c r="Q52" t="inlineStr">
         <is>
-          <t>Struttura operativa</t>
+          <t>Organo di condotta</t>
         </is>
       </c>
       <c r="R52" t="inlineStr"/>
       <c r="S52" t="inlineStr">
         <is>
-          <t>Oltre al Corpo nazionale dei vigili del fuoco, che opera quale componente fondamentale del Servizio nazionale della protezione civile, sono strutture operative nazionali: a) le Forze armate; b) le Forze di polizia; c) gli enti e istituti di ricerca di rilievo nazionale con finalità di protezione civile, anche organizzati come centri di competenza, l'Istituto nazionale di geofisica e vulcanologia e il Consiglio nazionale delle ricerche; d) le strutture del Servizio sanitario nazionale; e) il volontariato organizzato di protezione civile iscritto nell'elenco nazionale del volontariato di protezione civile, l'Associazione della Croce rossa italiana e il Corpo nazionale del soccorso alpino e speleologico; f) il Sistema nazionale per la protezione dell'ambiente; g) le strutture preposte alla gestione dei servizi meteorologici a livello nazionale.</t>
-        </is>
-      </c>
-      <c r="T52" t="inlineStr">
-        <is>
-          <t>Competenza della Protezione Civile</t>
-        </is>
-      </c>
+          <t>Gli organi di condotta vengono istituiti dalle autorità competenti per lo svolgimento dei seguenti compiti: a - informare la popolazione in merito ai pericoli che la minacciano come pure alle possibilità e alle misure di protezione esistenti; b - avvertire, dare l’allarme e impartire alla popolazione istruzioni sul comportamento; c - assicurare le attività di condotta; d - coordinare i preparativi e gli interventi delle 
+ organizzazioni partner; e - garantire, tempestivamente e in funzione della situazione, la disponibilità operativa e il rinforzo con personale e materiale della protezione della popolazione in vista di un conflitto armato.</t>
+        </is>
+      </c>
+      <c r="T52" t="inlineStr"/>
       <c r="U52" t="inlineStr"/>
       <c r="V52" t="inlineStr">
         <is>
-          <t>Art. 13</t>
-        </is>
-      </c>
-      <c r="W52" t="inlineStr">
-        <is>
-          <t>https://www.gazzettaufficiale.it/atto/serie_generale/caricaArticolo?art.progressivo=0&amp;art.idArticolo=13&amp;art.versione=1&amp;art.codiceRedazionale=18G00011&amp;art.dataPubblicazioneGazzetta=2018-01-22&amp;art.idGruppo=3&amp;art.idSottoArticolo1=10&amp;art.idSottoArticolo=1&amp;art.flagTipoArticolo=0#art</t>
-        </is>
-      </c>
+          <t>Art. 4</t>
+        </is>
+      </c>
+      <c r="W52" t="inlineStr"/>
       <c r="X52" t="inlineStr">
         <is>
-          <t>Decreto Legislativo 2 Gennaio 2018, N. 1, Codice Della Protezione Civile. (18G00011)</t>
-        </is>
-      </c>
-      <c r="Y52" t="inlineStr">
-        <is>
-          <t>Presidenza Del Consiglio Dei Ministri</t>
-        </is>
-      </c>
+          <t>Legge federale sulla protezione della popolazione e sulla protezione civile del 4 ottobre 2002</t>
+        </is>
+      </c>
+      <c r="Y52" t="inlineStr"/>
       <c r="Z52" t="inlineStr">
         <is>
-          <t>Gazzetta Ufficiale</t>
+          <t>Confederazione Elvetica</t>
         </is>
       </c>
       <c r="AA52" t="inlineStr">
         <is>
-          <t>https://www.gazzettaufficiale.it/eli/id/2018/1/22/18G00011/sg</t>
-        </is>
-      </c>
-      <c r="AB52" t="inlineStr">
-        <is>
-          <t>strutture operative in italia e organizzazioni partner in svizzera hanno la stessa connotazione all'interno di un sistema di protezione della popolazione.</t>
-        </is>
-      </c>
+          <t>https://www.admin.ch/opc/it/classified-compilation/20011872/201701010000/520.1.pdf</t>
+        </is>
+      </c>
+      <c r="AB52" t="inlineStr"/>
       <c r="AC52" s="2" t="n">
         <v>43766</v>
       </c>
       <c r="AD52" t="inlineStr">
         <is>
-          <t>ITCH00010</t>
+          <t>ITCH00011</t>
         </is>
       </c>
       <c r="AE52" t="inlineStr">
@@ -5736,34 +5757,34 @@
         <v>3000052</v>
       </c>
       <c r="E53" t="n">
-        <v>4000001</v>
+        <v>4000019</v>
       </c>
       <c r="F53" t="n">
-        <v>5000001</v>
+        <v>5000032</v>
       </c>
       <c r="G53" t="n">
         <v>6000052</v>
       </c>
       <c r="H53" t="n">
-        <v>7000001</v>
+        <v>7000024</v>
       </c>
       <c r="I53" t="n">
-        <v>8000048</v>
+        <v>8000019</v>
       </c>
       <c r="J53" t="n">
-        <v>9000003</v>
+        <v>9000019</v>
       </c>
       <c r="K53" t="n">
-        <v>10000026</v>
+        <v>10000019</v>
       </c>
       <c r="L53" t="n">
-        <v>11000048</v>
+        <v>11000019</v>
       </c>
       <c r="M53" t="n">
-        <v>12000001</v>
+        <v>12000052</v>
       </c>
       <c r="N53" t="n">
-        <v>13000048</v>
+        <v>13000032</v>
       </c>
       <c r="O53" t="n">
         <v>14000052</v>
@@ -5773,47 +5794,66 @@
       </c>
       <c r="Q53" t="inlineStr">
         <is>
-          <t>Organo di condotta</t>
+          <t>Emergenza / Stato di emergenza / Evento emergenziale / Evento</t>
         </is>
       </c>
       <c r="R53" t="inlineStr"/>
       <c r="S53" t="inlineStr">
         <is>
-          <t>Gli organi di condotta vengono istituiti dalle autorità competenti per lo svolgimento dei seguenti compiti: a - informare la popolazione in merito ai pericoli che la minacciano come pure alle possibilità e alle misure di protezione esistenti; b - avvertire, dare l’allarme e impartire alla popolazione istruzioni sul comportamento; c - assicurare le attività di condotta; d - coordinare i preparativi e gli interventi delle 
- organizzazioni partner; e - garantire, tempestivamente e in funzione della situazione, la disponibilità operativa e il rinforzo con personale e materiale della protezione della popolazione in vista di un conflitto armato.</t>
-        </is>
-      </c>
-      <c r="T53" t="inlineStr"/>
-      <c r="U53" t="inlineStr"/>
+          <t>Indica l'insieme delle emergenze di tipo A, B e C così come definiti dall' Art. 7, comma 1 del DL 02/01/2018, n°1.</t>
+        </is>
+      </c>
+      <c r="T53" t="inlineStr">
+        <is>
+          <t>Competenza di protezione civile</t>
+        </is>
+      </c>
+      <c r="U53" t="inlineStr">
+        <is>
+          <t>Tommaso Sansone</t>
+        </is>
+      </c>
       <c r="V53" t="inlineStr">
         <is>
-          <t>Art. 4</t>
-        </is>
-      </c>
-      <c r="W53" t="inlineStr"/>
+          <t>Art 7, Comma 1</t>
+        </is>
+      </c>
+      <c r="W53" t="inlineStr">
+        <is>
+          <t>https://www.gazzettaufficiale.it/atto/serie_generale/caricaArticolo?art.progressivo=0&amp;art.idArticolo=7&amp;art.versione=1&amp;art.codiceRedazionale=18G00011&amp;art.dataPubblicazioneGazzetta=2018-01-22&amp;art.idGruppo=2&amp;art.idSottoArticolo1=10&amp;art.idSottoArticolo=1&amp;art.flagTipoArticolo=0</t>
+        </is>
+      </c>
       <c r="X53" t="inlineStr">
         <is>
-          <t>Legge federale sulla protezione della popolazione e sulla protezione civile del 4 ottobre 2002</t>
-        </is>
-      </c>
-      <c r="Y53" t="inlineStr"/>
+          <t>Decreto Legislativo 2 Gennaio 2018, N. 1, Codice Della Protezione Civile. (18G00011)</t>
+        </is>
+      </c>
+      <c r="Y53" t="inlineStr">
+        <is>
+          <t>Presidenza Del Consiglio Dei Ministri</t>
+        </is>
+      </c>
       <c r="Z53" t="inlineStr">
         <is>
-          <t>Confederazione Elvetica</t>
+          <t>Gazzetta Ufficiale</t>
         </is>
       </c>
       <c r="AA53" t="inlineStr">
         <is>
-          <t>https://www.admin.ch/opc/it/classified-compilation/20011872/201701010000/520.1.pdf</t>
-        </is>
-      </c>
-      <c r="AB53" t="inlineStr"/>
+          <t>http://www.gazzettaufficiale.it/eli/id/2018/1/22/18G00011/sg</t>
+        </is>
+      </c>
+      <c r="AB53" t="inlineStr">
+        <is>
+          <t>Per il lato italiano, definizione rielaborata da Tommaso Sansone a partire dall'art 7 del decreto di protezione civile 2-1-2018</t>
+        </is>
+      </c>
       <c r="AC53" s="2" t="n">
-        <v>43766</v>
+        <v>43412</v>
       </c>
       <c r="AD53" t="inlineStr">
         <is>
-          <t>ITCH00011</t>
+          <t>ITCH00012</t>
         </is>
       </c>
       <c r="AE53" t="inlineStr">
@@ -5827,99 +5867,83 @@
         <v>52</v>
       </c>
       <c r="B54" t="n">
-        <v>1000054</v>
+        <v>1000053</v>
       </c>
       <c r="C54" t="n">
         <v>2000001</v>
       </c>
       <c r="D54" t="n">
-        <v>3000054</v>
+        <v>3000053</v>
       </c>
       <c r="E54" t="n">
-        <v>4000019</v>
+        <v>4000001</v>
       </c>
       <c r="F54" t="n">
-        <v>5000032</v>
+        <v>5000001</v>
       </c>
       <c r="G54" t="n">
-        <v>6000054</v>
+        <v>6000053</v>
       </c>
       <c r="H54" t="n">
-        <v>7000024</v>
+        <v>7000001</v>
       </c>
       <c r="I54" t="n">
-        <v>8000019</v>
+        <v>8000053</v>
       </c>
       <c r="J54" t="n">
-        <v>9000019</v>
+        <v>9000003</v>
       </c>
       <c r="K54" t="n">
-        <v>10000019</v>
+        <v>10000041</v>
       </c>
       <c r="L54" t="n">
-        <v>11000019</v>
+        <v>11000053</v>
       </c>
       <c r="M54" t="n">
-        <v>12000053</v>
+        <v>12000052</v>
       </c>
       <c r="N54" t="n">
         <v>13000032</v>
       </c>
       <c r="O54" t="n">
-        <v>14000053</v>
+        <v>14000052</v>
       </c>
       <c r="P54" t="n">
         <v>15000001</v>
       </c>
       <c r="Q54" t="inlineStr">
         <is>
-          <t>Emergenza / Stato di emergenza / Evento emergenziale / Evento</t>
+          <t>Stato di necessità</t>
         </is>
       </c>
       <c r="R54" t="inlineStr"/>
       <c r="S54" t="inlineStr">
         <is>
-          <t>Indica l'insieme delle emergenze di tipo A, B e C così come definiti dall' Art. 7, comma 1 del DL 02/01/2018, n°1.</t>
-        </is>
-      </c>
-      <c r="T54" t="inlineStr">
-        <is>
-          <t>Competenza di protezione civile</t>
-        </is>
-      </c>
-      <c r="U54" t="inlineStr">
-        <is>
-          <t>Tommaso Sansone</t>
-        </is>
-      </c>
+          <t>Si ha stato di necessità quando, a seguito di catastrofi, conflitti armati o altre situazioni d’emergenza che comportano un pericolo imminente per lo Stato, le persone o le cose, non sia più possibile garantire con i mezzi ordinari l’attività amministrativa o i servizi d’interesse pubblico e la protezione e l’assistenza delle persone e delle cose a livello cantonale, regionale o locale.</t>
+        </is>
+      </c>
+      <c r="T54" t="inlineStr"/>
+      <c r="U54" t="inlineStr"/>
       <c r="V54" t="inlineStr">
         <is>
-          <t>Art 7, Comma 1</t>
-        </is>
-      </c>
-      <c r="W54" t="inlineStr">
-        <is>
-          <t>https://www.gazzettaufficiale.it/atto/serie_generale/caricaArticolo?art.progressivo=0&amp;art.idArticolo=7&amp;art.versione=1&amp;art.codiceRedazionale=18G00011&amp;art.dataPubblicazioneGazzetta=2018-01-22&amp;art.idGruppo=2&amp;art.idSottoArticolo1=10&amp;art.idSottoArticolo=1&amp;art.flagTipoArticolo=0</t>
-        </is>
-      </c>
+          <t>Art. 20</t>
+        </is>
+      </c>
+      <c r="W54" t="inlineStr"/>
       <c r="X54" t="inlineStr">
         <is>
-          <t>Decreto Legislativo 2 Gennaio 2018, N. 1, Codice Della Protezione Civile. (18G00011)</t>
-        </is>
-      </c>
-      <c r="Y54" t="inlineStr">
-        <is>
-          <t>Presidenza Del Consiglio Dei Ministri</t>
-        </is>
-      </c>
+          <t>Legge sulla protezione della popolazione (del 26 febbraio 2007)</t>
+        </is>
+      </c>
+      <c r="Y54" t="inlineStr"/>
       <c r="Z54" t="inlineStr">
         <is>
-          <t>Gazzetta Ufficiale</t>
+          <t>Repubblica e Cantone Ticino</t>
         </is>
       </c>
       <c r="AA54" t="inlineStr">
         <is>
-          <t>http://www.gazzettaufficiale.it/eli/id/2018/1/22/18G00011/sg</t>
+          <t>https://m3.ti.ch/CAN/RLeggi/public/index.php/raccolta-leggi/legge/num/48</t>
         </is>
       </c>
       <c r="AB54" t="inlineStr">
@@ -5946,13 +5970,13 @@
         <v>53</v>
       </c>
       <c r="B55" t="n">
-        <v>1000053</v>
+        <v>1000054</v>
       </c>
       <c r="C55" t="n">
         <v>2000001</v>
       </c>
       <c r="D55" t="n">
-        <v>3000053</v>
+        <v>3000054</v>
       </c>
       <c r="E55" t="n">
         <v>4000001</v>
@@ -5961,81 +5985,77 @@
         <v>5000001</v>
       </c>
       <c r="G55" t="n">
-        <v>6000053</v>
+        <v>6000054</v>
       </c>
       <c r="H55" t="n">
         <v>7000001</v>
       </c>
       <c r="I55" t="n">
-        <v>8000053</v>
+        <v>8000047</v>
       </c>
       <c r="J55" t="n">
         <v>9000003</v>
       </c>
       <c r="K55" t="n">
-        <v>10000042</v>
+        <v>10000025</v>
       </c>
       <c r="L55" t="n">
-        <v>11000053</v>
+        <v>11000047</v>
       </c>
       <c r="M55" t="n">
-        <v>12000053</v>
+        <v>12000001</v>
       </c>
       <c r="N55" t="n">
-        <v>13000032</v>
+        <v>13000047</v>
       </c>
       <c r="O55" t="n">
-        <v>14000053</v>
+        <v>14000054</v>
       </c>
       <c r="P55" t="n">
         <v>15000001</v>
       </c>
       <c r="Q55" t="inlineStr">
         <is>
-          <t>Stato di necessità</t>
+          <t>Impianto di protezione</t>
         </is>
       </c>
       <c r="R55" t="inlineStr"/>
       <c r="S55" t="inlineStr">
         <is>
-          <t>Si ha stato di necessità quando, a seguito di catastrofi, conflitti armati o altre situazioni d’emergenza che comportano un pericolo imminente per lo Stato, le persone o le cose, non sia più possibile garantire con i mezzi ordinari l’attività amministrativa o i servizi d’interesse pubblico e la protezione e l’assistenza delle persone e delle cose a livello cantonale, regionale o locale.</t>
+          <t>Sono impianti di protezione: a - i posti di comando; b. gli impianti d’apprestamento; c - i centri sanitari protetti; d - gli ospedali protetti.</t>
         </is>
       </c>
       <c r="T55" t="inlineStr"/>
       <c r="U55" t="inlineStr"/>
       <c r="V55" t="inlineStr">
         <is>
-          <t>Art. 20</t>
+          <t>Art. 50</t>
         </is>
       </c>
       <c r="W55" t="inlineStr"/>
       <c r="X55" t="inlineStr">
         <is>
-          <t>Legge sulla protezione della popolazione (del 26 febbraio 2007)</t>
+          <t>Legge federale sulla protezione della popolazione e sulla protezione civile del 4 ottobre 2002</t>
         </is>
       </c>
       <c r="Y55" t="inlineStr"/>
       <c r="Z55" t="inlineStr">
         <is>
-          <t>Repubblica e Cantone Ticino</t>
+          <t>Confederazione Elvetica</t>
         </is>
       </c>
       <c r="AA55" t="inlineStr">
         <is>
-          <t>https://m3.ti.ch/CAN/RLeggi/public/index.php/raccolta-leggi/legge/num/48</t>
-        </is>
-      </c>
-      <c r="AB55" t="inlineStr">
-        <is>
-          <t>Per il lato italiano, definizione rielaborata da Tommaso Sansone a partire dall'art 7 del decreto di protezione civile 2-1-2018</t>
-        </is>
-      </c>
+          <t>https://www.admin.ch/opc/it/classified-compilation/20011872/201701010000/520.1.pdf</t>
+        </is>
+      </c>
+      <c r="AB55" t="inlineStr"/>
       <c r="AC55" s="2" t="n">
-        <v>43412</v>
+        <v>43766</v>
       </c>
       <c r="AD55" t="inlineStr">
         <is>
-          <t>ITCH00012</t>
+          <t>ITCH00013</t>
         </is>
       </c>
       <c r="AE55" t="inlineStr">
@@ -6070,22 +6090,22 @@
         <v>7000001</v>
       </c>
       <c r="I56" t="n">
-        <v>8000048</v>
+        <v>8000047</v>
       </c>
       <c r="J56" t="n">
         <v>9000003</v>
       </c>
       <c r="K56" t="n">
-        <v>10000026</v>
+        <v>10000025</v>
       </c>
       <c r="L56" t="n">
-        <v>11000048</v>
+        <v>11000047</v>
       </c>
       <c r="M56" t="n">
         <v>12000001</v>
       </c>
       <c r="N56" t="n">
-        <v>13000048</v>
+        <v>13000047</v>
       </c>
       <c r="O56" t="n">
         <v>14000055</v>
@@ -6095,20 +6115,20 @@
       </c>
       <c r="Q56" t="inlineStr">
         <is>
-          <t>Impianto di protezione</t>
+          <t>Costruzione di protezione</t>
         </is>
       </c>
       <c r="R56" t="inlineStr"/>
       <c r="S56" t="inlineStr">
         <is>
-          <t>Sono impianti di protezione: a - i posti di comando; b. gli impianti d’apprestamento; c - i centri sanitari protetti; d - gli ospedali protetti.</t>
+          <t>Le Costruzioni di protezione si distinguono in rifugi e impianti di protezione. Sono edifici che vengono costruiti o utilizzati ai fini di protezione della popolazione.</t>
         </is>
       </c>
       <c r="T56" t="inlineStr"/>
       <c r="U56" t="inlineStr"/>
       <c r="V56" t="inlineStr">
         <is>
-          <t>Art. 50</t>
+          <t>Art. 45 e Art. 50</t>
         </is>
       </c>
       <c r="W56" t="inlineStr"/>
@@ -6134,7 +6154,7 @@
       </c>
       <c r="AD56" t="inlineStr">
         <is>
-          <t>ITCH00013</t>
+          <t>ITCH00014</t>
         </is>
       </c>
       <c r="AE56" t="inlineStr">
@@ -6169,22 +6189,22 @@
         <v>7000001</v>
       </c>
       <c r="I57" t="n">
-        <v>8000048</v>
+        <v>8000047</v>
       </c>
       <c r="J57" t="n">
         <v>9000003</v>
       </c>
       <c r="K57" t="n">
-        <v>10000026</v>
+        <v>10000025</v>
       </c>
       <c r="L57" t="n">
-        <v>11000048</v>
+        <v>11000047</v>
       </c>
       <c r="M57" t="n">
         <v>12000001</v>
       </c>
       <c r="N57" t="n">
-        <v>13000048</v>
+        <v>13000047</v>
       </c>
       <c r="O57" t="n">
         <v>14000056</v>
@@ -6194,20 +6214,20 @@
       </c>
       <c r="Q57" t="inlineStr">
         <is>
-          <t>Costruzione di protezione</t>
+          <t>Rifugio</t>
         </is>
       </c>
       <c r="R57" t="inlineStr"/>
       <c r="S57" t="inlineStr">
         <is>
-          <t>Le Costruzioni di protezione si distinguono in rifugi e impianti di protezione. Sono edifici che vengono costruiti o utilizzati ai fini di protezione della popolazione.</t>
+          <t>posto protetto di cui ogni abitante deve disporre e che sia raggiungibile in tempo utile dalla propria abitazione.</t>
         </is>
       </c>
       <c r="T57" t="inlineStr"/>
       <c r="U57" t="inlineStr"/>
       <c r="V57" t="inlineStr">
         <is>
-          <t>Art. 45 e Art. 50</t>
+          <t>Art. 45</t>
         </is>
       </c>
       <c r="W57" t="inlineStr"/>
@@ -6233,7 +6253,7 @@
       </c>
       <c r="AD57" t="inlineStr">
         <is>
-          <t>ITCH00014</t>
+          <t>ITCH00015</t>
         </is>
       </c>
       <c r="AE57" t="inlineStr">
@@ -6268,22 +6288,22 @@
         <v>7000001</v>
       </c>
       <c r="I58" t="n">
-        <v>8000048</v>
+        <v>8000057</v>
       </c>
       <c r="J58" t="n">
-        <v>9000003</v>
+        <v>9000057</v>
       </c>
       <c r="K58" t="n">
-        <v>10000026</v>
+        <v>10000025</v>
       </c>
       <c r="L58" t="n">
-        <v>11000048</v>
+        <v>11000057</v>
       </c>
       <c r="M58" t="n">
         <v>12000001</v>
       </c>
       <c r="N58" t="n">
-        <v>13000048</v>
+        <v>13000040</v>
       </c>
       <c r="O58" t="n">
         <v>14000057</v>
@@ -6293,29 +6313,33 @@
       </c>
       <c r="Q58" t="inlineStr">
         <is>
-          <t>Rifugio</t>
+          <t>Addetto all'assistenza</t>
         </is>
       </c>
       <c r="R58" t="inlineStr"/>
       <c r="S58" t="inlineStr">
         <is>
-          <t>posto protetto di cui ogni abitante deve disporre e che sia raggiungibile in tempo utile dalla propria abitazione.</t>
+          <t>milite impiegato, in funzione dell'evento o della situazione d'emergenza, per assistere persone in cerca di protezione (senzatetto, evacuati, ecc.) o aiutare i servizi della sanità pubblica (per es. in case per anziani). L'addetto all'assistenza deve disporre di buone competenze sociali e capacità organizzative.</t>
         </is>
       </c>
       <c r="T58" t="inlineStr"/>
       <c r="U58" t="inlineStr"/>
       <c r="V58" t="inlineStr">
         <is>
-          <t>Art. 45</t>
+          <t>pag 10</t>
         </is>
       </c>
       <c r="W58" t="inlineStr"/>
       <c r="X58" t="inlineStr">
         <is>
-          <t>Legge federale sulla protezione della popolazione e sulla protezione civile del 4 ottobre 2002</t>
-        </is>
-      </c>
-      <c r="Y58" t="inlineStr"/>
+          <t>Il comando della protezione civile - Personale</t>
+        </is>
+      </c>
+      <c r="Y58" t="inlineStr">
+        <is>
+          <t>Ufficio Federale della Protezione della Popolazione</t>
+        </is>
+      </c>
       <c r="Z58" t="inlineStr">
         <is>
           <t>Confederazione Elvetica</t>
@@ -6323,16 +6347,16 @@
       </c>
       <c r="AA58" t="inlineStr">
         <is>
-          <t>https://www.admin.ch/opc/it/classified-compilation/20011872/201701010000/520.1.pdf</t>
+          <t>https://www.babs.admin.ch/content/babs-internet/it/publikservice/downloads/unterlagen-ausbildung/_jcr_content/contentPar/accordion_1920886228/accordionItems/kommando_zivilschutz/accordionPar/downloadlist_copy/downloadItems/829_1459931125997.download/personal170191103it.pdf</t>
         </is>
       </c>
       <c r="AB58" t="inlineStr"/>
       <c r="AC58" s="2" t="n">
-        <v>43766</v>
+        <v>43767</v>
       </c>
       <c r="AD58" t="inlineStr">
         <is>
-          <t>ITCH00015</t>
+          <t>ITCH00016</t>
         </is>
       </c>
       <c r="AE58" t="inlineStr">
@@ -6367,22 +6391,22 @@
         <v>7000001</v>
       </c>
       <c r="I59" t="n">
-        <v>8000058</v>
+        <v>8000057</v>
       </c>
       <c r="J59" t="n">
-        <v>9000058</v>
+        <v>9000057</v>
       </c>
       <c r="K59" t="n">
-        <v>10000026</v>
+        <v>10000025</v>
       </c>
       <c r="L59" t="n">
-        <v>11000058</v>
+        <v>11000057</v>
       </c>
       <c r="M59" t="n">
         <v>12000001</v>
       </c>
       <c r="N59" t="n">
-        <v>13000058</v>
+        <v>13000040</v>
       </c>
       <c r="O59" t="n">
         <v>14000058</v>
@@ -6392,20 +6416,20 @@
       </c>
       <c r="Q59" t="inlineStr">
         <is>
-          <t>Addetto all'assistenza</t>
+          <t>Assistente di stato maggiore</t>
         </is>
       </c>
       <c r="R59" t="inlineStr"/>
       <c r="S59" t="inlineStr">
         <is>
-          <t>milite impiegato, in funzione dell'evento o della situazione d'emergenza, per assistere persone in cerca di protezione (senzatetto, evacuati, ecc.) o aiutare i servizi della sanità pubblica (per es. in case per anziani). L'addetto all'assistenza deve disporre di buone competenze sociali e capacità organizzative.</t>
+          <t>milite impiegato per prestare aiuto alla condotta in seno all'organo di condotta o a favore dei partner ed istruito in materia di analisi della situazione e telematica. L'assistente di stato maggiore deve essere polivalente.</t>
         </is>
       </c>
       <c r="T59" t="inlineStr"/>
       <c r="U59" t="inlineStr"/>
       <c r="V59" t="inlineStr">
         <is>
-          <t>pag 10</t>
+          <t>pag 9</t>
         </is>
       </c>
       <c r="W59" t="inlineStr"/>
@@ -6435,7 +6459,7 @@
       </c>
       <c r="AD59" t="inlineStr">
         <is>
-          <t>ITCH00016</t>
+          <t>ITCH00017</t>
         </is>
       </c>
       <c r="AE59" t="inlineStr">
@@ -6458,7 +6482,7 @@
         <v>3000059</v>
       </c>
       <c r="E60" t="n">
-        <v>4000001</v>
+        <v>4000002</v>
       </c>
       <c r="F60" t="n">
         <v>5000001</v>
@@ -6470,22 +6494,22 @@
         <v>7000001</v>
       </c>
       <c r="I60" t="n">
-        <v>8000058</v>
+        <v>8000059</v>
       </c>
       <c r="J60" t="n">
-        <v>9000058</v>
+        <v>9000003</v>
       </c>
       <c r="K60" t="n">
-        <v>10000026</v>
+        <v>10000041</v>
       </c>
       <c r="L60" t="n">
-        <v>11000058</v>
+        <v>11000059</v>
       </c>
       <c r="M60" t="n">
         <v>12000001</v>
       </c>
       <c r="N60" t="n">
-        <v>13000058</v>
+        <v>13000040</v>
       </c>
       <c r="O60" t="n">
         <v>14000059</v>
@@ -6495,41 +6519,41 @@
       </c>
       <c r="Q60" t="inlineStr">
         <is>
-          <t>Assistente di stato maggiore</t>
+          <t>Organizzazione degli Stati maggiori di condotta</t>
         </is>
       </c>
       <c r="R60" t="inlineStr"/>
       <c r="S60" t="inlineStr">
         <is>
-          <t>milite impiegato per prestare aiuto alla condotta in seno all'organo di condotta o a favore dei partner ed istruito in materia di analisi della situazione e telematica. L'assistente di stato maggiore deve essere polivalente.</t>
-        </is>
-      </c>
-      <c r="T60" t="inlineStr"/>
+          <t>L’Organizzazione degli Stati maggiori di condotta (OSMC) è composta dai rappresentanti della Polizia cantonale, della Federazione cantonale ticinese corpi pompieri, della Federazione cantonale ticinese servizi autoambulanze, del Servizio della protezione civile cantonale, dei servizi tecnici e del Dipartimento delle istituzioni; ogni organizzazione designa il proprio rappresentante. A seconda delle necessità possono essere designati ulteriori responsabili per i servizi tecnici. L’OSMC è diretta dal rappresentante del Dipartimento.</t>
+        </is>
+      </c>
+      <c r="T60" t="inlineStr">
+        <is>
+          <t>Competenza della Protezione Civile</t>
+        </is>
+      </c>
       <c r="U60" t="inlineStr"/>
       <c r="V60" t="inlineStr">
         <is>
-          <t>pag 9</t>
+          <t>Art. 6</t>
         </is>
       </c>
       <c r="W60" t="inlineStr"/>
       <c r="X60" t="inlineStr">
         <is>
-          <t>Il comando della protezione civile - Personale</t>
-        </is>
-      </c>
-      <c r="Y60" t="inlineStr">
-        <is>
-          <t>Ufficio Federale della Protezione della Popolazione</t>
-        </is>
-      </c>
+          <t>Regolamento sulla protezione della popolazione (RProtPop) (del 18 ottobre 2017)</t>
+        </is>
+      </c>
+      <c r="Y60" t="inlineStr"/>
       <c r="Z60" t="inlineStr">
         <is>
-          <t>Confederazione Elvetica</t>
+          <t>Repubblica e Cantone Ticino</t>
         </is>
       </c>
       <c r="AA60" t="inlineStr">
         <is>
-          <t>https://www.babs.admin.ch/content/babs-internet/it/publikservice/downloads/unterlagen-ausbildung/_jcr_content/contentPar/accordion_1920886228/accordionItems/kommando_zivilschutz/accordionPar/downloadlist_copy/downloadItems/829_1459931125997.download/personal170191103it.pdf</t>
+          <t>https://m3.ti.ch/CAN/RLeggi/public/index.php/index/nuovafinestra/atto/49/volume/5%20SICUREZZA/numLegge/500.110</t>
         </is>
       </c>
       <c r="AB60" t="inlineStr"/>
@@ -6538,7 +6562,7 @@
       </c>
       <c r="AD60" t="inlineStr">
         <is>
-          <t>ITCH00017</t>
+          <t>ITCH00018</t>
         </is>
       </c>
       <c r="AE60" t="inlineStr">
@@ -6561,34 +6585,34 @@
         <v>3000060</v>
       </c>
       <c r="E61" t="n">
-        <v>4000002</v>
+        <v>4000001</v>
       </c>
       <c r="F61" t="n">
         <v>5000001</v>
       </c>
       <c r="G61" t="n">
-        <v>6000060</v>
+        <v>6000057</v>
       </c>
       <c r="H61" t="n">
         <v>7000001</v>
       </c>
       <c r="I61" t="n">
-        <v>8000060</v>
+        <v>8000057</v>
       </c>
       <c r="J61" t="n">
-        <v>9000003</v>
+        <v>9000057</v>
       </c>
       <c r="K61" t="n">
-        <v>10000042</v>
+        <v>10000025</v>
       </c>
       <c r="L61" t="n">
-        <v>11000060</v>
+        <v>11000057</v>
       </c>
       <c r="M61" t="n">
         <v>12000001</v>
       </c>
       <c r="N61" t="n">
-        <v>13000058</v>
+        <v>13000040</v>
       </c>
       <c r="O61" t="n">
         <v>14000060</v>
@@ -6598,41 +6622,44 @@
       </c>
       <c r="Q61" t="inlineStr">
         <is>
-          <t>Organizzazione degli Stati maggiori di condotta</t>
+          <t>Pioniere</t>
         </is>
       </c>
       <c r="R61" t="inlineStr"/>
       <c r="S61" t="inlineStr">
         <is>
-          <t>L’Organizzazione degli Stati maggiori di condotta (OSMC) è composta dai rappresentanti della Polizia cantonale, della Federazione cantonale ticinese corpi pompieri, della Federazione cantonale ticinese servizi autoambulanze, del Servizio della protezione civile cantonale, dei servizi tecnici e del Dipartimento delle istituzioni; ogni organizzazione designa il proprio rappresentante. A seconda delle necessità possono essere designati ulteriori responsabili per i servizi tecnici. L’OSMC è diretta dal rappresentante del Dipartimento.</t>
-        </is>
-      </c>
-      <c r="T61" t="inlineStr">
-        <is>
-          <t>Competenza della Protezione Civile</t>
-        </is>
-      </c>
+          <t>milite impiegato soprattutto per assistere le organizzazioni
+partner nell'esecuzione dei lavori necessari per limitare o ripristinare i
+danni. Il pioniere deve presentare una corporatura robusta ed essere
+abile al lavoro manuale.</t>
+        </is>
+      </c>
+      <c r="T61" t="inlineStr"/>
       <c r="U61" t="inlineStr"/>
       <c r="V61" t="inlineStr">
         <is>
-          <t>Art. 6</t>
+          <t>pag 10</t>
         </is>
       </c>
       <c r="W61" t="inlineStr"/>
       <c r="X61" t="inlineStr">
         <is>
-          <t>Regolamento sulla protezione della popolazione (RProtPop) (del 18 ottobre 2017)</t>
-        </is>
-      </c>
-      <c r="Y61" t="inlineStr"/>
+          <t>Il comando della protezione civile - Personale</t>
+        </is>
+      </c>
+      <c r="Y61" t="inlineStr">
+        <is>
+          <t>Ufficio Federale della Protezione della Popolazione</t>
+        </is>
+      </c>
       <c r="Z61" t="inlineStr">
         <is>
-          <t>Repubblica e Cantone Ticino</t>
+          <t>Confederazione Elvetica</t>
         </is>
       </c>
       <c r="AA61" t="inlineStr">
         <is>
-          <t>https://m3.ti.ch/CAN/RLeggi/public/index.php/index/nuovafinestra/atto/49/volume/5%20SICUREZZA/numLegge/500.110</t>
+          <t>https://www.babs.admin.ch/content/babs-internet/it/publikservice/downloads/unterlagen-ausbildung/_jcr_content/contentPar/accordion_1920886228/accordionItems/kommando_zivilschutz/accordionPar/downloadlist_copy/downloadItems/829_1459931125997.download/personal170191103it.pdf</t>
         </is>
       </c>
       <c r="AB61" t="inlineStr"/>
@@ -6641,7 +6668,7 @@
       </c>
       <c r="AD61" t="inlineStr">
         <is>
-          <t>ITCH00018</t>
+          <t>ITCH00019</t>
         </is>
       </c>
       <c r="AE61" t="inlineStr">
@@ -6664,34 +6691,34 @@
         <v>3000061</v>
       </c>
       <c r="E62" t="n">
-        <v>4000001</v>
+        <v>4000002</v>
       </c>
       <c r="F62" t="n">
         <v>5000001</v>
       </c>
       <c r="G62" t="n">
-        <v>6000058</v>
+        <v>6000048</v>
       </c>
       <c r="H62" t="n">
         <v>7000001</v>
       </c>
       <c r="I62" t="n">
-        <v>8000058</v>
+        <v>8000053</v>
       </c>
       <c r="J62" t="n">
-        <v>9000058</v>
+        <v>9000003</v>
       </c>
       <c r="K62" t="n">
-        <v>10000026</v>
+        <v>10000041</v>
       </c>
       <c r="L62" t="n">
-        <v>11000058</v>
+        <v>11000053</v>
       </c>
       <c r="M62" t="n">
         <v>12000001</v>
       </c>
       <c r="N62" t="n">
-        <v>13000058</v>
+        <v>13000040</v>
       </c>
       <c r="O62" t="n">
         <v>14000061</v>
@@ -6701,44 +6728,41 @@
       </c>
       <c r="Q62" t="inlineStr">
         <is>
-          <t>Pioniere</t>
+          <t>Stato maggiore cantonale di condotta</t>
         </is>
       </c>
       <c r="R62" t="inlineStr"/>
       <c r="S62" t="inlineStr">
         <is>
-          <t>milite impiegato soprattutto per assistere le organizzazioni
-partner nell'esecuzione dei lavori necessari per limitare o ripristinare i
-danni. Il pioniere deve presentare una corporatura robusta ed essere
-abile al lavoro manuale.</t>
-        </is>
-      </c>
-      <c r="T62" t="inlineStr"/>
+          <t>Lo SMCC è l’organo cantonale di condotta del Consiglio di Stato, che ne definisce la composizione, l’organizzazione e il funzionamento. Esso elabora le basi decisionali per il Consiglio di Stato, lo coadiuva nelle funzioni di direzione e coordinamento ed esegue le sue decisioni. Esso è competente quando le circostanze lo esigono, per predisporre e coordinare, in collaborazione con le autorità locali, le necessarie misure d’urgenza e di assistenza e condurne l’attuazione. La sua attivazione è decisa dal Comandante della Polizia cantonale; in caso di impedimento di questo e in successione, dal suo sostituto o dall’ufficiale di picchetto della Polizia cantonale.</t>
+        </is>
+      </c>
+      <c r="T62" t="inlineStr">
+        <is>
+          <t>Competenza della Protezione Civile</t>
+        </is>
+      </c>
       <c r="U62" t="inlineStr"/>
       <c r="V62" t="inlineStr">
         <is>
-          <t>pag 10</t>
+          <t>Art. 10</t>
         </is>
       </c>
       <c r="W62" t="inlineStr"/>
       <c r="X62" t="inlineStr">
         <is>
-          <t>Il comando della protezione civile - Personale</t>
-        </is>
-      </c>
-      <c r="Y62" t="inlineStr">
-        <is>
-          <t>Ufficio Federale della Protezione della Popolazione</t>
-        </is>
-      </c>
+          <t>Legge sulla protezione della popolazione (del 26 febbraio 2007)</t>
+        </is>
+      </c>
+      <c r="Y62" t="inlineStr"/>
       <c r="Z62" t="inlineStr">
         <is>
-          <t>Confederazione Elvetica</t>
+          <t>Repubblica e Cantone Ticino</t>
         </is>
       </c>
       <c r="AA62" t="inlineStr">
         <is>
-          <t>https://www.babs.admin.ch/content/babs-internet/it/publikservice/downloads/unterlagen-ausbildung/_jcr_content/contentPar/accordion_1920886228/accordionItems/kommando_zivilschutz/accordionPar/downloadlist_copy/downloadItems/829_1459931125997.download/personal170191103it.pdf</t>
+          <t>https://m3.ti.ch/CAN/RLeggi/public/index.php/raccolta-leggi/legge/num/48</t>
         </is>
       </c>
       <c r="AB62" t="inlineStr"/>
@@ -6747,7 +6771,7 @@
       </c>
       <c r="AD62" t="inlineStr">
         <is>
-          <t>ITCH00019</t>
+          <t>ITCH00020</t>
         </is>
       </c>
       <c r="AE62" t="inlineStr">
@@ -6770,34 +6794,34 @@
         <v>3000062</v>
       </c>
       <c r="E63" t="n">
-        <v>4000002</v>
+        <v>4000001</v>
       </c>
       <c r="F63" t="n">
-        <v>5000001</v>
+        <v>5000032</v>
       </c>
       <c r="G63" t="n">
-        <v>6000049</v>
+        <v>6000001</v>
       </c>
       <c r="H63" t="n">
         <v>7000001</v>
       </c>
       <c r="I63" t="n">
-        <v>8000053</v>
+        <v>8000032</v>
       </c>
       <c r="J63" t="n">
         <v>9000003</v>
       </c>
       <c r="K63" t="n">
-        <v>10000042</v>
+        <v>10000032</v>
       </c>
       <c r="L63" t="n">
-        <v>11000053</v>
+        <v>11000032</v>
       </c>
       <c r="M63" t="n">
         <v>12000001</v>
       </c>
       <c r="N63" t="n">
-        <v>13000058</v>
+        <v>13000047</v>
       </c>
       <c r="O63" t="n">
         <v>14000062</v>
@@ -6807,50 +6831,34 @@
       </c>
       <c r="Q63" t="inlineStr">
         <is>
-          <t>Stato maggiore cantonale di condotta</t>
+          <t>Sistema d’allarme acqua</t>
         </is>
       </c>
       <c r="R63" t="inlineStr"/>
       <c r="S63" t="inlineStr">
         <is>
-          <t>Lo SMCC è l’organo cantonale di condotta del Consiglio di Stato, che ne definisce la composizione, l’organizzazione e il funzionamento. Esso elabora le basi decisionali per il Consiglio di Stato, lo coadiuva nelle funzioni di direzione e coordinamento ed esegue le sue decisioni. Esso è competente quando le circostanze lo esigono, per predisporre e coordinare, in collaborazione con le autorità locali, le necessarie misure d’urgenza e di assistenza e condurne l’attuazione. La sua attivazione è decisa dal Comandante della Polizia cantonale; in caso di impedimento di questo e in successione, dal suo sostituto o dall’ufficiale di picchetto della Polizia cantonale.</t>
-        </is>
-      </c>
-      <c r="T63" t="inlineStr">
-        <is>
-          <t>Competenza della Protezione Civile</t>
-        </is>
-      </c>
-      <c r="U63" t="inlineStr"/>
-      <c r="V63" t="inlineStr">
-        <is>
-          <t>Art. 10</t>
-        </is>
-      </c>
+          <t>Sistema di allertamento per eventi di tipo idrometeorologico.</t>
+        </is>
+      </c>
+      <c r="T63" t="inlineStr"/>
+      <c r="U63" t="inlineStr">
+        <is>
+          <t>Tommaso Sansone</t>
+        </is>
+      </c>
+      <c r="V63" t="inlineStr"/>
       <c r="W63" t="inlineStr"/>
-      <c r="X63" t="inlineStr">
-        <is>
-          <t>Legge sulla protezione della popolazione (del 26 febbraio 2007)</t>
-        </is>
-      </c>
+      <c r="X63" t="inlineStr"/>
       <c r="Y63" t="inlineStr"/>
-      <c r="Z63" t="inlineStr">
-        <is>
-          <t>Repubblica e Cantone Ticino</t>
-        </is>
-      </c>
-      <c r="AA63" t="inlineStr">
-        <is>
-          <t>https://m3.ti.ch/CAN/RLeggi/public/index.php/raccolta-leggi/legge/num/48</t>
-        </is>
-      </c>
+      <c r="Z63" t="inlineStr"/>
+      <c r="AA63" t="inlineStr"/>
       <c r="AB63" t="inlineStr"/>
       <c r="AC63" s="2" t="n">
-        <v>43767</v>
+        <v>43766</v>
       </c>
       <c r="AD63" t="inlineStr">
         <is>
-          <t>ITCH00020</t>
+          <t>ITCH00021</t>
         </is>
       </c>
       <c r="AE63" t="inlineStr">
@@ -6876,7 +6884,7 @@
         <v>4000001</v>
       </c>
       <c r="F64" t="n">
-        <v>5000032</v>
+        <v>5000001</v>
       </c>
       <c r="G64" t="n">
         <v>6000001</v>
@@ -6885,22 +6893,22 @@
         <v>7000001</v>
       </c>
       <c r="I64" t="n">
-        <v>8000032</v>
+        <v>8000063</v>
       </c>
       <c r="J64" t="n">
         <v>9000003</v>
       </c>
       <c r="K64" t="n">
-        <v>10000032</v>
+        <v>10000025</v>
       </c>
       <c r="L64" t="n">
-        <v>11000032</v>
+        <v>11000063</v>
       </c>
       <c r="M64" t="n">
         <v>12000001</v>
       </c>
       <c r="N64" t="n">
-        <v>13000048</v>
+        <v>13000040</v>
       </c>
       <c r="O64" t="n">
         <v>14000063</v>
@@ -6910,34 +6918,42 @@
       </c>
       <c r="Q64" t="inlineStr">
         <is>
-          <t>Sistema d’allarme acqua</t>
+          <t>Allarme acqua</t>
         </is>
       </c>
       <c r="R64" t="inlineStr"/>
       <c r="S64" t="inlineStr">
         <is>
-          <t>Sistema di allertamento per eventi di tipo idrometeorologico.</t>
+          <t>Il segnale d'allarme acqua viene emesso esclusivamente nelle regioni minacciate a valle di impianti d'accumulazione. Le sirene emettono dodici suoni continui e gravi in sequenze di 20 secondi e a intervalli di 10 secondi. L’allarme acqua esorta la popolazione ad abbandonare immediatamente la regione minacciata.</t>
         </is>
       </c>
       <c r="T64" t="inlineStr"/>
-      <c r="U64" t="inlineStr">
-        <is>
-          <t>Tommaso Sansone</t>
-        </is>
-      </c>
+      <c r="U64" t="inlineStr"/>
       <c r="V64" t="inlineStr"/>
       <c r="W64" t="inlineStr"/>
-      <c r="X64" t="inlineStr"/>
+      <c r="X64" t="inlineStr">
+        <is>
+          <t>Segnali di allarme in Svizzera</t>
+        </is>
+      </c>
       <c r="Y64" t="inlineStr"/>
-      <c r="Z64" t="inlineStr"/>
-      <c r="AA64" t="inlineStr"/>
+      <c r="Z64" t="inlineStr">
+        <is>
+          <t>Confederazione Elvetica</t>
+        </is>
+      </c>
+      <c r="AA64" t="inlineStr">
+        <is>
+          <t>https://www.ch.ch/it/allarme-sirene/</t>
+        </is>
+      </c>
       <c r="AB64" t="inlineStr"/>
       <c r="AC64" s="2" t="n">
-        <v>43766</v>
+        <v>43767</v>
       </c>
       <c r="AD64" t="inlineStr">
         <is>
-          <t>ITCH00021</t>
+          <t>ITCH00022</t>
         </is>
       </c>
       <c r="AE64" t="inlineStr">
@@ -6960,34 +6976,34 @@
         <v>3000064</v>
       </c>
       <c r="E65" t="n">
-        <v>4000001</v>
+        <v>4000002</v>
       </c>
       <c r="F65" t="n">
         <v>5000001</v>
       </c>
       <c r="G65" t="n">
-        <v>6000001</v>
+        <v>6000064</v>
       </c>
       <c r="H65" t="n">
         <v>7000001</v>
       </c>
       <c r="I65" t="n">
-        <v>8000064</v>
+        <v>8000053</v>
       </c>
       <c r="J65" t="n">
         <v>9000003</v>
       </c>
       <c r="K65" t="n">
-        <v>10000026</v>
+        <v>10000041</v>
       </c>
       <c r="L65" t="n">
-        <v>11000064</v>
+        <v>11000053</v>
       </c>
       <c r="M65" t="n">
         <v>12000001</v>
       </c>
       <c r="N65" t="n">
-        <v>13000058</v>
+        <v>13000040</v>
       </c>
       <c r="O65" t="n">
         <v>14000064</v>
@@ -6997,33 +7013,41 @@
       </c>
       <c r="Q65" t="inlineStr">
         <is>
-          <t>Allarme acqua</t>
+          <t>Stato maggiore regionale di condotta</t>
         </is>
       </c>
       <c r="R65" t="inlineStr"/>
       <c r="S65" t="inlineStr">
         <is>
-          <t>Il segnale d'allarme acqua viene emesso esclusivamente nelle regioni minacciate a valle di impianti d'accumulazione. Le sirene emettono dodici suoni continui e gravi in sequenze di 20 secondi e a intervalli di 10 secondi. L’allarme acqua esorta la popolazione ad abbandonare immediatamente la regione minacciata.</t>
-        </is>
-      </c>
-      <c r="T65" t="inlineStr"/>
+          <t>Lo SMRC è un organo di condotta che permette la coordinazione di più SMEPI attivi nella medesima regione. La costituzione di uno SMRC può essere ordinata o autorizzata dal Comandante dello SMCC. Esso è di norma condotto da un ufficiale della Polizia cantonale.</t>
+        </is>
+      </c>
+      <c r="T65" t="inlineStr">
+        <is>
+          <t>Competenza della Protezione Civile</t>
+        </is>
+      </c>
       <c r="U65" t="inlineStr"/>
-      <c r="V65" t="inlineStr"/>
+      <c r="V65" t="inlineStr">
+        <is>
+          <t>Art. 11</t>
+        </is>
+      </c>
       <c r="W65" t="inlineStr"/>
       <c r="X65" t="inlineStr">
         <is>
-          <t>Segnali di allarme in Svizzera</t>
+          <t>Legge sulla protezione della popolazione (del 26 febbraio 2007)</t>
         </is>
       </c>
       <c r="Y65" t="inlineStr"/>
       <c r="Z65" t="inlineStr">
         <is>
-          <t>Confederazione Elvetica</t>
+          <t>Repubblica e Cantone Ticino</t>
         </is>
       </c>
       <c r="AA65" t="inlineStr">
         <is>
-          <t>https://www.ch.ch/it/allarme-sirene/</t>
+          <t>https://m3.ti.ch/CAN/RLeggi/public/index.php/raccolta-leggi/legge/num/48</t>
         </is>
       </c>
       <c r="AB65" t="inlineStr"/>
@@ -7032,7 +7056,7 @@
       </c>
       <c r="AD65" t="inlineStr">
         <is>
-          <t>ITCH00022</t>
+          <t>ITCH00023</t>
         </is>
       </c>
       <c r="AE65" t="inlineStr">
@@ -7055,7 +7079,7 @@
         <v>3000065</v>
       </c>
       <c r="E66" t="n">
-        <v>4000002</v>
+        <v>4000001</v>
       </c>
       <c r="F66" t="n">
         <v>5000001</v>
@@ -7073,7 +7097,7 @@
         <v>9000003</v>
       </c>
       <c r="K66" t="n">
-        <v>10000042</v>
+        <v>10000041</v>
       </c>
       <c r="L66" t="n">
         <v>11000053</v>
@@ -7082,7 +7106,7 @@
         <v>12000001</v>
       </c>
       <c r="N66" t="n">
-        <v>13000058</v>
+        <v>13000040</v>
       </c>
       <c r="O66" t="n">
         <v>14000065</v>
@@ -7092,24 +7116,20 @@
       </c>
       <c r="Q66" t="inlineStr">
         <is>
-          <t>Stato maggiore regionale di condotta</t>
+          <t>Stato maggiore enti di primo intervento</t>
         </is>
       </c>
       <c r="R66" t="inlineStr"/>
       <c r="S66" t="inlineStr">
         <is>
-          <t>Lo SMRC è un organo di condotta che permette la coordinazione di più SMEPI attivi nella medesima regione. La costituzione di uno SMRC può essere ordinata o autorizzata dal Comandante dello SMCC. Esso è di norma condotto da un ufficiale della Polizia cantonale.</t>
-        </is>
-      </c>
-      <c r="T66" t="inlineStr">
-        <is>
-          <t>Competenza della Protezione Civile</t>
-        </is>
-      </c>
+          <t>Lo SMEPI coordina l’intervento dei primi enti mobilitati, di regola polizia, pompieri e servizi d’autoambulanza. Esso è condotto, di principio, dalla Polizia cantonale.</t>
+        </is>
+      </c>
+      <c r="T66" t="inlineStr"/>
       <c r="U66" t="inlineStr"/>
       <c r="V66" t="inlineStr">
         <is>
-          <t>Art. 11</t>
+          <t>Art. 12</t>
         </is>
       </c>
       <c r="W66" t="inlineStr"/>
@@ -7135,7 +7155,7 @@
       </c>
       <c r="AD66" t="inlineStr">
         <is>
-          <t>ITCH00023</t>
+          <t>ITCH00024</t>
         </is>
       </c>
       <c r="AE66" t="inlineStr">
@@ -7158,7 +7178,7 @@
         <v>3000066</v>
       </c>
       <c r="E67" t="n">
-        <v>4000001</v>
+        <v>4000002</v>
       </c>
       <c r="F67" t="n">
         <v>5000001</v>
@@ -7170,22 +7190,22 @@
         <v>7000001</v>
       </c>
       <c r="I67" t="n">
-        <v>8000053</v>
+        <v>8000066</v>
       </c>
       <c r="J67" t="n">
-        <v>9000003</v>
+        <v>9000066</v>
       </c>
       <c r="K67" t="n">
-        <v>10000042</v>
+        <v>10000041</v>
       </c>
       <c r="L67" t="n">
-        <v>11000053</v>
+        <v>11000066</v>
       </c>
       <c r="M67" t="n">
-        <v>12000001</v>
+        <v>12000066</v>
       </c>
       <c r="N67" t="n">
-        <v>13000058</v>
+        <v>13000066</v>
       </c>
       <c r="O67" t="n">
         <v>14000066</v>
@@ -7195,29 +7215,39 @@
       </c>
       <c r="Q67" t="inlineStr">
         <is>
-          <t>Stato maggiore enti di primo intervento</t>
+          <t>Protezione della popolazione</t>
         </is>
       </c>
       <c r="R67" t="inlineStr"/>
       <c r="S67" t="inlineStr">
         <is>
-          <t>Lo SMEPI coordina l’intervento dei primi enti mobilitati, di regola polizia, pompieri e servizi d’autoambulanza. Esso è condotto, di principio, dalla Polizia cantonale.</t>
-        </is>
-      </c>
-      <c r="T67" t="inlineStr"/>
+          <t>Il servizio della protezione della popolazione si occupa prevalentemente dei preparativi per i casi di emergenza e di catastrofe.
+Assicura la collaborazione con i servizi delle Amministrazioni: federale, cantonale e comunali direttamente collegate con i temi trattati dal servizio e si occupa della coordinazione fra i partner del concetto “protezione della popolazione” (polizia cantonale, Federazione cantonale ticinese dei Corpi Pompieri, Federazione cantonale ticinese dei Servizi autoambulanze, organizzazioni regionali di protezione civile, servizi tecnici cantonali, servizi dello Stato Maggiore cantonale di catastrofe, ecc…).
+Per il tramite di esercitazioni teoriche e pratiche, approfondisce con le istanze militari, la collaborazione civile-militare.</t>
+        </is>
+      </c>
+      <c r="T67" t="inlineStr">
+        <is>
+          <t>Competenza della Protezione Civile</t>
+        </is>
+      </c>
       <c r="U67" t="inlineStr"/>
       <c r="V67" t="inlineStr">
         <is>
-          <t>Art. 12</t>
+          <t>Presentazione</t>
         </is>
       </c>
       <c r="W67" t="inlineStr"/>
       <c r="X67" t="inlineStr">
         <is>
-          <t>Legge sulla protezione della popolazione (del 26 febbraio 2007)</t>
-        </is>
-      </c>
-      <c r="Y67" t="inlineStr"/>
+          <t>Servizio della protezione della popolazione</t>
+        </is>
+      </c>
+      <c r="Y67" t="inlineStr">
+        <is>
+          <t>Repubblica e Cantone Ticino</t>
+        </is>
+      </c>
       <c r="Z67" t="inlineStr">
         <is>
           <t>Repubblica e Cantone Ticino</t>
@@ -7225,16 +7255,21 @@
       </c>
       <c r="AA67" t="inlineStr">
         <is>
-          <t>https://m3.ti.ch/CAN/RLeggi/public/index.php/raccolta-leggi/legge/num/48</t>
-        </is>
-      </c>
-      <c r="AB67" t="inlineStr"/>
+          <t>https://www4.ti.ch/di/smpp/chi-siamo/servizio-della-protezione-della-popolazione/</t>
+        </is>
+      </c>
+      <c r="AB67" t="inlineStr">
+        <is>
+          <t>Il significato italiano di protezione civile coincide a livello di strutture con io significato svizzero di protezione della popolazione.
+Definizioni riorganizzate da Tommaso Sansone, Politecnico di Milano.</t>
+        </is>
+      </c>
       <c r="AC67" s="2" t="n">
-        <v>43767</v>
+        <v>43815</v>
       </c>
       <c r="AD67" t="inlineStr">
         <is>
-          <t>ITCH00024</t>
+          <t>ITCH00025</t>
         </is>
       </c>
       <c r="AE67" t="inlineStr">
@@ -7248,93 +7283,95 @@
         <v>66</v>
       </c>
       <c r="B68" t="n">
-        <v>1000068</v>
+        <v>1000041</v>
       </c>
       <c r="C68" t="n">
         <v>2000001</v>
       </c>
       <c r="D68" t="n">
-        <v>3000068</v>
+        <v>3000042</v>
       </c>
       <c r="E68" t="n">
-        <v>4000002</v>
+        <v>4000019</v>
       </c>
       <c r="F68" t="n">
         <v>5000001</v>
       </c>
       <c r="G68" t="n">
-        <v>6000068</v>
+        <v>6000002</v>
       </c>
       <c r="H68" t="n">
-        <v>7000001</v>
+        <v>7000009</v>
       </c>
       <c r="I68" t="n">
-        <v>8000068</v>
+        <v>8000019</v>
       </c>
       <c r="J68" t="n">
-        <v>9000068</v>
+        <v>9000019</v>
       </c>
       <c r="K68" t="n">
-        <v>10000042</v>
+        <v>10000019</v>
       </c>
       <c r="L68" t="n">
-        <v>11000068</v>
+        <v>11000019</v>
       </c>
       <c r="M68" t="n">
-        <v>12000067</v>
+        <v>12000066</v>
       </c>
       <c r="N68" t="n">
-        <v>13000067</v>
+        <v>13000066</v>
       </c>
       <c r="O68" t="n">
-        <v>14000067</v>
+        <v>14000066</v>
       </c>
       <c r="P68" t="n">
         <v>15000001</v>
       </c>
       <c r="Q68" t="inlineStr">
         <is>
-          <t>Protezione della popolazione</t>
+          <t>Protezione civile</t>
         </is>
       </c>
       <c r="R68" t="inlineStr"/>
       <c r="S68" t="inlineStr">
         <is>
-          <t>Il servizio della protezione della popolazione si occupa prevalentemente dei preparativi per i casi di emergenza e di catastrofe.
-Assicura la collaborazione con i servizi delle Amministrazioni: federale, cantonale e comunali direttamente collegate con i temi trattati dal servizio e si occupa della coordinazione fra i partner del concetto “protezione della popolazione” (polizia cantonale, Federazione cantonale ticinese dei Corpi Pompieri, Federazione cantonale ticinese dei Servizi autoambulanze, organizzazioni regionali di protezione civile, servizi tecnici cantonali, servizi dello Stato Maggiore cantonale di catastrofe, ecc…).
-Per il tramite di esercitazioni teoriche e pratiche, approfondisce con le istanze militari, la collaborazione civile-militare.</t>
+          <t>Il Servizio nazionale della protezione civile, di seguito Servizio nazionale, definito di pubblica utilita', e' il sistema che esercita la funzione di protezione civile costituita dall'insieme delle competenze e delle attivita' volte a tutelare la vita, l'integrita' fisica, i beni, gli insediamenti, gli animali e l'ambiente dai danni o dal pericolo di danni derivanti da eventi calamitosi di origine naturale o derivanti dall'attivita' dell'uomo.</t>
         </is>
       </c>
       <c r="T68" t="inlineStr">
         <is>
-          <t>Competenza della Protezione Civile</t>
+          <t>Competenza di protezione civile</t>
         </is>
       </c>
       <c r="U68" t="inlineStr"/>
       <c r="V68" t="inlineStr">
         <is>
-          <t>Presentazione</t>
-        </is>
-      </c>
-      <c r="W68" t="inlineStr"/>
+          <t>Art 1, comma 1</t>
+        </is>
+      </c>
+      <c r="W68" t="inlineStr">
+        <is>
+          <t>https://www.gazzettaufficiale.it/atto/serie_generale/caricaArticolo?art.progressivo=0&amp;art.idArticolo=1&amp;art.versione=1&amp;art.codiceRedazionale=18G00011&amp;art.dataPubblicazioneGazzetta=2018-01-22&amp;art.idGruppo=1&amp;art.idSottoArticolo1=10&amp;art.idSottoArticolo=1&amp;art.flagTipoArticolo=0</t>
+        </is>
+      </c>
       <c r="X68" t="inlineStr">
         <is>
-          <t>Servizio della protezione della popolazione</t>
+          <t>Decreto Legislativo 2 Gennaio 2018, N. 1, Codice Della Protezione Civile. (18G00011)</t>
         </is>
       </c>
       <c r="Y68" t="inlineStr">
         <is>
-          <t>Repubblica e Cantone Ticino</t>
+          <t>Presidenza Del Consiglio Dei Ministri</t>
         </is>
       </c>
       <c r="Z68" t="inlineStr">
         <is>
-          <t>Repubblica e Cantone Ticino</t>
+          <t>Gazzetta Ufficiale</t>
         </is>
       </c>
       <c r="AA68" t="inlineStr">
         <is>
-          <t>https://www4.ti.ch/di/smpp/chi-siamo/servizio-della-protezione-della-popolazione/</t>
+          <t>http://www.gazzettaufficiale.it/eli/id/2018/1/22/18G00011/sg</t>
         </is>
       </c>
       <c r="AB68" t="inlineStr">
@@ -7362,109 +7399,88 @@
         <v>67</v>
       </c>
       <c r="B69" t="n">
-        <v>1000042</v>
+        <v>1000068</v>
       </c>
       <c r="C69" t="n">
         <v>2000001</v>
       </c>
       <c r="D69" t="n">
-        <v>3000043</v>
+        <v>3000068</v>
       </c>
       <c r="E69" t="n">
-        <v>4000019</v>
+        <v>4000001</v>
       </c>
       <c r="F69" t="n">
         <v>5000001</v>
       </c>
       <c r="G69" t="n">
-        <v>6000002</v>
+        <v>6000001</v>
       </c>
       <c r="H69" t="n">
-        <v>7000009</v>
+        <v>7000001</v>
       </c>
       <c r="I69" t="n">
-        <v>8000019</v>
+        <v>8000068</v>
       </c>
       <c r="J69" t="n">
-        <v>9000019</v>
+        <v>9000003</v>
       </c>
       <c r="K69" t="n">
-        <v>10000019</v>
+        <v>10000003</v>
       </c>
       <c r="L69" t="n">
-        <v>11000019</v>
+        <v>11000045</v>
       </c>
       <c r="M69" t="n">
-        <v>12000067</v>
+        <v>12000001</v>
       </c>
       <c r="N69" t="n">
-        <v>13000067</v>
+        <v>13000068</v>
       </c>
       <c r="O69" t="n">
-        <v>14000067</v>
+        <v>14000068</v>
       </c>
       <c r="P69" t="n">
         <v>15000001</v>
       </c>
       <c r="Q69" t="inlineStr">
         <is>
-          <t>Protezione civile</t>
+          <t>Dipartimento della protezione civile</t>
         </is>
       </c>
       <c r="R69" t="inlineStr"/>
       <c r="S69" t="inlineStr">
         <is>
-          <t>Il Servizio nazionale della protezione civile, di seguito Servizio nazionale, definito di pubblica utilita', e' il sistema che esercita la funzione di protezione civile costituita dall'insieme delle competenze e delle attivita' volte a tutelare la vita, l'integrita' fisica, i beni, gli insediamenti, gli animali e l'ambiente dai danni o dal pericolo di danni derivanti da eventi calamitosi di origine naturale o derivanti dall'attivita' dell'uomo.</t>
-        </is>
-      </c>
-      <c r="T69" t="inlineStr">
-        <is>
-          <t>Competenza di protezione civile</t>
-        </is>
-      </c>
+          <t>Il Dipartimento della protezione civile è una struttura della Presidenza del Consiglio dei Ministri. Il Dipartimento, operando in stretto raccordo con le Regioni e le Province autonome, si occupa di tutte le attività volte alla previsione e alla prevenzione dei rischi, al soccorso e all’assistenza delle popolazioni colpite da calamità, al contrasto e al superamento dell’emergenza.</t>
+        </is>
+      </c>
+      <c r="T69" t="inlineStr"/>
       <c r="U69" t="inlineStr"/>
-      <c r="V69" t="inlineStr">
-        <is>
-          <t>Art 1, comma 1</t>
-        </is>
-      </c>
-      <c r="W69" t="inlineStr">
-        <is>
-          <t>https://www.gazzettaufficiale.it/atto/serie_generale/caricaArticolo?art.progressivo=0&amp;art.idArticolo=1&amp;art.versione=1&amp;art.codiceRedazionale=18G00011&amp;art.dataPubblicazioneGazzetta=2018-01-22&amp;art.idGruppo=1&amp;art.idSottoArticolo1=10&amp;art.idSottoArticolo=1&amp;art.flagTipoArticolo=0</t>
-        </is>
-      </c>
+      <c r="V69" t="inlineStr"/>
+      <c r="W69" t="inlineStr"/>
       <c r="X69" t="inlineStr">
         <is>
-          <t>Decreto Legislativo 2 Gennaio 2018, N. 1, Codice Della Protezione Civile. (18G00011)</t>
-        </is>
-      </c>
-      <c r="Y69" t="inlineStr">
-        <is>
-          <t>Presidenza Del Consiglio Dei Ministri</t>
-        </is>
-      </c>
+          <t>Dipartimento</t>
+        </is>
+      </c>
+      <c r="Y69" t="inlineStr"/>
       <c r="Z69" t="inlineStr">
         <is>
-          <t>Gazzetta Ufficiale</t>
+          <t>Dipartimento della protezione civile</t>
         </is>
       </c>
       <c r="AA69" t="inlineStr">
         <is>
-          <t>http://www.gazzettaufficiale.it/eli/id/2018/1/22/18G00011/sg</t>
-        </is>
-      </c>
-      <c r="AB69" t="inlineStr">
-        <is>
-          <t>Il significato italiano di protezione civile coincide a livello di strutture con io significato svizzero di protezione della popolazione.
-Definizioni riorganizzate da Tommaso Sansone, Politecnico di Milano.</t>
-        </is>
-      </c>
+          <t>http://www.protezionecivile.gov.it/dipartimento</t>
+        </is>
+      </c>
+      <c r="AB69" t="inlineStr"/>
       <c r="AC69" s="2" t="n">
-        <v>43815</v>
+        <v>43817</v>
       </c>
       <c r="AD69" t="inlineStr">
         <is>
-          <t>ITCH00025</t>
+          <t>ITCH00026</t>
         </is>
       </c>
       <c r="AE69" t="inlineStr">
@@ -7478,7 +7494,7 @@
         <v>68</v>
       </c>
       <c r="B70" t="n">
-        <v>1000069</v>
+        <v>1000042</v>
       </c>
       <c r="C70" t="n">
         <v>2000001</v>
@@ -7487,31 +7503,31 @@
         <v>3000069</v>
       </c>
       <c r="E70" t="n">
-        <v>4000001</v>
+        <v>4000046</v>
       </c>
       <c r="F70" t="n">
-        <v>5000001</v>
+        <v>5000032</v>
       </c>
       <c r="G70" t="n">
-        <v>6000001</v>
+        <v>6000069</v>
       </c>
       <c r="H70" t="n">
         <v>7000001</v>
       </c>
       <c r="I70" t="n">
-        <v>8000046</v>
+        <v>8000069</v>
       </c>
       <c r="J70" t="n">
-        <v>9000003</v>
+        <v>9000069</v>
       </c>
       <c r="K70" t="n">
-        <v>10000003</v>
+        <v>10000032</v>
       </c>
       <c r="L70" t="n">
-        <v>11000069</v>
+        <v>11000032</v>
       </c>
       <c r="M70" t="n">
-        <v>12000001</v>
+        <v>12000069</v>
       </c>
       <c r="N70" t="n">
         <v>13000069</v>
@@ -7524,42 +7540,54 @@
       </c>
       <c r="Q70" t="inlineStr">
         <is>
-          <t>Dipartimento della protezione civile</t>
+          <t>Legge federale sulla protezione della popolazione e sulla protezione civile</t>
         </is>
       </c>
       <c r="R70" t="inlineStr"/>
       <c r="S70" t="inlineStr">
         <is>
-          <t>Il Dipartimento della protezione civile è una struttura della Presidenza del Consiglio dei Ministri. Il Dipartimento, operando in stretto raccordo con le Regioni e le Province autonome, si occupa di tutte le attività volte alla previsione e alla prevenzione dei rischi, al soccorso e all’assistenza delle popolazioni colpite da calamità, al contrasto e al superamento dell’emergenza.</t>
-        </is>
-      </c>
-      <c r="T70" t="inlineStr"/>
-      <c r="U70" t="inlineStr"/>
-      <c r="V70" t="inlineStr"/>
+          <t>La legge federale sulla protezione della popolazione e sulla protezione civile (LPPC) del 4 ottobre 2002 può essere considerata come la più importante legge dello stato svizzero in materia di protezione della protezione della popolazione, che costituisce quadro normativo di riferimento per altre leggi federali e cantonali in materia di protezione della popolazione. Essa disciplina principalmente due ambiti: - la collaborazione tra Confederazione e Cantoni nella protezione della popolazione. - il ruolo e i doveri degli organi e dei corpi della protezione della popolazione.</t>
+        </is>
+      </c>
+      <c r="T70" t="inlineStr">
+        <is>
+          <t>Normativa</t>
+        </is>
+      </c>
+      <c r="U70" t="inlineStr">
+        <is>
+          <t>Tommaso Sansone</t>
+        </is>
+      </c>
+      <c r="V70" t="inlineStr">
+        <is>
+          <t>Normativa nazionale: Legge federale sulla protezione della popolazione e sulla protezione civile (LPPC) del 4 ottobre 2002</t>
+        </is>
+      </c>
       <c r="W70" t="inlineStr"/>
       <c r="X70" t="inlineStr">
         <is>
-          <t>Dipartimento</t>
-        </is>
-      </c>
-      <c r="Y70" t="inlineStr"/>
-      <c r="Z70" t="inlineStr">
-        <is>
-          <t>Dipartimento della protezione civile</t>
-        </is>
-      </c>
-      <c r="AA70" t="inlineStr">
-        <is>
-          <t>http://www.protezionecivile.gov.it/dipartimento</t>
-        </is>
-      </c>
-      <c r="AB70" t="inlineStr"/>
+          <t>-- documento confronto normativa -- wp 3.2 gestisco -- da completare</t>
+        </is>
+      </c>
+      <c r="Y70" t="inlineStr">
+        <is>
+          <t>Tommaso Sansone</t>
+        </is>
+      </c>
+      <c r="Z70" t="inlineStr"/>
+      <c r="AA70" t="inlineStr"/>
+      <c r="AB70" t="inlineStr">
+        <is>
+          <t>definizione lato italiano, oggetto lato svizzero</t>
+        </is>
+      </c>
       <c r="AC70" s="2" t="n">
-        <v>43817</v>
+        <v>43780</v>
       </c>
       <c r="AD70" t="inlineStr">
         <is>
-          <t>ITCH00026</t>
+          <t>ITCH00027</t>
         </is>
       </c>
       <c r="AE70" t="inlineStr">
@@ -7573,31 +7601,31 @@
         <v>69</v>
       </c>
       <c r="B71" t="n">
-        <v>1000038</v>
+        <v>1000042</v>
       </c>
       <c r="C71" t="n">
         <v>2000001</v>
       </c>
       <c r="D71" t="n">
-        <v>3000071</v>
+        <v>3000070</v>
       </c>
       <c r="E71" t="n">
-        <v>4000047</v>
+        <v>4000001</v>
       </c>
       <c r="F71" t="n">
-        <v>5000032</v>
+        <v>5000001</v>
       </c>
       <c r="G71" t="n">
-        <v>6000071</v>
+        <v>6000001</v>
       </c>
       <c r="H71" t="n">
         <v>7000001</v>
       </c>
       <c r="I71" t="n">
-        <v>8000071</v>
+        <v>8000032</v>
       </c>
       <c r="J71" t="n">
-        <v>9000071</v>
+        <v>9000003</v>
       </c>
       <c r="K71" t="n">
         <v>10000032</v>
@@ -7606,50 +7634,30 @@
         <v>11000032</v>
       </c>
       <c r="M71" t="n">
-        <v>12000070</v>
+        <v>12000069</v>
       </c>
       <c r="N71" t="n">
-        <v>13000070</v>
+        <v>13000069</v>
       </c>
       <c r="O71" t="n">
-        <v>14000070</v>
+        <v>14000069</v>
       </c>
       <c r="P71" t="n">
         <v>15000001</v>
       </c>
-      <c r="Q71" t="inlineStr"/>
+      <c r="Q71" t="inlineStr">
+        <is>
+          <t>Legge federale sulla protezione della popolazione e sulla protezione civile</t>
+        </is>
+      </c>
       <c r="R71" t="inlineStr"/>
-      <c r="S71" t="inlineStr">
-        <is>
-          <t>La legge federale sulla protezione della popolazione e sulla protezione civile (LPPC) del 4 ottobre 2002 può essere considerata come la più importante legge dello stato svizzero in materia di protezione della protezione della popolazione, che costituisce quadro normativo di riferimento per altre leggi federali e cantonali in materia di protezione della popolazione. Essa disciplina principalmente due ambiti: - la collaborazione tra Confederazione e Cantoni nella protezione della popolazione. - il ruolo e i doveri degli organi e dei corpi della protezione della popolazione.</t>
-        </is>
-      </c>
-      <c r="T71" t="inlineStr">
-        <is>
-          <t>Normativa</t>
-        </is>
-      </c>
-      <c r="U71" t="inlineStr">
-        <is>
-          <t>Tommaso Sansone</t>
-        </is>
-      </c>
-      <c r="V71" t="inlineStr">
-        <is>
-          <t>Normativa nazionale: Legge federale sulla protezione della popolazione e sulla protezione civile (LPPC) del 4 ottobre 2002</t>
-        </is>
-      </c>
+      <c r="S71" t="inlineStr"/>
+      <c r="T71" t="inlineStr"/>
+      <c r="U71" t="inlineStr"/>
+      <c r="V71" t="inlineStr"/>
       <c r="W71" t="inlineStr"/>
-      <c r="X71" t="inlineStr">
-        <is>
-          <t>-- documento confronto normativa -- wp 3.2 gestisco -- da completare</t>
-        </is>
-      </c>
-      <c r="Y71" t="inlineStr">
-        <is>
-          <t>Tommaso Sansone</t>
-        </is>
-      </c>
+      <c r="X71" t="inlineStr"/>
+      <c r="Y71" t="inlineStr"/>
       <c r="Z71" t="inlineStr"/>
       <c r="AA71" t="inlineStr"/>
       <c r="AB71" t="inlineStr">
@@ -7676,22 +7684,22 @@
         <v>70</v>
       </c>
       <c r="B72" t="n">
-        <v>1000070</v>
+        <v>1000071</v>
       </c>
       <c r="C72" t="n">
         <v>2000001</v>
       </c>
       <c r="D72" t="n">
-        <v>3000070</v>
+        <v>3000071</v>
       </c>
       <c r="E72" t="n">
-        <v>4000001</v>
+        <v>4000002</v>
       </c>
       <c r="F72" t="n">
         <v>5000001</v>
       </c>
       <c r="G72" t="n">
-        <v>6000001</v>
+        <v>6000071</v>
       </c>
       <c r="H72" t="n">
         <v>7000001</v>
@@ -7703,49 +7711,65 @@
         <v>9000003</v>
       </c>
       <c r="K72" t="n">
-        <v>10000032</v>
+        <v>10000003</v>
       </c>
       <c r="L72" t="n">
-        <v>11000032</v>
+        <v>11000035</v>
       </c>
       <c r="M72" t="n">
-        <v>12000070</v>
+        <v>12000001</v>
       </c>
       <c r="N72" t="n">
-        <v>13000070</v>
+        <v>13000040</v>
       </c>
       <c r="O72" t="n">
-        <v>14000070</v>
+        <v>14000071</v>
       </c>
       <c r="P72" t="n">
         <v>15000001</v>
       </c>
       <c r="Q72" t="inlineStr">
         <is>
-          <t>Legge federale sulla protezione della popolazione e sulla protezione civile</t>
+          <t>Volontario di protezione civile</t>
         </is>
       </c>
       <c r="R72" t="inlineStr"/>
-      <c r="S72" t="inlineStr"/>
-      <c r="T72" t="inlineStr"/>
+      <c r="S72" t="inlineStr">
+        <is>
+          <t>Il decreto legislativo n. 1 del 2018, Codice della Protezioone Civile, include il volontariato organizzato di protezione civile iscritto nell'elenco nazionale del volontariato di protezione civile tra le strutture operative del Servizio nazionale. Il volontariato si integra con gli altri livelli territoriali di intervento previsti nell'organizzazione del sistema nazionale della protezione civile, in base al principio della sussidiarietà verticale. È inoltre attore del sistema e del proprio territorio: protegge la comunità in collaborazione con le istituzioni, in base al principio della sussidiarietà orizzontale.</t>
+        </is>
+      </c>
+      <c r="T72" t="inlineStr">
+        <is>
+          <t>Competenza della Protezione Civile</t>
+        </is>
+      </c>
       <c r="U72" t="inlineStr"/>
-      <c r="V72" t="inlineStr"/>
+      <c r="V72" t="inlineStr">
+        <is>
+          <t>Home &gt; Servizio Nazionale &gt; Strutture operative &gt; Volontariato</t>
+        </is>
+      </c>
       <c r="W72" t="inlineStr"/>
       <c r="X72" t="inlineStr"/>
       <c r="Y72" t="inlineStr"/>
-      <c r="Z72" t="inlineStr"/>
-      <c r="AA72" t="inlineStr"/>
-      <c r="AB72" t="inlineStr">
-        <is>
-          <t>definizione lato italiano, oggetto lato svizzero</t>
-        </is>
-      </c>
+      <c r="Z72" t="inlineStr">
+        <is>
+          <t>Dipartimento della protezione civile</t>
+        </is>
+      </c>
+      <c r="AA72" t="inlineStr">
+        <is>
+          <t>http://www.protezionecivile.gov.it/servizio-nazionale/strutture-operative/volontariato</t>
+        </is>
+      </c>
+      <c r="AB72" t="inlineStr"/>
       <c r="AC72" s="2" t="n">
-        <v>43780</v>
+        <v>43767</v>
       </c>
       <c r="AD72" t="inlineStr">
         <is>
-          <t>ITCH00027</t>
+          <t>ITCH00028</t>
         </is>
       </c>
       <c r="AE72" t="inlineStr">
@@ -7759,7 +7783,7 @@
         <v>71</v>
       </c>
       <c r="B73" t="n">
-        <v>1000072</v>
+        <v>1000071</v>
       </c>
       <c r="C73" t="n">
         <v>2000001</v>
@@ -7771,34 +7795,34 @@
         <v>4000002</v>
       </c>
       <c r="F73" t="n">
-        <v>5000001</v>
+        <v>5000072</v>
       </c>
       <c r="G73" t="n">
-        <v>6000072</v>
+        <v>6000069</v>
       </c>
       <c r="H73" t="n">
         <v>7000001</v>
       </c>
       <c r="I73" t="n">
-        <v>8000032</v>
+        <v>8000069</v>
       </c>
       <c r="J73" t="n">
-        <v>9000003</v>
+        <v>9000072</v>
       </c>
       <c r="K73" t="n">
-        <v>10000003</v>
+        <v>10000032</v>
       </c>
       <c r="L73" t="n">
-        <v>11000034</v>
+        <v>11000047</v>
       </c>
       <c r="M73" t="n">
         <v>12000001</v>
       </c>
       <c r="N73" t="n">
-        <v>13000058</v>
+        <v>13000040</v>
       </c>
       <c r="O73" t="n">
-        <v>14000072</v>
+        <v>14000071</v>
       </c>
       <c r="P73" t="n">
         <v>15000001</v>
@@ -7811,7 +7835,8 @@
       <c r="R73" t="inlineStr"/>
       <c r="S73" t="inlineStr">
         <is>
-          <t>Il decreto legislativo n. 1 del 2018, Codice della Protezioone Civile, include il volontariato organizzato di protezione civile iscritto nell'elenco nazionale del volontariato di protezione civile tra le strutture operative del Servizio nazionale. Il volontariato si integra con gli altri livelli territoriali di intervento previsti nell'organizzazione del sistema nazionale della protezione civile, in base al principio della sussidiarietà verticale. È inoltre attore del sistema e del proprio territorio: protegge la comunità in collaborazione con le istituzioni, in base al principio della sussidiarietà orizzontale.</t>
+          <t>La legge LPPC 2002 stabilisce che possono prestare volontariamente servizio di protezione civile: a. gli uomini prosciolti dall’obbligo di prestare servizio nella protezione civile; b. gli uomini soggetti all’obbligo militare prosciolti dall’obbligo di prestare servizio militare o civile; c. gli uomini prosciolti dall’obbligo di prestare servizio militare o civile; d. le cittadine svizzere, a partire dall’anno in cui compiono i 20 anni; e. gli stranieri domiciliati in Svizzera, a partire dall’anno in cui compiono i 20 anni. Bisogna porre attenzione al fatto che secondo la stessa legge, l’unica differenza tra un milite e un volontario (entrambi di protezione civile) è il fatto che i volontari sono prosciolti dall’obbligo di prestare servizio su domanda. Infatti, per il resto, militi e volontari hanno gli stessi diritti e doveri. 
+I diritti dei militi sono essenzialmente quattro: soldo e vitto, alloggio, trasporto gratuiti, cui si aggiungono alcune agevolazioni fiscali e indennità.</t>
         </is>
       </c>
       <c r="T73" t="inlineStr">
@@ -7819,23 +7844,31 @@
           <t>Competenza della Protezione Civile</t>
         </is>
       </c>
-      <c r="U73" t="inlineStr"/>
+      <c r="U73" t="inlineStr">
+        <is>
+          <t>Tommaso sansone</t>
+        </is>
+      </c>
       <c r="V73" t="inlineStr">
         <is>
-          <t>Home &gt; Servizio Nazionale &gt; Strutture operative &gt; Volontariato</t>
+          <t>Normativa nazionale: Legge federale sulla protezione della popolazione e sulla protezione civile (LPPC) del 4 ottobre 2002</t>
         </is>
       </c>
       <c r="W73" t="inlineStr"/>
-      <c r="X73" t="inlineStr"/>
-      <c r="Y73" t="inlineStr"/>
-      <c r="Z73" t="inlineStr">
-        <is>
-          <t>Dipartimento della protezione civile</t>
-        </is>
-      </c>
+      <c r="X73" t="inlineStr">
+        <is>
+          <t>-- documento confronto normativa -- wp 3.2 gestisco -- da completare</t>
+        </is>
+      </c>
+      <c r="Y73" t="inlineStr">
+        <is>
+          <t>Tommaso sansone</t>
+        </is>
+      </c>
+      <c r="Z73" t="inlineStr"/>
       <c r="AA73" t="inlineStr">
         <is>
-          <t>http://www.protezionecivile.gov.it/servizio-nazionale/strutture-operative/volontariato</t>
+          <t>https://www.admin.ch/opc/it/classified-compilation/20011872/201701010000/520.1.pdf</t>
         </is>
       </c>
       <c r="AB73" t="inlineStr"/>
@@ -7858,7 +7891,7 @@
         <v>72</v>
       </c>
       <c r="B74" t="n">
-        <v>1000072</v>
+        <v>1000073</v>
       </c>
       <c r="C74" t="n">
         <v>2000001</v>
@@ -7867,92 +7900,88 @@
         <v>3000073</v>
       </c>
       <c r="E74" t="n">
-        <v>4000002</v>
+        <v>4000001</v>
       </c>
       <c r="F74" t="n">
-        <v>5000073</v>
+        <v>5000001</v>
       </c>
       <c r="G74" t="n">
-        <v>6000071</v>
+        <v>6000073</v>
       </c>
       <c r="H74" t="n">
         <v>7000001</v>
       </c>
       <c r="I74" t="n">
-        <v>8000071</v>
+        <v>8000053</v>
       </c>
       <c r="J74" t="n">
-        <v>9000073</v>
+        <v>9000057</v>
       </c>
       <c r="K74" t="n">
-        <v>10000032</v>
+        <v>10000041</v>
       </c>
       <c r="L74" t="n">
-        <v>11000048</v>
+        <v>11000073</v>
       </c>
       <c r="M74" t="n">
         <v>12000001</v>
       </c>
       <c r="N74" t="n">
-        <v>13000058</v>
+        <v>13000068</v>
       </c>
       <c r="O74" t="n">
-        <v>14000072</v>
+        <v>14000073</v>
       </c>
       <c r="P74" t="n">
         <v>15000001</v>
       </c>
       <c r="Q74" t="inlineStr">
         <is>
-          <t>Volontario di protezione civile</t>
+          <t>Consiglio di stato</t>
         </is>
       </c>
       <c r="R74" t="inlineStr"/>
       <c r="S74" t="inlineStr">
         <is>
-          <t>La legge LPPC 2002 stabilisce che possono prestare volontariamente servizio di protezione civile: a. gli uomini prosciolti dall’obbligo di prestare servizio nella protezione civile; b. gli uomini soggetti all’obbligo militare prosciolti dall’obbligo di prestare servizio militare o civile; c. gli uomini prosciolti dall’obbligo di prestare servizio militare o civile; d. le cittadine svizzere, a partire dall’anno in cui compiono i 20 anni; e. gli stranieri domiciliati in Svizzera, a partire dall’anno in cui compiono i 20 anni. Bisogna porre attenzione al fatto che secondo la stessa legge, l’unica differenza tra un milite e un volontario (entrambi di protezione civile) è il fatto che i volontari sono prosciolti dall’obbligo di prestare servizio su domanda. Infatti, per il resto, militi e volontari hanno gli stessi diritti e doveri. 
-I diritti dei militi sono essenzialmente quattro: soldo e vitto, alloggio, trasporto gratuiti, cui si aggiungono alcune agevolazioni fiscali e indennità.</t>
-        </is>
-      </c>
-      <c r="T74" t="inlineStr">
-        <is>
-          <t>Competenza della Protezione Civile</t>
-        </is>
-      </c>
-      <c r="U74" t="inlineStr">
-        <is>
-          <t>Tommaso sansone</t>
-        </is>
-      </c>
+          <t>Il Consiglio di Stato è l’autorità competente per: a) assicurare la condotta, l’intervento e il coordinamento delle organizzazioni partner; b) assicurare l’istruzione e la formazione, anche degli organi di condotta locali; c) promuovere l’aiuto intercomunale, così come la cooperazione intercantonale e
+transfrontaliera; d) esercitare le altre funzioni attribuitegli dalla presente legge.</t>
+        </is>
+      </c>
+      <c r="T74" t="inlineStr"/>
+      <c r="U74" t="inlineStr"/>
       <c r="V74" t="inlineStr">
         <is>
-          <t>Normativa nazionale: Legge federale sulla protezione della popolazione e sulla protezione civile (LPPC) del 4 ottobre 2002</t>
+          <t>Art. 7</t>
         </is>
       </c>
       <c r="W74" t="inlineStr"/>
       <c r="X74" t="inlineStr">
         <is>
-          <t>-- documento confronto normativa -- wp 3.2 gestisco -- da completare</t>
+          <t>Legge sulla protezione della popolazione (del 26 febbraio 2007)</t>
         </is>
       </c>
       <c r="Y74" t="inlineStr">
         <is>
-          <t>Tommaso sansone</t>
-        </is>
-      </c>
-      <c r="Z74" t="inlineStr"/>
+          <t>Ufficio Federale della Protezione della Popolazione</t>
+        </is>
+      </c>
+      <c r="Z74" t="inlineStr">
+        <is>
+          <t>Repubblica e Cantone Ticino</t>
+        </is>
+      </c>
       <c r="AA74" t="inlineStr">
         <is>
-          <t>https://www.admin.ch/opc/it/classified-compilation/20011872/201701010000/520.1.pdf</t>
+          <t>https://m3.ti.ch/CAN/RLeggi/public/index.php/raccolta-leggi/pdfatto/atto/48</t>
         </is>
       </c>
       <c r="AB74" t="inlineStr"/>
       <c r="AC74" s="2" t="n">
-        <v>43767</v>
+        <v>43817</v>
       </c>
       <c r="AD74" t="inlineStr">
         <is>
-          <t>ITCH00028</t>
+          <t>ITCH00029</t>
         </is>
       </c>
       <c r="AE74" t="inlineStr">
@@ -7978,31 +8007,31 @@
         <v>4000001</v>
       </c>
       <c r="F75" t="n">
-        <v>5000001</v>
+        <v>5000032</v>
       </c>
       <c r="G75" t="n">
-        <v>6000074</v>
+        <v>6000069</v>
       </c>
       <c r="H75" t="n">
         <v>7000001</v>
       </c>
       <c r="I75" t="n">
-        <v>8000053</v>
+        <v>8000069</v>
       </c>
       <c r="J75" t="n">
-        <v>9000058</v>
+        <v>9000069</v>
       </c>
       <c r="K75" t="n">
-        <v>10000042</v>
+        <v>10000032</v>
       </c>
       <c r="L75" t="n">
-        <v>11000074</v>
+        <v>11000032</v>
       </c>
       <c r="M75" t="n">
-        <v>12000001</v>
+        <v>12000002</v>
       </c>
       <c r="N75" t="n">
-        <v>13000069</v>
+        <v>13000047</v>
       </c>
       <c r="O75" t="n">
         <v>14000074</v>
@@ -8012,51 +8041,51 @@
       </c>
       <c r="Q75" t="inlineStr">
         <is>
-          <t>Consiglio di stato</t>
+          <t>Milite</t>
         </is>
       </c>
       <c r="R75" t="inlineStr"/>
       <c r="S75" t="inlineStr">
         <is>
-          <t>Il Consiglio di Stato è l’autorità competente per: a) assicurare la condotta, l’intervento e il coordinamento delle organizzazioni partner; b) assicurare l’istruzione e la formazione, anche degli organi di condotta locali; c) promuovere l’aiuto intercomunale, così come la cooperazione intercantonale e
-transfrontaliera; d) esercitare le altre funzioni attribuitegli dalla presente legge.</t>
+          <t>I militi svizzeri sono reclutati dall’esercito e dalla protezione civile e di norma vengono assegnati al loro cantone di domicilio, oppure ad altri cantoni, se deciso dal cantone di domicilio, cui comunque spetta la scelta. I militi, oltre ad essere arruolati in maniera ordinaria, possono essere incorporati nel personale di riserva. Se un milite entra a far parte del personale di riserva non deve essere necessariamente formato e non ha diritto a prestare servizio di protezione civile.
+Una volta reclutati e addestrasti, i militi possono essere chiamati a prestare servizio dal consiglio federale o dal cantone cui sono assegnati. Il Consiglio federale e il cantone di assegnamento possono chiamare in servizio i militi di protezione civile in caso di catastrofi e situazioni d’emergenza che colpiscono uno o più Cantoni, oppure le zone limitrofe di Paesi confinanti, oppure in caso di conflitto armato. I militi possono inoltre essere mobilitati anche in assenza di emergenza per svolgere dei lavori di ripristino di pubblica utilità. In quest’ultimo caso però, esistono dei limiti al potere di convocazione esercitato dalle autorità sui militi .</t>
         </is>
       </c>
       <c r="T75" t="inlineStr"/>
-      <c r="U75" t="inlineStr"/>
+      <c r="U75" t="inlineStr">
+        <is>
+          <t>Tommaso Sansone</t>
+        </is>
+      </c>
       <c r="V75" t="inlineStr">
         <is>
-          <t>Art. 7</t>
+          <t>Normativa nazionale: Legge federale sulla protezione della popolazione e sulla protezione civile (LPPC) del 4 ottobre 2002</t>
         </is>
       </c>
       <c r="W75" t="inlineStr"/>
       <c r="X75" t="inlineStr">
         <is>
-          <t>Legge sulla protezione della popolazione (del 26 febbraio 2007)</t>
+          <t>-- documento confronto normativa -- wp 3.2 gestisco -- da completare</t>
         </is>
       </c>
       <c r="Y75" t="inlineStr">
         <is>
-          <t>Ufficio Federale della Protezione della Popolazione</t>
-        </is>
-      </c>
-      <c r="Z75" t="inlineStr">
-        <is>
-          <t>Repubblica e Cantone Ticino</t>
-        </is>
-      </c>
-      <c r="AA75" t="inlineStr">
-        <is>
-          <t>https://m3.ti.ch/CAN/RLeggi/public/index.php/raccolta-leggi/pdfatto/atto/48</t>
-        </is>
-      </c>
-      <c r="AB75" t="inlineStr"/>
+          <t>Tommaso Sansone</t>
+        </is>
+      </c>
+      <c r="Z75" t="inlineStr"/>
+      <c r="AA75" t="inlineStr"/>
+      <c r="AB75" t="inlineStr">
+        <is>
+          <t>Definizione italiana, oggetto svizzero</t>
+        </is>
+      </c>
       <c r="AC75" s="2" t="n">
-        <v>43817</v>
+        <v>43766</v>
       </c>
       <c r="AD75" t="inlineStr">
         <is>
-          <t>ITCH00029</t>
+          <t>ITCH00030</t>
         </is>
       </c>
       <c r="AE75" t="inlineStr">
@@ -8070,7 +8099,7 @@
         <v>74</v>
       </c>
       <c r="B76" t="n">
-        <v>1000075</v>
+        <v>1000069</v>
       </c>
       <c r="C76" t="n">
         <v>2000001</v>
@@ -8082,19 +8111,19 @@
         <v>4000001</v>
       </c>
       <c r="F76" t="n">
-        <v>5000032</v>
+        <v>5000072</v>
       </c>
       <c r="G76" t="n">
-        <v>6000071</v>
+        <v>6000075</v>
       </c>
       <c r="H76" t="n">
         <v>7000001</v>
       </c>
       <c r="I76" t="n">
-        <v>8000071</v>
+        <v>8000075</v>
       </c>
       <c r="J76" t="n">
-        <v>9000071</v>
+        <v>9000069</v>
       </c>
       <c r="K76" t="n">
         <v>10000032</v>
@@ -8103,10 +8132,10 @@
         <v>11000032</v>
       </c>
       <c r="M76" t="n">
-        <v>12000002</v>
+        <v>12000075</v>
       </c>
       <c r="N76" t="n">
-        <v>13000048</v>
+        <v>13000068</v>
       </c>
       <c r="O76" t="n">
         <v>14000075</v>
@@ -8116,31 +8145,31 @@
       </c>
       <c r="Q76" t="inlineStr">
         <is>
-          <t>Milite</t>
+          <t>Legge sulla protezione della popolazione del 26 febbraio 2007</t>
         </is>
       </c>
       <c r="R76" t="inlineStr"/>
       <c r="S76" t="inlineStr">
         <is>
-          <t>I militi svizzeri sono reclutati dall’esercito e dalla protezione civile e di norma vengono assegnati al loro cantone di domicilio, oppure ad altri cantoni, se deciso dal cantone di domicilio, cui comunque spetta la scelta. I militi, oltre ad essere arruolati in maniera ordinaria, possono essere incorporati nel personale di riserva. Se un milite entra a far parte del personale di riserva non deve essere necessariamente formato e non ha diritto a prestare servizio di protezione civile.
-Una volta reclutati e addestrasti, i militi possono essere chiamati a prestare servizio dal consiglio federale o dal cantone cui sono assegnati. Il Consiglio federale e il cantone di assegnamento possono chiamare in servizio i militi di protezione civile in caso di catastrofi e situazioni d’emergenza che colpiscono uno o più Cantoni, oppure le zone limitrofe di Paesi confinanti, oppure in caso di conflitto armato. I militi possono inoltre essere mobilitati anche in assenza di emergenza per svolgere dei lavori di ripristino di pubblica utilità. In quest’ultimo caso però, esistono dei limiti al potere di convocazione esercitato dalle autorità sui militi .</t>
+          <t>La legge cantonale del 26 febbraio 2007 è legge di maggior riferimento del Canton Ticino in materia di protezione della popolazione.
+Essa riprende alcuni argomenti già sanciti dalla legge federale LPPC del 2002, approfondisce la struttura e i compiti di alcuni organi di protezione della popolazione cantonali, quali gli organi di condotta, e descrive il concetto di stato di necessità a livello cantonale.</t>
         </is>
       </c>
       <c r="T76" t="inlineStr"/>
       <c r="U76" t="inlineStr">
         <is>
-          <t>Tommaso Sansone</t>
+          <t>Tommaso sansone</t>
         </is>
       </c>
       <c r="V76" t="inlineStr">
         <is>
-          <t>Normativa nazionale: Legge federale sulla protezione della popolazione e sulla protezione civile (LPPC) del 4 ottobre 2002</t>
+          <t>Normativa cantonale: Legge sulla protezione della popolazione (LProtPop) del 26 febbraio 2007</t>
         </is>
       </c>
       <c r="W76" t="inlineStr"/>
       <c r="X76" t="inlineStr">
         <is>
-          <t>-- documento confronto normativa -- wp 3.2 gestisco -- da completare</t>
+          <t>-- -- documento confronto normativa -- wp 3.2 gestisco -- da completare</t>
         </is>
       </c>
       <c r="Y76" t="inlineStr">
@@ -8152,15 +8181,15 @@
       <c r="AA76" t="inlineStr"/>
       <c r="AB76" t="inlineStr">
         <is>
-          <t>Definizione italiana, oggetto svizzero</t>
+          <t>definizione italiana, oggetto svizzero</t>
         </is>
       </c>
       <c r="AC76" s="2" t="n">
-        <v>43766</v>
+        <v>43817</v>
       </c>
       <c r="AD76" t="inlineStr">
         <is>
-          <t>ITCH00030</t>
+          <t>ITCH00031</t>
         </is>
       </c>
       <c r="AE76" t="inlineStr">
@@ -8174,7 +8203,7 @@
         <v>75</v>
       </c>
       <c r="B77" t="n">
-        <v>1000076</v>
+        <v>1000026</v>
       </c>
       <c r="C77" t="n">
         <v>2000001</v>
@@ -8186,31 +8215,31 @@
         <v>4000001</v>
       </c>
       <c r="F77" t="n">
-        <v>5000073</v>
+        <v>5000001</v>
       </c>
       <c r="G77" t="n">
-        <v>6000076</v>
+        <v>6000001</v>
       </c>
       <c r="H77" t="n">
         <v>7000001</v>
       </c>
       <c r="I77" t="n">
-        <v>8000076</v>
+        <v>8000016</v>
       </c>
       <c r="J77" t="n">
-        <v>9000071</v>
+        <v>9000003</v>
       </c>
       <c r="K77" t="n">
-        <v>10000032</v>
+        <v>10000016</v>
       </c>
       <c r="L77" t="n">
-        <v>11000032</v>
+        <v>11000016</v>
       </c>
       <c r="M77" t="n">
-        <v>12000076</v>
+        <v>12000001</v>
       </c>
       <c r="N77" t="n">
-        <v>13000069</v>
+        <v>13000001</v>
       </c>
       <c r="O77" t="n">
         <v>14000076</v>
@@ -8220,149 +8249,45 @@
       </c>
       <c r="Q77" t="inlineStr">
         <is>
-          <t>Legge sulla protezione della popolazione del 26 febbraio 2007</t>
+          <t>Centro operativo regionale</t>
         </is>
       </c>
       <c r="R77" t="inlineStr"/>
       <c r="S77" t="inlineStr">
         <is>
-          <t>La legge cantonale del 26 febbraio 2007 è legge di maggior riferimento del Canton Ticino in materia di protezione della popolazione.
-Essa riprende alcuni argomenti già sanciti dalla legge federale LPPC del 2002, approfondisce la struttura e i compiti di alcuni organi di protezione della popolazione cantonali, quali gli organi di condotta, e descrive il concetto di stato di necessità a livello cantonale.</t>
+          <t>E’ una struttura costituita a livello regionale nell’ambito del sistema integrato di lotta agli incendi boschivi; provvede al coordinamento di tutte le attività in materia.</t>
         </is>
       </c>
       <c r="T77" t="inlineStr"/>
-      <c r="U77" t="inlineStr">
-        <is>
-          <t>Tommaso sansone</t>
-        </is>
-      </c>
-      <c r="V77" t="inlineStr">
-        <is>
-          <t>Normativa cantonale: Legge sulla protezione della popolazione (LProtPop) del 26 febbraio 2007</t>
-        </is>
-      </c>
+      <c r="U77" t="inlineStr"/>
+      <c r="V77" t="inlineStr"/>
       <c r="W77" t="inlineStr"/>
       <c r="X77" t="inlineStr">
         <is>
-          <t>-- -- documento confronto normativa -- wp 3.2 gestisco -- da completare</t>
-        </is>
-      </c>
-      <c r="Y77" t="inlineStr">
-        <is>
-          <t>Tommaso Sansone</t>
-        </is>
-      </c>
-      <c r="Z77" t="inlineStr"/>
-      <c r="AA77" t="inlineStr"/>
-      <c r="AB77" t="inlineStr">
-        <is>
-          <t>definizione italiana, oggetto svizzero</t>
-        </is>
-      </c>
+          <t>Piano Comunale Di Emergenza - Glossario</t>
+        </is>
+      </c>
+      <c r="Y77" t="inlineStr"/>
+      <c r="Z77" t="inlineStr">
+        <is>
+          <t>Comune di Modena</t>
+        </is>
+      </c>
+      <c r="AA77" t="inlineStr">
+        <is>
+          <t>https://www.comune.modena.it/ambiente/protezione-civile/piano-comunale-di-protezione-civile/scheda-19-glossario</t>
+        </is>
+      </c>
+      <c r="AB77" t="inlineStr"/>
       <c r="AC77" s="2" t="n">
-        <v>43817</v>
+        <v>43838</v>
       </c>
       <c r="AD77" t="inlineStr">
         <is>
-          <t>ITCH00031</t>
+          <t>ITCH00040</t>
         </is>
       </c>
       <c r="AE77" t="inlineStr">
-        <is>
-          <t>show</t>
-        </is>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" s="1" t="n">
-        <v>76</v>
-      </c>
-      <c r="B78" t="n">
-        <v>1000077</v>
-      </c>
-      <c r="C78" t="n">
-        <v>2000001</v>
-      </c>
-      <c r="D78" t="n">
-        <v>3000077</v>
-      </c>
-      <c r="E78" t="n">
-        <v>4000001</v>
-      </c>
-      <c r="F78" t="n">
-        <v>5000001</v>
-      </c>
-      <c r="G78" t="n">
-        <v>6000001</v>
-      </c>
-      <c r="H78" t="n">
-        <v>7000001</v>
-      </c>
-      <c r="I78" t="n">
-        <v>8000016</v>
-      </c>
-      <c r="J78" t="n">
-        <v>9000003</v>
-      </c>
-      <c r="K78" t="n">
-        <v>10000016</v>
-      </c>
-      <c r="L78" t="n">
-        <v>11000016</v>
-      </c>
-      <c r="M78" t="n">
-        <v>12000001</v>
-      </c>
-      <c r="N78" t="n">
-        <v>13000001</v>
-      </c>
-      <c r="O78" t="n">
-        <v>14000077</v>
-      </c>
-      <c r="P78" t="n">
-        <v>15000001</v>
-      </c>
-      <c r="Q78" t="inlineStr">
-        <is>
-          <t>Centro operativo regionale</t>
-        </is>
-      </c>
-      <c r="R78" t="inlineStr"/>
-      <c r="S78" t="inlineStr">
-        <is>
-          <t>E’ una struttura costituita a livello regionale nell’ambito del sistema integrato di lotta agli incendi boschivi; provvede al coordinamento di tutte le attività in materia.</t>
-        </is>
-      </c>
-      <c r="T78" t="inlineStr"/>
-      <c r="U78" t="inlineStr"/>
-      <c r="V78" t="inlineStr"/>
-      <c r="W78" t="inlineStr"/>
-      <c r="X78" t="inlineStr">
-        <is>
-          <t>Piano Comunale Di Emergenza - Glossario</t>
-        </is>
-      </c>
-      <c r="Y78" t="inlineStr"/>
-      <c r="Z78" t="inlineStr">
-        <is>
-          <t>Comune di Modena</t>
-        </is>
-      </c>
-      <c r="AA78" t="inlineStr">
-        <is>
-          <t>https://www.comune.modena.it/ambiente/protezione-civile/piano-comunale-di-protezione-civile/scheda-19-glossario</t>
-        </is>
-      </c>
-      <c r="AB78" t="inlineStr"/>
-      <c r="AC78" s="2" t="n">
-        <v>43838</v>
-      </c>
-      <c r="AD78" t="inlineStr">
-        <is>
-          <t>ITCH00040</t>
-        </is>
-      </c>
-      <c r="AE78" t="inlineStr">
         <is>
           <t>show</t>
         </is>

</xml_diff>

<commit_message>
corretto algoritmo PGI su processig e riversamento, mancava l'acronimo che si perdeva alla fine dell'algoritmo, tutti erano assegnati come mancanti
</commit_message>
<xml_diff>
--- a/static/saved_dataframes/Elab1.xlsx
+++ b/static/saved_dataframes/Elab1.xlsx
@@ -576,7 +576,11 @@
           <t>Centro Operativo Comunale</t>
         </is>
       </c>
-      <c r="R2" t="inlineStr"/>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>COC</t>
+        </is>
+      </c>
       <c r="S2" t="inlineStr">
         <is>
           <t>rappresenta la struttura di coordinamento di cui il sindaco, in qualità di autorità di protezione civile, si può avvalere per garantire una pronta e coordinata risposta,in caso di eventi critici, per il soccorso e l’assistenza alla popolazione, la difesa dell’ambiente e dei beni. Il c.o.c., in relazione alle esigenze riscontrate dall’ amministrazione, è organizzato in uffici, funzioni di supporto, ai quali il sindaco affida compiti specifici. Per ogni funzione di supporto attivata è individuato, nel piano comunale di protezione civile, un referente specifico, che ne coordinerà le attività avvalendosi del personale dell’amministrazione, del volontario o di altri enti/strutture. Il centro operativo comunale va quindi inteso come una struttura altamente flessibile che coadiuva il sindaco, quale autorità di protezione civile, in tutte le attività necessarie alla gestione di eventi critici o emergenziali.</t>
@@ -629,7 +633,7 @@
         <v>1000002</v>
       </c>
       <c r="C3" t="n">
-        <v>2000001</v>
+        <v>2000002</v>
       </c>
       <c r="D3" t="n">
         <v>3000002</v>
@@ -675,7 +679,11 @@
           <t>Centro Assistenziale Di Pronto Intervento</t>
         </is>
       </c>
-      <c r="R3" t="inlineStr"/>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>CAPI</t>
+        </is>
+      </c>
       <c r="S3" t="inlineStr">
         <is>
           <t>Polo logistico dove vengono stoccati e mantenuti in efficienza risorse da distribuire in caso di emergenza per il soccorso e l’assistenza alla popolazione (tende, impiantistica, effetti letterecci, generatori, etc.) e per l’operatività dei soccorritori (veicoli, idrovore, potabilizzatori,etc.). Consiste in un deposito di materiale vario da utilizzarsi in caso di calamità. Ve ne sono 14 in tutta italia e fanno capo alle seguenti prefetture: alessandria, ancona, bologna, cagliari, caserta, catania, catanzaro, firenze, palermo, potenza, reggio calabria, roma, temi e trieste.</t>
@@ -728,7 +736,7 @@
         <v>1000003</v>
       </c>
       <c r="C4" t="n">
-        <v>2000001</v>
+        <v>2000003</v>
       </c>
       <c r="D4" t="n">
         <v>3000003</v>
@@ -774,7 +782,11 @@
           <t>Centro Operativo Avanzato</t>
         </is>
       </c>
-      <c r="R4" t="inlineStr"/>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>COA</t>
+        </is>
+      </c>
       <c r="S4" t="inlineStr">
         <is>
           <t>Centro operativo che viene attivato in alcune situazioni particolari. È competente per specifici settori di intervento in un’area territoriale ristretta.</t>
@@ -823,7 +835,7 @@
         <v>1000004</v>
       </c>
       <c r="C5" t="n">
-        <v>2000001</v>
+        <v>2000004</v>
       </c>
       <c r="D5" t="n">
         <v>3000004</v>
@@ -869,7 +881,11 @@
           <t>Centro Operativo Intercomunale</t>
         </is>
       </c>
-      <c r="R5" t="inlineStr"/>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>COI</t>
+        </is>
+      </c>
       <c r="S5" t="inlineStr">
         <is>
           <t>Centro operativo che coordina gli interventi di emergenza in un ambito territoriale che generalmente comprende più comuni limitrofi o si riferisce al territorio di competenza della comunità montana. In molte realtà territoriali il coi non si attiva solo in situazione di emergenza ma è operativo anche in ordinario e funge da punto di riferimento e di raccordo sul territorio per le attività di protezione civile.</t>
@@ -918,7 +934,7 @@
         <v>1000005</v>
       </c>
       <c r="C6" t="n">
-        <v>2000001</v>
+        <v>2000005</v>
       </c>
       <c r="D6" t="n">
         <v>3000005</v>
@@ -1017,7 +1033,7 @@
         <v>1000006</v>
       </c>
       <c r="C7" t="n">
-        <v>2000001</v>
+        <v>2000006</v>
       </c>
       <c r="D7" t="n">
         <v>3000006</v>
@@ -1063,7 +1079,11 @@
           <t>Rischio</t>
         </is>
       </c>
-      <c r="R7" t="inlineStr"/>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
       <c r="S7" t="inlineStr">
         <is>
           <t>Ai fini di protezione civile, il rischio è rappresentato dalla possibilità che un fenomeno naturale o indotto dalle attività dell’uomo possa causare effetti dannosi sulla popolazione, gli insediamenti abitativi e produttivi e le infrastrutture, all’interno di una particolare area, in un determinato periodo di tempo. Il rischio è traducibile nella formula r = probabilità x vulnerabilità x esposizione.</t>
@@ -1116,7 +1136,7 @@
         <v>1000007</v>
       </c>
       <c r="C8" t="n">
-        <v>2000001</v>
+        <v>2000007</v>
       </c>
       <c r="D8" t="n">
         <v>3000007</v>
@@ -1162,7 +1182,11 @@
           <t>Centro di monitoraggio e informazione</t>
         </is>
       </c>
-      <c r="R8" t="inlineStr"/>
+      <c r="R8" t="inlineStr">
+        <is>
+          <t>CIM</t>
+        </is>
+      </c>
       <c r="S8" t="inlineStr">
         <is>
           <t>centro attivo 24 ore su 24 che rappresenta la componente operativa del meccanismo comunitario di protezione civile ed è collocato all’interno dell’unità di protezione civile nella direzione generale per gli aiuti umanitari e la protezione civile. Fornisce ai paesi l’accesso ad una piattaforma comunitaria di protezione civile, in cui vengono raccolte le richieste dei paesi dell’unione europea o extra europei colpiti da calamità e le offerte d’aiuto da parte dei paesi membri.</t>
@@ -1211,7 +1235,7 @@
         <v>1000008</v>
       </c>
       <c r="C9" t="n">
-        <v>2000001</v>
+        <v>2000008</v>
       </c>
       <c r="D9" t="n">
         <v>3000008</v>
@@ -1257,7 +1281,11 @@
           <t>Centro Operativo Aereo Unificato</t>
         </is>
       </c>
-      <c r="R9" t="inlineStr"/>
+      <c r="R9" t="inlineStr">
+        <is>
+          <t>COAU</t>
+        </is>
+      </c>
       <c r="S9" t="inlineStr">
         <is>
           <t>Struttura con cui il dipartimento della protezione civile coordina l'attività di spegnimento degli incendi boschivi con la flotta aerea dello stato sul territorio nazionale. Nel coau confluiscono le richieste di intervento inoltrate dalle sale operative regionali. Il coau è un servizio operativo dell'ufficio iv - gestione delle emergenze</t>
@@ -1306,7 +1334,7 @@
         <v>1000009</v>
       </c>
       <c r="C10" t="n">
-        <v>2000001</v>
+        <v>2000009</v>
       </c>
       <c r="D10" t="n">
         <v>3000009</v>
@@ -1352,7 +1380,11 @@
           <t>Centro Operativo</t>
         </is>
       </c>
-      <c r="R10" t="inlineStr"/>
+      <c r="R10" t="inlineStr">
+        <is>
+          <t>CO</t>
+        </is>
+      </c>
       <c r="S10" t="inlineStr">
         <is>
           <t>Centro di protezione civile attivato sul territorio colpito dall’emergenza per garantire la gestione coordinata degli interventi. Il centro deve essere collocato in area sicura rispetto alle diverse tipologie di rischio, in una struttura idonea dal punto di vista strutturale, funzionale e logistico. È strutturato in funzioni di supporto, secondo il metodo augustus, dove sono rappresentate tutte le amministrazioni, gli enti e i soggetti che concorrono alla gestione dell’emergenza. La catena classica di coordinamento, in un modello puramente teorico, prevede, dal livello locale a quallo nazionale l’attivazione dei seguenti centri gerarchicamente sovraordinati: coc - centro operativo comunale, com - centro operativo misto, ccs, - centro coordinamento soccorsi, dicomac - direzione comando e controllo.</t>
@@ -1413,7 +1445,7 @@
         <v>1000010</v>
       </c>
       <c r="C11" t="n">
-        <v>2000001</v>
+        <v>2000010</v>
       </c>
       <c r="D11" t="n">
         <v>3000010</v>
@@ -1459,7 +1491,11 @@
           <t>Centro Medico Di Evacuazione</t>
         </is>
       </c>
-      <c r="R11" t="inlineStr"/>
+      <c r="R11" t="inlineStr">
+        <is>
+          <t>CME</t>
+        </is>
+      </c>
       <c r="S11" t="inlineStr">
         <is>
           <t>Dispositivo strutturale di trattamento sanitario delle vittime che viene attivato in caso di catastrofi in un territorio particolarmente esteso. È localizzato lungo il percorso della noria di evacuazione per permettere di stabilizzare il trattamento dei feriti ed ottimizzare, su più ampia scala, l'utilizzazione delle risorse di trasporto sanitario e quelle di cura definitiva. Ad uno stesso cme possono afferire più pma. È sinonimo di ospedale da campo.</t>
@@ -1508,7 +1544,7 @@
         <v>1000011</v>
       </c>
       <c r="C12" t="n">
-        <v>2000001</v>
+        <v>2000011</v>
       </c>
       <c r="D12" t="n">
         <v>3000011</v>
@@ -1554,7 +1590,11 @@
           <t>Centro Operativo Combinato</t>
         </is>
       </c>
-      <c r="R12" t="inlineStr"/>
+      <c r="R12" t="inlineStr">
+        <is>
+          <t>COP</t>
+        </is>
+      </c>
       <c r="S12" t="inlineStr">
         <is>
           <t>E’ costituito a livello centrale presso il ministro per il coordinamento della p.c., per la direzione ed il coordinamento in emergenza degli interventi di p.c.</t>
@@ -1607,7 +1647,7 @@
         <v>1000012</v>
       </c>
       <c r="C13" t="n">
-        <v>2000001</v>
+        <v>2000012</v>
       </c>
       <c r="D13" t="n">
         <v>3000012</v>
@@ -1653,7 +1693,11 @@
           <t>Centro Polifunzionale</t>
         </is>
       </c>
-      <c r="R13" t="inlineStr"/>
+      <c r="R13" t="inlineStr">
+        <is>
+          <t>CESI</t>
+        </is>
+      </c>
       <c r="S13" t="inlineStr">
         <is>
           <t>E’ una struttura di supporto ad ogni attività di p.c.; trovasi in castelnuovo di porto (roma) e dipende dal servizio emergenze del dipartimento di p.c. Fa parte del servizio emergenze del dipartimento centro situazioni della p.c. E funziona ininterrottamente per qualsiasi evenienza o segnale d’emergenza; provvede agli interventi più importanti ed immediati.</t>
@@ -1706,7 +1750,7 @@
         <v>1000013</v>
       </c>
       <c r="C14" t="n">
-        <v>2000001</v>
+        <v>2000013</v>
       </c>
       <c r="D14" t="n">
         <v>3000013</v>
@@ -1752,7 +1796,11 @@
           <t>Centro operativo misto</t>
         </is>
       </c>
-      <c r="R14" t="inlineStr"/>
+      <c r="R14" t="inlineStr">
+        <is>
+          <t>COM</t>
+        </is>
+      </c>
       <c r="S14" t="inlineStr">
         <is>
           <t>Struttura operativa che coordina i servizi di emergenza a livello provinciale. Le strutture adibite a sede COM devono avere una suddivisione interna che preveda almeno: una sala per le riunioni, una sala per le funzioni di supporto, una sala per il volontariato, una sala per le telecomunicazioni. Il c.o.m. È una struttura operativa decentrata il cui responsabile dipende dal c.c.s. (centro coordinamento soccorsi); vi partecipano i rappresentanti dei comuni e delle strutture operative. Può essere istituito presso i comuni a cura del prefetto competente per territorio. I compiti del c.o.m. sono quelli di favorire il coordinamento dei servizi di emergenza organizzati a livello provinciale con gli interventi dei sindaci appartenenti al c.o.m. Stesso. L’ubicazione del c.o.m. Deve essere baricentrica rispetto ai comuni coordinati e localizzata in locali non vulnerabili.</t>
@@ -1805,7 +1853,7 @@
         <v>1000014</v>
       </c>
       <c r="C15" t="n">
-        <v>2000001</v>
+        <v>2000012</v>
       </c>
       <c r="D15" t="n">
         <v>3000014</v>
@@ -1851,7 +1899,11 @@
           <t>Centro Situazioni</t>
         </is>
       </c>
-      <c r="R15" t="inlineStr"/>
+      <c r="R15" t="inlineStr">
+        <is>
+          <t>CESI</t>
+        </is>
+      </c>
       <c r="S15" t="inlineStr">
         <is>
           <t>Centro nazionale che raccoglie e valuta informazioni e notizie relative a qualsiasi evento che possa determinare l'attivazione di strutture operative di protezione civile. In situazioni di emergenza si attiva come sala operativa a livello nazionale.</t>
@@ -1900,7 +1952,7 @@
         <v>1000015</v>
       </c>
       <c r="C16" t="n">
-        <v>2000001</v>
+        <v>2000015</v>
       </c>
       <c r="D16" t="n">
         <v>3000015</v>
@@ -1946,7 +1998,11 @@
           <t>Centro Coordinamento Soccorsi</t>
         </is>
       </c>
-      <c r="R16" t="inlineStr"/>
+      <c r="R16" t="inlineStr">
+        <is>
+          <t>CCS</t>
+        </is>
+      </c>
       <c r="S16" t="inlineStr">
         <is>
           <t>Rappresenta il massimo organo di coordinamento delle attività di protezione civile a livello provinciale. È composto dai responsabili di tutte le strutture operative presenti sul territorio provinciale. I compiti del ccs consistono nell'individuazione delle strategie e delle operatività di intervento necessarie al superamento dell'emergenza attraverso il coordinamento dei com.</t>
@@ -1999,7 +2055,7 @@
         <v>1000016</v>
       </c>
       <c r="C17" t="n">
-        <v>2000001</v>
+        <v>2000004</v>
       </c>
       <c r="D17" t="n">
         <v>3000016</v>
@@ -2045,7 +2101,11 @@
           <t>Centro Operativo Interforze</t>
         </is>
       </c>
-      <c r="R17" t="inlineStr"/>
+      <c r="R17" t="inlineStr">
+        <is>
+          <t>COI</t>
+        </is>
+      </c>
       <c r="S17" t="inlineStr">
         <is>
           <t>E’ costituito presso lo stato maggiore dell’esercito per la pianificazione ed il coordinamento specifico degli interventi delle forze armate in concorso.</t>
@@ -2094,7 +2154,7 @@
         <v>1000017</v>
       </c>
       <c r="C18" t="n">
-        <v>2000001</v>
+        <v>2000017</v>
       </c>
       <c r="D18" t="n">
         <v>3000017</v>
@@ -2140,7 +2200,11 @@
           <t>Centro Operativo Locale</t>
         </is>
       </c>
-      <c r="R18" t="inlineStr"/>
+      <c r="R18" t="inlineStr">
+        <is>
+          <t>COL</t>
+        </is>
+      </c>
       <c r="S18" t="inlineStr">
         <is>
           <t>E’ una struttura costituita localmente (stazione del corpo forestale dello stato) nell’ambito del sistema integrato di lotta agli incendi boschivi; controlla un’area più o meno estesa del territorio comunale od intercomunale. Ad esso sono collegate diverse stazioni fisse di rilevamento ed é predisposto a ricevere comunicazioni (aib) da aerei, finalizzate all’avvistamento. Valuta sulla base delle informazioni, l’esigenza di intervento aereo e la segnala al centro operativo provinciale (c.o.p.)</t>
@@ -2193,7 +2257,7 @@
         <v>1000018</v>
       </c>
       <c r="C19" t="n">
-        <v>2000001</v>
+        <v>2000011</v>
       </c>
       <c r="D19" t="n">
         <v>3000018</v>
@@ -2239,7 +2303,11 @@
           <t>Centro Operativo Provinciale</t>
         </is>
       </c>
-      <c r="R19" t="inlineStr"/>
+      <c r="R19" t="inlineStr">
+        <is>
+          <t>COP</t>
+        </is>
+      </c>
       <c r="S19" t="inlineStr">
         <is>
           <t>E’ una struttura costituita a livello provinciale nell’ambito del sistema integrato di lotta agli incendi boschivi; provvede al coordinamento dell’attività di tutti i col di competenza, al controllo ed alla gestione dell’intervento e delle risorse a livello provinciale, al collegamento operativo con il cor.</t>
@@ -2288,7 +2356,7 @@
         <v>1000019</v>
       </c>
       <c r="C20" t="n">
-        <v>2000001</v>
+        <v>2000005</v>
       </c>
       <c r="D20" t="n">
         <v>3000019</v>
@@ -2399,7 +2467,7 @@
         <v>1000020</v>
       </c>
       <c r="C21" t="n">
-        <v>2000001</v>
+        <v>2000005</v>
       </c>
       <c r="D21" t="n">
         <v>3000020</v>
@@ -2510,7 +2578,7 @@
         <v>1000021</v>
       </c>
       <c r="C22" t="n">
-        <v>2000001</v>
+        <v>2000005</v>
       </c>
       <c r="D22" t="n">
         <v>3000021</v>
@@ -2621,7 +2689,7 @@
         <v>1000022</v>
       </c>
       <c r="C23" t="n">
-        <v>2000001</v>
+        <v>2000005</v>
       </c>
       <c r="D23" t="n">
         <v>3000022</v>
@@ -2732,7 +2800,7 @@
         <v>1000023</v>
       </c>
       <c r="C24" t="n">
-        <v>2000001</v>
+        <v>2000005</v>
       </c>
       <c r="D24" t="n">
         <v>3000023</v>
@@ -2843,7 +2911,7 @@
         <v>1000024</v>
       </c>
       <c r="C25" t="n">
-        <v>2000001</v>
+        <v>2000024</v>
       </c>
       <c r="D25" t="n">
         <v>3000024</v>
@@ -2889,7 +2957,11 @@
           <t>Emergenza Di Tipo A</t>
         </is>
       </c>
-      <c r="R25" t="inlineStr"/>
+      <c r="R25" t="inlineStr">
+        <is>
+          <t>a)</t>
+        </is>
+      </c>
       <c r="S25" t="inlineStr">
         <is>
           <t>Emergenze connesse con eventi calamitosi di origine naturale o derivanti dall'attivita' dell'uomo che possono essere fronteggiati mediante interventi attuabili, dai singoli enti e amministrazioni competenti in via ordinaria;</t>
@@ -2954,7 +3026,7 @@
         <v>1000025</v>
       </c>
       <c r="C26" t="n">
-        <v>2000001</v>
+        <v>2000026</v>
       </c>
       <c r="D26" t="n">
         <v>3000026</v>
@@ -3000,7 +3072,11 @@
           <t>Emergenza Di Tipo B</t>
         </is>
       </c>
-      <c r="R26" t="inlineStr"/>
+      <c r="R26" t="inlineStr">
+        <is>
+          <t>b)</t>
+        </is>
+      </c>
       <c r="S26" t="inlineStr">
         <is>
           <t>Emergenze connesse con eventi calamitosi di origine naturale o derivanti dall'attivita' dell'uomo che per loro natura o estensione comportano l'intervento coordinato di piu' enti o amministrazioni, e debbono essere fronteggiati con mezzi e poteri straordinari da impiegare durante limitati e predefiniti periodi di tempo, disciplinati dalle Regioni e dalle Province autonome di Trento e di Bolzano nell'esercizio della rispettiva potesta' legislativa;</t>
@@ -3061,7 +3137,7 @@
         <v>1000025</v>
       </c>
       <c r="C27" t="n">
-        <v>2000001</v>
+        <v>2000025</v>
       </c>
       <c r="D27" t="n">
         <v>3000025</v>
@@ -3107,7 +3183,11 @@
           <t>Emergenza Di Tipo B</t>
         </is>
       </c>
-      <c r="R27" t="inlineStr"/>
+      <c r="R27" t="inlineStr">
+        <is>
+          <t>NBC - B</t>
+        </is>
+      </c>
       <c r="S27" t="inlineStr">
         <is>
           <t>Emergenza determinata dall'emissione illecita di sostanze biologiche, organismi patogeni (che causano malattie) o dei loro prodotti metabolici. L'emissione può essere accidentale (incidente) o intenzionale (atto criminale o terroristico).</t>
@@ -3160,7 +3240,7 @@
         <v>1000027</v>
       </c>
       <c r="C28" t="n">
-        <v>2000001</v>
+        <v>2000027</v>
       </c>
       <c r="D28" t="n">
         <v>3000027</v>
@@ -3206,7 +3286,11 @@
           <t>Emergenza Di Tipo C</t>
         </is>
       </c>
-      <c r="R28" t="inlineStr"/>
+      <c r="R28" t="inlineStr">
+        <is>
+          <t>c)</t>
+        </is>
+      </c>
       <c r="S28" t="inlineStr">
         <is>
           <t>Emergenze di rilievo nazionale connesse con eventi calamitosi di origine naturale o derivanti dall'attivita' dell'uomo che in ragione della loro intensita' o estensione debbono, con immediatezza d'intervento, essere fronteggiate con mezzi e poteri straordinari da impiegare durante limitati e predefiniti periodi di tempo ai sensi dell'articolo 24.</t>
@@ -3271,7 +3355,7 @@
         <v>1000028</v>
       </c>
       <c r="C29" t="n">
-        <v>2000001</v>
+        <v>2000005</v>
       </c>
       <c r="D29" t="n">
         <v>3000028</v>
@@ -3378,7 +3462,7 @@
         <v>1000029</v>
       </c>
       <c r="C30" t="n">
-        <v>2000001</v>
+        <v>2000005</v>
       </c>
       <c r="D30" t="n">
         <v>3000029</v>
@@ -3489,7 +3573,7 @@
         <v>1000030</v>
       </c>
       <c r="C31" t="n">
-        <v>2000001</v>
+        <v>2000005</v>
       </c>
       <c r="D31" t="n">
         <v>3000030</v>
@@ -3600,7 +3684,7 @@
         <v>1000031</v>
       </c>
       <c r="C32" t="n">
-        <v>2000001</v>
+        <v>2000005</v>
       </c>
       <c r="D32" t="n">
         <v>3000031</v>
@@ -3711,7 +3795,7 @@
         <v>1000032</v>
       </c>
       <c r="C33" t="n">
-        <v>2000001</v>
+        <v>2000005</v>
       </c>
       <c r="D33" t="n">
         <v>3000032</v>
@@ -3798,7 +3882,7 @@
         <v>1000033</v>
       </c>
       <c r="C34" t="n">
-        <v>2000001</v>
+        <v>2000005</v>
       </c>
       <c r="D34" t="n">
         <v>3000033</v>
@@ -3897,7 +3981,7 @@
         <v>1000034</v>
       </c>
       <c r="C35" t="n">
-        <v>2000001</v>
+        <v>2000034</v>
       </c>
       <c r="D35" t="n">
         <v>3000034</v>
@@ -3943,7 +4027,11 @@
           <t>Centrale nazionale d'allarme</t>
         </is>
       </c>
-      <c r="R35" t="inlineStr"/>
+      <c r="R35" t="inlineStr">
+        <is>
+          <t>CENAL</t>
+        </is>
+      </c>
       <c r="S35" t="inlineStr">
         <is>
           <t>La CENAL, una divisione dell'Ufficio federale della protezione della popolazione (UFPP), è l'organo federale competente per gli eventi straordinari. Il compito principale della CENAL è quello di tracciare il quadro della situazione prioritaria per la protezione della popolazione. A tal fine, sia nella quotidianità che in caso d'evento scambia informazioni con le autorità competenti dei Cantoni, diversi uffici federali, i gestori delle reti di telecomunicazione, dell'energia e dei trasporti, organizzazioni internazionali e con i centri d'analisi della situazione dei Paesi limitrofi. In caso d'evento, funge da primo punto di contatto per i Cantoni in relazione a tutte le questioni inerenti alla protezione della popolazione. In caso di eventi maggiori, la CENAL informa lo stato maggiore federale Protezione della popolazione e l'assiste nel suo lavoro.</t>
@@ -3996,7 +4084,7 @@
         <v>1000035</v>
       </c>
       <c r="C36" t="n">
-        <v>2000001</v>
+        <v>2000035</v>
       </c>
       <c r="D36" t="n">
         <v>3000035</v>
@@ -4042,7 +4130,11 @@
           <t>Stato maggiore federale Protezione della popolazione</t>
         </is>
       </c>
-      <c r="R36" t="inlineStr"/>
+      <c r="R36" t="inlineStr">
+        <is>
+          <t>SMFP</t>
+        </is>
+      </c>
       <c r="S36" t="inlineStr">
         <is>
           <t>Nel caso in cui si delinea o si è verificato un evento di portata nazionale rilevante per la protezione della popolazione, lo SMFP assume i compiti seguenti (art. 4, cpv. 2 OSMFP):
@@ -4101,7 +4193,7 @@
         <v>1000036</v>
       </c>
       <c r="C37" t="n">
-        <v>2000001</v>
+        <v>2000037</v>
       </c>
       <c r="D37" t="n">
         <v>3000037</v>
@@ -4147,7 +4239,11 @@
           <t>Protezione civile</t>
         </is>
       </c>
-      <c r="R37" t="inlineStr"/>
+      <c r="R37" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="S37" t="inlineStr">
         <is>
           <t>Il Servizio nazionale della protezione civile, di seguito Servizio nazionale, definito di pubblica utilita', e' il sistema che esercita la funzione di protezione civile costituita dall'insieme delle competenze e delle attivita' volte a tutelare la vita, l'integrita' fisica, i beni, gli insediamenti, gli animali e l'ambiente dai danni o dal pericolo di danni derivanti da eventi calamitosi di origine naturale o derivanti dall'attivita' dell'uomo.</t>
@@ -4216,7 +4312,7 @@
         <v>1000036</v>
       </c>
       <c r="C38" t="n">
-        <v>2000001</v>
+        <v>2000005</v>
       </c>
       <c r="D38" t="n">
         <v>3000036</v>
@@ -4323,7 +4419,7 @@
         <v>1000038</v>
       </c>
       <c r="C39" t="n">
-        <v>2000001</v>
+        <v>2000005</v>
       </c>
       <c r="D39" t="n">
         <v>3000038</v>
@@ -4427,7 +4523,7 @@
         <v>1000039</v>
       </c>
       <c r="C40" t="n">
-        <v>2000001</v>
+        <v>2000005</v>
       </c>
       <c r="D40" t="n">
         <v>3000039</v>
@@ -4530,7 +4626,7 @@
         <v>1000040</v>
       </c>
       <c r="C41" t="n">
-        <v>2000001</v>
+        <v>2000040</v>
       </c>
       <c r="D41" t="n">
         <v>3000040</v>
@@ -4576,7 +4672,11 @@
           <t>Evento NBC</t>
         </is>
       </c>
-      <c r="R41" t="inlineStr"/>
+      <c r="R41" t="inlineStr">
+        <is>
+          <t>NBC</t>
+        </is>
+      </c>
       <c r="S41" t="inlineStr">
         <is>
           <t>Per evento NBC s'intende l'emissione illecita di sostanze nucleari (atomiche e radiologiche, N), biologiche (B) o chimiche (C). L'emissione può essere accidentale (incidente) o intenzionale (atto criminale o terroristico). Si distinguono i seguenti settori:
@@ -4636,7 +4736,7 @@
         <v>1000041</v>
       </c>
       <c r="C42" t="n">
-        <v>2000001</v>
+        <v>2000005</v>
       </c>
       <c r="D42" t="n">
         <v>3000041</v>
@@ -4743,7 +4843,7 @@
         <v>1000042</v>
       </c>
       <c r="C43" t="n">
-        <v>2000001</v>
+        <v>2000005</v>
       </c>
       <c r="D43" t="n">
         <v>3000042</v>
@@ -4850,7 +4950,7 @@
         <v>1000043</v>
       </c>
       <c r="C44" t="n">
-        <v>2000001</v>
+        <v>2000043</v>
       </c>
       <c r="D44" t="n">
         <v>3000043</v>
@@ -4896,7 +4996,11 @@
           <t>Vigili del fuoco</t>
         </is>
       </c>
-      <c r="R44" t="inlineStr"/>
+      <c r="R44" t="inlineStr">
+        <is>
+          <t>VVFF</t>
+        </is>
+      </c>
       <c r="S44" t="inlineStr">
         <is>
           <t>In occasione degli eventi calamitosi, il Corpo nazionale dei vigili del fuoco opera gli interventi di soccorso tecnico indifferibili e urgenti: di ricerca e salvataggio delle persone e – ai fini della salvaguardia della pubblica incolumità – anche di messa in sicurezza dei luoghi, delle strutture e degli impianti.</t>
@@ -4965,7 +5069,7 @@
         <v>1000045</v>
       </c>
       <c r="C45" t="n">
-        <v>2000001</v>
+        <v>2000005</v>
       </c>
       <c r="D45" t="n">
         <v>3000045</v>
@@ -5076,7 +5180,7 @@
         <v>1000044</v>
       </c>
       <c r="C46" t="n">
-        <v>2000001</v>
+        <v>2000005</v>
       </c>
       <c r="D46" t="n">
         <v>3000044</v>
@@ -5191,7 +5295,7 @@
         <v>1000046</v>
       </c>
       <c r="C47" t="n">
-        <v>2000001</v>
+        <v>2000005</v>
       </c>
       <c r="D47" t="n">
         <v>3000046</v>
@@ -5291,7 +5395,7 @@
         <v>1000047</v>
       </c>
       <c r="C48" t="n">
-        <v>2000001</v>
+        <v>2000005</v>
       </c>
       <c r="D48" t="n">
         <v>3000047</v>
@@ -5394,7 +5498,7 @@
         <v>1000048</v>
       </c>
       <c r="C49" t="n">
-        <v>2000001</v>
+        <v>2000005</v>
       </c>
       <c r="D49" t="n">
         <v>3000048</v>
@@ -5513,7 +5617,7 @@
         <v>1000049</v>
       </c>
       <c r="C50" t="n">
-        <v>2000001</v>
+        <v>2000005</v>
       </c>
       <c r="D50" t="n">
         <v>3000049</v>
@@ -5612,7 +5716,7 @@
         <v>1000050</v>
       </c>
       <c r="C51" t="n">
-        <v>2000001</v>
+        <v>2000005</v>
       </c>
       <c r="D51" t="n">
         <v>3000050</v>
@@ -5711,7 +5815,7 @@
         <v>1000051</v>
       </c>
       <c r="C52" t="n">
-        <v>2000001</v>
+        <v>2000005</v>
       </c>
       <c r="D52" t="n">
         <v>3000051</v>
@@ -5810,7 +5914,7 @@
         <v>1000052</v>
       </c>
       <c r="C53" t="n">
-        <v>2000001</v>
+        <v>2000005</v>
       </c>
       <c r="D53" t="n">
         <v>3000052</v>
@@ -5913,7 +6017,7 @@
         <v>1000053</v>
       </c>
       <c r="C54" t="n">
-        <v>2000001</v>
+        <v>2000005</v>
       </c>
       <c r="D54" t="n">
         <v>3000053</v>
@@ -6016,7 +6120,7 @@
         <v>1000054</v>
       </c>
       <c r="C55" t="n">
-        <v>2000001</v>
+        <v>2000054</v>
       </c>
       <c r="D55" t="n">
         <v>3000054</v>
@@ -6062,7 +6166,11 @@
           <t>Organizzazione degli Stati maggiori di condotta</t>
         </is>
       </c>
-      <c r="R55" t="inlineStr"/>
+      <c r="R55" t="inlineStr">
+        <is>
+          <t>OSMC</t>
+        </is>
+      </c>
       <c r="S55" t="inlineStr">
         <is>
           <t>L’Organizzazione degli Stati maggiori di condotta (OSMC) è composta dai rappresentanti della Polizia cantonale, della Federazione cantonale ticinese corpi pompieri, della Federazione cantonale ticinese servizi autoambulanze, del Servizio della protezione civile cantonale, dei servizi tecnici e del Dipartimento delle istituzioni; ogni organizzazione designa il proprio rappresentante. A seconda delle necessità possono essere designati ulteriori responsabili per i servizi tecnici. L’OSMC è diretta dal rappresentante del Dipartimento.</t>
@@ -6119,7 +6227,7 @@
         <v>1000055</v>
       </c>
       <c r="C56" t="n">
-        <v>2000001</v>
+        <v>2000005</v>
       </c>
       <c r="D56" t="n">
         <v>3000055</v>
@@ -6225,7 +6333,7 @@
         <v>1000056</v>
       </c>
       <c r="C57" t="n">
-        <v>2000001</v>
+        <v>2000056</v>
       </c>
       <c r="D57" t="n">
         <v>3000056</v>
@@ -6271,7 +6379,11 @@
           <t>Stato maggiore cantonale di condotta</t>
         </is>
       </c>
-      <c r="R57" t="inlineStr"/>
+      <c r="R57" t="inlineStr">
+        <is>
+          <t>SMCC</t>
+        </is>
+      </c>
       <c r="S57" t="inlineStr">
         <is>
           <t>Lo SMCC è l’organo cantonale di condotta del Consiglio di Stato, che ne definisce la composizione, l’organizzazione e il funzionamento. Esso elabora le basi decisionali per il Consiglio di Stato, lo coadiuva nelle funzioni di direzione e coordinamento ed esegue le sue decisioni. Esso è competente quando le circostanze lo esigono, per predisporre e coordinare, in collaborazione con le autorità locali, le necessarie misure d’urgenza e di assistenza e condurne l’attuazione. La sua attivazione è decisa dal Comandante della Polizia cantonale; in caso di impedimento di questo e in successione, dal suo sostituto o dall’ufficiale di picchetto della Polizia cantonale.</t>
@@ -6328,7 +6440,7 @@
         <v>1000057</v>
       </c>
       <c r="C58" t="n">
-        <v>2000001</v>
+        <v>2000005</v>
       </c>
       <c r="D58" t="n">
         <v>3000057</v>
@@ -6415,7 +6527,7 @@
         <v>1000058</v>
       </c>
       <c r="C59" t="n">
-        <v>2000001</v>
+        <v>2000005</v>
       </c>
       <c r="D59" t="n">
         <v>3000058</v>
@@ -6510,7 +6622,7 @@
         <v>1000059</v>
       </c>
       <c r="C60" t="n">
-        <v>2000001</v>
+        <v>2000059</v>
       </c>
       <c r="D60" t="n">
         <v>3000059</v>
@@ -6556,7 +6668,11 @@
           <t>Stato maggiore regionale di condotta</t>
         </is>
       </c>
-      <c r="R60" t="inlineStr"/>
+      <c r="R60" t="inlineStr">
+        <is>
+          <t>SMRC</t>
+        </is>
+      </c>
       <c r="S60" t="inlineStr">
         <is>
           <t>Lo SMRC è un organo di condotta che permette la coordinazione di più SMEPI attivi nella medesima regione. La costituzione di uno SMRC può essere ordinata o autorizzata dal Comandante dello SMCC. Esso è di norma condotto da un ufficiale della Polizia cantonale.</t>
@@ -6613,7 +6729,7 @@
         <v>1000060</v>
       </c>
       <c r="C61" t="n">
-        <v>2000001</v>
+        <v>2000060</v>
       </c>
       <c r="D61" t="n">
         <v>3000060</v>
@@ -6659,7 +6775,11 @@
           <t>Stato maggiore enti di primo intervento</t>
         </is>
       </c>
-      <c r="R61" t="inlineStr"/>
+      <c r="R61" t="inlineStr">
+        <is>
+          <t>SMEPI</t>
+        </is>
+      </c>
       <c r="S61" t="inlineStr">
         <is>
           <t>Lo SMEPI coordina l’intervento dei primi enti mobilitati, di regola polizia, pompieri e servizi d’autoambulanza. Esso è condotto, di principio, dalla Polizia cantonale.</t>
@@ -6712,7 +6832,7 @@
         <v>1000036</v>
       </c>
       <c r="C62" t="n">
-        <v>2000001</v>
+        <v>2000037</v>
       </c>
       <c r="D62" t="n">
         <v>3000037</v>
@@ -6758,7 +6878,11 @@
           <t>Protezione civile</t>
         </is>
       </c>
-      <c r="R62" t="inlineStr"/>
+      <c r="R62" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="S62" t="inlineStr">
         <is>
           <t>Il Servizio nazionale della protezione civile, di seguito Servizio nazionale, definito di pubblica utilita', e' il sistema che esercita la funzione di protezione civile costituita dall'insieme delle competenze e delle attivita' volte a tutelare la vita, l'integrita' fisica, i beni, gli insediamenti, gli animali e l'ambiente dai danni o dal pericolo di danni derivanti da eventi calamitosi di origine naturale o derivanti dall'attivita' dell'uomo.</t>
@@ -6828,7 +6952,7 @@
         <v>1000062</v>
       </c>
       <c r="C63" t="n">
-        <v>2000001</v>
+        <v>2000005</v>
       </c>
       <c r="D63" t="n">
         <v>3000062</v>
@@ -6942,7 +7066,7 @@
         <v>1000063</v>
       </c>
       <c r="C64" t="n">
-        <v>2000001</v>
+        <v>2000005</v>
       </c>
       <c r="D64" t="n">
         <v>3000063</v>
@@ -7037,7 +7161,7 @@
         <v>1000064</v>
       </c>
       <c r="C65" t="n">
-        <v>2000001</v>
+        <v>2000005</v>
       </c>
       <c r="D65" t="n">
         <v>3000061</v>
@@ -7144,7 +7268,7 @@
         <v>1000064</v>
       </c>
       <c r="C66" t="n">
-        <v>2000001</v>
+        <v>2000064</v>
       </c>
       <c r="D66" t="n">
         <v>3000064</v>
@@ -7190,7 +7314,11 @@
           <t>Legge federale sulla protezione della popolazione e sulla protezione civile</t>
         </is>
       </c>
-      <c r="R66" t="inlineStr"/>
+      <c r="R66" t="inlineStr">
+        <is>
+          <t>LPPC</t>
+        </is>
+      </c>
       <c r="S66" t="inlineStr"/>
       <c r="T66" t="inlineStr"/>
       <c r="U66" t="inlineStr"/>
@@ -7227,7 +7355,7 @@
         <v>1000066</v>
       </c>
       <c r="C67" t="n">
-        <v>2000001</v>
+        <v>2000005</v>
       </c>
       <c r="D67" t="n">
         <v>3000067</v>
@@ -7335,7 +7463,7 @@
         <v>1000066</v>
       </c>
       <c r="C68" t="n">
-        <v>2000001</v>
+        <v>2000005</v>
       </c>
       <c r="D68" t="n">
         <v>3000066</v>
@@ -7434,7 +7562,7 @@
         <v>1000068</v>
       </c>
       <c r="C69" t="n">
-        <v>2000001</v>
+        <v>2000005</v>
       </c>
       <c r="D69" t="n">
         <v>3000068</v>
@@ -7538,7 +7666,7 @@
         <v>1000069</v>
       </c>
       <c r="C70" t="n">
-        <v>2000001</v>
+        <v>2000005</v>
       </c>
       <c r="D70" t="n">
         <v>3000069</v>
@@ -7642,7 +7770,7 @@
         <v>1000070</v>
       </c>
       <c r="C71" t="n">
-        <v>2000001</v>
+        <v>2000070</v>
       </c>
       <c r="D71" t="n">
         <v>3000070</v>
@@ -7688,7 +7816,11 @@
           <t>Legge sulla protezione della popolazione del 26 febbraio 2007</t>
         </is>
       </c>
-      <c r="R71" t="inlineStr"/>
+      <c r="R71" t="inlineStr">
+        <is>
+          <t>LProtPop</t>
+        </is>
+      </c>
       <c r="S71" t="inlineStr">
         <is>
           <t>La legge cantonale del 26 febbraio 2007 è legge di maggior riferimento del Canton Ticino in materia di protezione della popolazione.
@@ -7746,7 +7878,7 @@
         <v>1000071</v>
       </c>
       <c r="C72" t="n">
-        <v>2000001</v>
+        <v>2000071</v>
       </c>
       <c r="D72" t="n">
         <v>3000071</v>
@@ -7792,7 +7924,11 @@
           <t>Nucleo Unitario di Valutazione e Risposta Emergenze transfrontaliere</t>
         </is>
       </c>
-      <c r="R72" t="inlineStr"/>
+      <c r="R72" t="inlineStr">
+        <is>
+          <t>NUVRE</t>
+        </is>
+      </c>
       <c r="S72" t="inlineStr">
         <is>
           <t>team transfrontaliero di coordinamento costituito congiuntamente da personale qualificato, formato e attrezzato, della protezione civile lombarda e ticinese. Esso ha il compito, durante le emergenze nei territori di confine, di operare insieme sia per la valutazione dell’evento in corso e per i reciproci possibili riflessi sui rispettivi territori, sia quali “ufficiali di collegamento” per collegare le rispettive sale operative di ambo i lati del confine, consentendo una efficiente ed efficace relazione operativa. Il NUVRE viene introdotto dal progetto Gestisco 2018-2021.</t>
@@ -7829,7 +7965,7 @@
         <v>1000043</v>
       </c>
       <c r="C73" t="n">
-        <v>2000001</v>
+        <v>2000072</v>
       </c>
       <c r="D73" t="n">
         <v>3000072</v>
@@ -7875,7 +8011,11 @@
           <t>Vigili del fuoco</t>
         </is>
       </c>
-      <c r="R73" t="inlineStr"/>
+      <c r="R73" t="inlineStr">
+        <is>
+          <t>VVF</t>
+        </is>
+      </c>
       <c r="S73" t="inlineStr">
         <is>
           <t>Struttura operativa della protezione civile.</t>
@@ -7916,7 +8056,7 @@
         <v>1000073</v>
       </c>
       <c r="C74" t="n">
-        <v>2000001</v>
+        <v>2000073</v>
       </c>
       <c r="D74" t="n">
         <v>3000073</v>
@@ -7962,7 +8102,11 @@
           <t>Sala Operativa Regionale dell'Emergenza Urgenza</t>
         </is>
       </c>
-      <c r="R74" t="inlineStr"/>
+      <c r="R74" t="inlineStr">
+        <is>
+          <t>SOREU</t>
+        </is>
+      </c>
       <c r="S74" t="inlineStr">
         <is>
           <t>Le SOREU hanno valenza interprovinciale: gestiscono le chiamate di soccorso sanitario con l'invio dei mezzi più appropriati fino al completamento del soccorso e/o all'eventuale affidamento del paziente alle strutture ospedaliere più idonee. Le SOREU operano tramite le dotazioni tecnologiche assegnate da AREU che permettono loro una costante interconnessione con i Call Center NUE 112 di riferimento, con i mezzi di soccorso delle AAT della propria area di competenza e con i Call Center sanitari specialistici, in modo da ottimizzare i tempi di risposta e intervento.</t>
@@ -8011,7 +8155,7 @@
         <v>1000074</v>
       </c>
       <c r="C75" t="n">
-        <v>2000001</v>
+        <v>2000005</v>
       </c>
       <c r="D75" t="n">
         <v>3000074</v>
@@ -8106,7 +8250,7 @@
         <v>1000075</v>
       </c>
       <c r="C76" t="n">
-        <v>2000001</v>
+        <v>2000075</v>
       </c>
       <c r="D76" t="n">
         <v>3000075</v>
@@ -8152,7 +8296,11 @@
           <t>sezione del militare e della protezione della popolazione</t>
         </is>
       </c>
-      <c r="R76" t="inlineStr"/>
+      <c r="R76" t="inlineStr">
+        <is>
+          <t>SMPP</t>
+        </is>
+      </c>
       <c r="S76" t="inlineStr">
         <is>
           <t>La Sezione è articolata in cinque servizi con distinte aree di competenza: il Servizio amministrativo, il Servizio degli affari militari e del comando di circondario, il Servizio della protezione civile, il Servizio costruzioni di protezione civile e il Servizio della protezione della popolazione. 
@@ -8206,7 +8354,7 @@
         <v>1000026</v>
       </c>
       <c r="C77" t="n">
-        <v>2000001</v>
+        <v>2000076</v>
       </c>
       <c r="D77" t="n">
         <v>3000076</v>
@@ -8252,7 +8400,11 @@
           <t>Centro operativo regionale</t>
         </is>
       </c>
-      <c r="R77" t="inlineStr"/>
+      <c r="R77" t="inlineStr">
+        <is>
+          <t>COR</t>
+        </is>
+      </c>
       <c r="S77" t="inlineStr">
         <is>
           <t>E’ una struttura costituita a livello regionale nell’ambito del sistema integrato di lotta agli incendi boschivi; provvede al coordinamento di tutte le attività in materia.</t>

</xml_diff>

<commit_message>
aggiunto algoritmo di sostituzione apici, virgolette è e perchè scritti male
</commit_message>
<xml_diff>
--- a/static/saved_dataframes/Elab1.xlsx
+++ b/static/saved_dataframes/Elab1.xlsx
@@ -726,7 +726,7 @@
       </c>
       <c r="AD2" t="inlineStr">
         <is>
-          <t>Centro operativo che viene attivato in alcune situazioni particolari. È competente per specifici settori di intervento in un’area territoriale ristretta.</t>
+          <t>Centro operativo che viene attivato in alcune situazioni particolari. È competente per specifici settori di intervento in un'area territoriale ristretta.</t>
         </is>
       </c>
       <c r="AE2" t="inlineStr"/>
@@ -1024,7 +1024,7 @@
       <c r="AC4" t="inlineStr"/>
       <c r="AD4" t="inlineStr">
         <is>
-          <t>Probabilità che in una data area si verifichi un evento dannoso di una determinata intensità entro un determinato periodo di tempo, il tempo di ritorno. La pericolosità è funzione della frequenza dell’evento. In alcuni casi, ad esempio le alluvioni, è possibile stimare con un’approssimazione accettabile la probabilità che si verifichi un determinato evento entro il periodo di ritorno. In altri casi, come per alcuni tipi di frane, la stima è invece più difficile.</t>
+          <t>Probabilità che in una data area si verifichi un evento dannoso di una determinata intensità entro un determinato periodo di tempo, il tempo di ritorno. La pericolosità è funzione della frequenza dell'evento. In alcuni casi, ad esempio le alluvioni, è possibile stimare con un'approssimazione accettabile la probabilità che si verifichi un determinato evento entro il periodo di ritorno. In altri casi, come per alcuni tipi di frane, la stima è invece più difficile.</t>
         </is>
       </c>
       <c r="AE4" t="inlineStr"/>
@@ -1175,7 +1175,7 @@
       </c>
       <c r="AD5" t="inlineStr">
         <is>
-          <t>Ai fini di protezione civile, il rischio è rappresentato dalla possibilità che un fenomeno naturale o indotto dalle attività dell’uomo possa causare effetti dannosi sulla popolazione, gli insediamenti abitativi e produttivi e le infrastrutture, all’interno di una particolare area, in un determinato periodo di tempo. Il rischio è traducibile nella formula r = probabilità x vulnerabilità x esposizione.</t>
+          <t>Ai fini di protezione civile, il rischio è rappresentato dalla possibilità che un fenomeno naturale o indotto dalle attività dell'uomo possa causare effetti dannosi sulla popolazione, gli insediamenti abitativi e produttivi e le infrastrutture, all'interno di una particolare area, in un determinato periodo di tempo. Il rischio è traducibile nella formula r = probabilità x vulnerabilità x esposizione.</t>
         </is>
       </c>
       <c r="AE5" t="inlineStr"/>
@@ -1326,7 +1326,7 @@
       </c>
       <c r="AD6" t="inlineStr">
         <is>
-          <t>centro attivo 24 ore su 24 che rappresenta la componente operativa del meccanismo comunitario di protezione civile ed è collocato all’interno dell’unità di protezione civile nella direzione generale per gli aiuti umanitari e la protezione civile. Fornisce ai paesi l’accesso ad una piattaforma comunitaria di protezione civile, in cui vengono raccolte le richieste dei paesi dell’unione europea o extra europei colpiti da calamità e le offerte d’aiuto da parte dei paesi membri.</t>
+          <t>centro attivo 24 ore su 24 che rappresenta la componente operativa del meccanismo comunitario di protezione civile ed è collocato all'interno dell'unità di protezione civile nella direzione generale per gli aiuti umanitari e la protezione civile. Fornisce ai paesi l'accesso ad una piattaforma comunitaria di protezione civile, in cui vengono raccolte le richieste dei paesi dell'unione europea o extra europei colpiti da calamità e le offerte d'aiuto da parte dei paesi membri.</t>
         </is>
       </c>
       <c r="AE6" t="inlineStr"/>
@@ -1628,7 +1628,7 @@
       </c>
       <c r="AD8" t="inlineStr">
         <is>
-          <t>Centro di protezione civile attivato sul territorio colpito dall’emergenza per garantire la gestione coordinata degli interventi. Il centro deve essere collocato in area sicura rispetto alle diverse tipologie di rischio, in una struttura idonea dal punto di vista strutturale, funzionale e logistico. È strutturato in funzioni di supporto, secondo il metodo augustus, dove sono rappresentate tutte le amministrazioni, gli enti e i soggetti che concorrono alla gestione dell’emergenza. La catena classica di coordinamento, in un modello puramente teorico, prevede, dal livello locale a quallo nazionale l’attivazione dei seguenti centri gerarchicamente sovraordinati: coc - centro operativo comunale, com - centro operativo misto, ccs, - centro coordinamento soccorsi, dicomac - direzione comando e controllo.</t>
+          <t>Centro di protezione civile attivato sul territorio colpito dall'emergenza per garantire la gestione coordinata degli interventi. Il centro deve essere collocato in area sicura rispetto alle diverse tipologie di rischio, in una struttura idonea dal punto di vista strutturale, funzionale e logistico. È strutturato in funzioni di supporto, secondo il metodo augustus, dove sono rappresentate tutte le amministrazioni, gli enti e i soggetti che concorrono alla gestione dell'emergenza. La catena classica di coordinamento, in un modello puramente teorico, prevede, dal livello locale a quallo nazionale l'attivazione dei seguenti centri gerarchicamente sovraordinati: coc - centro operativo comunale, com - centro operativo misto, ccs, - centro coordinamento soccorsi, dicomac - direzione comando e controllo.</t>
         </is>
       </c>
       <c r="AE8" t="inlineStr">
@@ -2085,7 +2085,7 @@
       </c>
       <c r="AD11" t="inlineStr">
         <is>
-          <t>Comando del Capo di Stato Maggiore della Difesa che concorre alla Pianificazione generale della Difesa, effettua la pianificazione operativa e dirige le operazioni ed esercitazioni interforze. Sviluppa le metodologie per la simulazione degli scenari strategici e operativi, analizza le attività e contribuisce all’elaborazione della dottrina Nato e di altre organizzazioni internazionali</t>
+          <t>Comando del Capo di Stato Maggiore della Difesa che concorre alla Pianificazione generale della Difesa, effettua la pianificazione operativa e dirige le operazioni ed esercitazioni interforze. Sviluppa le metodologie per la simulazione degli scenari strategici e operativi, analizza le attività e contribuisce all'elaborazione della dottrina Nato e di altre organizzazioni internazionali</t>
         </is>
       </c>
       <c r="AE11" t="inlineStr"/>
@@ -2697,7 +2697,7 @@
       <c r="AC15" t="inlineStr"/>
       <c r="AD15" t="inlineStr">
         <is>
-          <t>In coerenza con le tipologie dei rischi di cui all'articolo 16, la Commissione nazionale per la previsione e la prevenzione dei grandi rischi e' organo di consulenza tecnico-scientifica del Dipartimento della protezione civile.</t>
+          <t>In coerenza con le tipologie dei rischi di cui all'articolo 16, la Commissione nazionale per la previsione e la prevenzione dei grandi rischi è organo di consulenza tecnico-scientifica del Dipartimento della protezione civile.</t>
         </is>
       </c>
       <c r="AE15" t="inlineStr">
@@ -2852,7 +2852,7 @@
       <c r="AC16" t="inlineStr"/>
       <c r="AD16" t="inlineStr">
         <is>
-          <t>L'Elenco nazionale del volontariato di protezione civile costituisce lo strumento operativo mediante il quale viene assicurata la partecipazione del volontariato organizzato alle attivita' di cui all'articolo 2, garantendone l'indirizzo unitario, nel rispetto delle peculiarita' dei territori, grazie a specifiche modalita' di registrazione. L'Elenco nazionale del volontariato di protezione civile e' costituito dall'insieme: a) degli elenchi territoriali del volontariato di protezione civile, istituiti presso le Regioni e le Province autonome di Trento e di Bolzano; b) dell'elenco centrale del volontariato di protezione civile, istituito presso il Dipartimento della protezione civile.</t>
+          <t>L'Elenco nazionale del volontariato di protezione civile costituisce lo strumento operativo mediante il quale viene assicurata la partecipazione del volontariato organizzato alle attivita' di cui all'articolo 2, garantendone l'indirizzo unitario, nel rispetto delle peculiarita' dei territori, grazie a specifiche modalita' di registrazione. L'Elenco nazionale del volontariato di protezione civile è costituito dall'insieme: a) degli elenchi territoriali del volontariato di protezione civile, istituiti presso le Regioni e le Province autonome di Trento e di Bolzano; b) dell'elenco centrale del volontariato di protezione civile, istituito presso il Dipartimento della protezione civile.</t>
         </is>
       </c>
       <c r="AE16" t="inlineStr">
@@ -3496,7 +3496,7 @@
       <c r="AC20" t="inlineStr"/>
       <c r="AD20" t="inlineStr">
         <is>
-          <t>La pianificazione di protezione civile ai diversi livelli territoriali e' l'attivita' di prevenzione non strutturale, basata sulle attivita' di previsione e, in particolare, di identificazione degli scenari di cui all'articolo 2, comma 2, finalizzata: a) alla definizione delle strategie operative e del modello di intervento contenente l'organizzazione delle strutture per lo svolgimento, in forma coordinata, delle attivita' di protezione civile e della risposta operativa per la gestione degli eventi calamitosi previsti o in atto, garantendo l'effettivita' delle funzioni da svolgere con particolare riguardo alle persone in condizioni di fragilita' sociale e con disabilita', in relazione agli ambiti ottimali di cui all'articolo 11, comma 3, definiti su base provinciale e comunale, quest'ultimo anche in forma aggregata; b) ad assicurare il necessario raccordo informativo con le strutture preposte all'allertamento del Servizio nazionale; c) alla definizione dei flussi di comunicazione tra le componenti e strutture operative del Servizio nazionale interessate; d) alla definizione dei meccanismi e delle procedure per la revisione e l'aggiornamento della pianificazione, per l'organizzazione di esercitazioni e per la relativa informazione alla popolazione, da assicurare anche in corso di evento;</t>
+          <t>La pianificazione di protezione civile ai diversi livelli territoriali è l'attivita' di prevenzione non strutturale, basata sulle attivita' di previsione e, in particolare, di identificazione degli scenari di cui all'articolo 2, comma 2, finalizzata: a) alla definizione delle strategie operative e del modello di intervento contenente l'organizzazione delle strutture per lo svolgimento, in forma coordinata, delle attivita' di protezione civile e della risposta operativa per la gestione degli eventi calamitosi previsti o in atto, garantendo l'effettivita' delle funzioni da svolgere con particolare riguardo alle persone in condizioni di fragilita' sociale e con disabilita', in relazione agli ambiti ottimali di cui all'articolo 11, comma 3, definiti su base provinciale e comunale, quest'ultimo anche in forma aggregata; b) ad assicurare il necessario raccordo informativo con le strutture preposte all'allertamento del Servizio nazionale; c) alla definizione dei flussi di comunicazione tra le componenti e strutture operative del Servizio nazionale interessate; d) alla definizione dei meccanismi e delle procedure per la revisione e l'aggiornamento della pianificazione, per l'organizzazione di esercitazioni e per la relativa informazione alla popolazione, da assicurare anche in corso di evento;</t>
         </is>
       </c>
       <c r="AE20" t="inlineStr"/>
@@ -4112,7 +4112,7 @@
       <c r="AC24" t="inlineStr"/>
       <c r="AD24" t="inlineStr">
         <is>
-          <t>Può intendersi la stima – quantitativa o qualitativa – della tipologia, del volume (o dell’area) nonché della distribuzione delle frane esistenti o che potrebbero verificarsi all’interno di una ben determinata area. La suscettibilità potrebbe anche includere una descrizione della velocità e della intensità delle frane esistenti o potenziali.</t>
+          <t>Può intendersi la stima – quantitativa o qualitativa – della tipologia, del volume (o dell'area) nonché della distribuzione delle frane esistenti o che potrebbero verificarsi all'interno di una ben determinata area. La suscettibilità potrebbe anche includere una descrizione della velocità e della intensità delle frane esistenti o potenziali.</t>
         </is>
       </c>
       <c r="AE24" t="inlineStr">
@@ -4420,7 +4420,7 @@
           <t>Nel caso in cui si delinea o si è verificato un evento di portata nazionale rilevante per la protezione della popolazione, lo SMFP assume i compiti seguenti (art. 4, cpv. 2 OSMFP):
 - assicura lo scambio di informazioni e il coordinamento con altri stati maggiori e organi della Confederazione e dei Cantoni, con i gestori di infrastrutture critiche e con i competenti organi all'estero;
 riunisce le situazioni settoriali e parziali per ottenere un quadro generale della situazione e ne effettua la valutazione.
-- elabora le basi decisionali all’attenzione del Consiglio federale, del dipartimento o dell’ufficio competente;
+- elabora le basi decisionali all'attenzione del Consiglio federale, del dipartimento o dell'ufficio competente;
 - coordina le conoscenze degli esperti a livello federale;
 - coordina l'impiego delle risorse nazionali e internazionali.
 Lo SMFP si compone di una conferenza dei direttori, un elemento di pianificazione formato da esperti degli organi competenti e un elemento d'intervento e di supporto.</t>
@@ -4559,7 +4559,7 @@
       </c>
       <c r="AD27" t="inlineStr">
         <is>
-          <t>Il Servizio nazionale della protezione civile, di seguito Servizio nazionale, definito di pubblica utilita', e' il sistema che esercita la funzione di protezione civile costituita dall'insieme delle competenze e delle attivita' volte a tutelare la vita, l'integrita' fisica, i beni, gli insediamenti, gli animali e l'ambiente dai danni o dal pericolo di danni derivanti da eventi calamitosi di origine naturale o derivanti dall'attivita' dell'uomo.</t>
+          <t>Il Servizio nazionale della protezione civile, di seguito Servizio nazionale, definito di pubblica utilita', è il sistema che esercita la funzione di protezione civile costituita dall'insieme delle competenze e delle attivita' volte a tutelare la vita, l'integrita' fisica, i beni, gli insediamenti, gli animali e l'ambiente dai danni o dal pericolo di danni derivanti da eventi calamitosi di origine naturale o derivanti dall'attivita' dell'uomo.</t>
         </is>
       </c>
       <c r="AE27" t="inlineStr">
@@ -4606,7 +4606,7 @@
       <c r="AN27" t="inlineStr"/>
       <c r="AO27" t="inlineStr">
         <is>
-          <t>La protezione civile protegge la popolazione, assiste le persone in cerca di protezione, protegge i beni culturali, sostiene gli organi di condotta e le altre organizzazioni partner nonché svolge lavori di ripristino e di pubblica utilità. Essa è un’organizzazione civile che opera singolarmente o in maniera coordinata, come organizzazione partner, all'interno della struttura svizzera di di protezione della popolazione.</t>
+          <t>La protezione civile protegge la popolazione, assiste le persone in cerca di protezione, protegge i beni culturali, sostiene gli organi di condotta e le altre organizzazioni partner nonché svolge lavori di ripristino e di pubblica utilità. Essa è un'organizzazione civile che opera singolarmente o in maniera coordinata, come organizzazione partner, all'interno della struttura svizzera di di protezione della popolazione.</t>
         </is>
       </c>
       <c r="AP27" t="inlineStr">
@@ -4757,11 +4757,11 @@
       <c r="AN28" t="inlineStr"/>
       <c r="AO28" t="inlineStr">
         <is>
-          <t>Il comando della protezione civile è l’organo che dirige la protezione civile, ed è generalmente costituito dal comandante della protezione civile e dai suoi sostituti. I suoi compiti fondamentali sono i seguenti:
+          <t>Il comando della protezione civile è l'organo che dirige la protezione civile, ed è generalmente costituito dal comandante della protezione civile e dai suoi sostituti. I suoi compiti fondamentali sono i seguenti:
 - condurre gli interventi
 - condurre la protezione civile dal punto di vista organizzativo, amministrativo, del personale e del materiale
 - preparare, svolgere e valutare i corsi di ripetizione
-- assicurare l’efficienza operativa di costruzioni di protezione, materiale e infrastrutture per la diffusione dell’allarme
+- assicurare l'efficienza operativa di costruzioni di protezione, materiale e infrastrutture per la diffusione dell'allarme
 - rappresentare le questioni della protezione civile presso le autorità, le organizzazioni partner, gli organi di condotta e la popolazione</t>
         </is>
       </c>
@@ -4905,7 +4905,7 @@
       <c r="AN29" t="inlineStr"/>
       <c r="AO29" t="inlineStr">
         <is>
-          <t>Si definiscono impianti di protezione i posti di comando, gli impianti d'apprestamento, i centri sanitari protetti e gli ospedali protetti. Essi vengono utilizzati soprattutto per garantire la condotta e l’operatività dei mezzi della protezione della popolazione.</t>
+          <t>Si definiscono impianti di protezione i posti di comando, gli impianti d'apprestamento, i centri sanitari protetti e gli ospedali protetti. Essi vengono utilizzati soprattutto per garantire la condotta e l'operatività dei mezzi della protezione della popolazione.</t>
         </is>
       </c>
       <c r="AP29" t="inlineStr">
@@ -5195,7 +5195,7 @@
       <c r="AC31" t="inlineStr"/>
       <c r="AD31" t="inlineStr">
         <is>
-          <t>La suscettibilità da frana è la probabilità che una frana avvenga in un territorio, sulla base delle condizioni locali. E’ una misura del grado in cui un territorio potrà essere interessato da frane, ossia una stima di “dove” le frane potranno accadere. La suscettibilità non considera la ricorrenza temporale, né la dimensione delle frane. In termini matematici, la suscettibilità da frana è comunemente espressa come la probabilità d’occorrenza spaziale di un dissesto, dato un insieme di condizioni territoriali e ambientali.</t>
+          <t>La suscettibilità da frana è la probabilità che una frana avvenga in un territorio, sulla base delle condizioni locali. È una misura del grado in cui un territorio potrà essere interessato da frane, ossia una stima di "dove" le frane potranno accadere. La suscettibilità non considera la ricorrenza temporale, né la dimensione delle frane. In termini matematici, la suscettibilità da frana è comunemente espressa come la probabilità d'occorrenza spaziale di un dissesto, dato un insieme di condizioni territoriali e ambientali.</t>
         </is>
       </c>
       <c r="AE31" t="inlineStr">
@@ -5397,7 +5397,7 @@
       <c r="AN32" t="inlineStr"/>
       <c r="AO32" t="inlineStr">
         <is>
-          <t>I pompieri sono responsabili di salvataggio e lotta contro i sinistri in generale, compresa la lotta antincendio e contro i sinistri ordinari. Intervengono anche in caso d’emissioni tossiche, fuoriuscite di carburanti e contaminazioni radioattive. Sono un mezzo di primo intervento.</t>
+          <t>I pompieri sono responsabili di salvataggio e lotta contro i sinistri in generale, compresa la lotta antincendio e contro i sinistri ordinari. Intervengono anche in caso d'emissioni tossiche, fuoriuscite di carburanti e contaminazioni radioattive. Sono un mezzo di primo intervento.</t>
         </is>
       </c>
       <c r="AP32" t="inlineStr">
@@ -5739,7 +5739,7 @@
       <c r="AN34" t="inlineStr"/>
       <c r="AO34" t="inlineStr">
         <is>
-          <t>Gli organi di condotta vengono istituiti dalle autorità competenti per lo svolgimento dei seguenti compiti: a - informare la popolazione in merito ai pericoli che la minacciano come pure alle possibilità e alle misure di protezione esistenti; b - avvertire, dare l’allarme e impartire alla popolazione istruzioni sul comportamento; c - assicurare le attività di condotta; d - coordinare i preparativi e gli interventi delle 
+          <t>Gli organi di condotta vengono istituiti dalle autorità competenti per lo svolgimento dei seguenti compiti: a - informare la popolazione in merito ai pericoli che la minacciano come pure alle possibilità e alle misure di protezione esistenti; b - avvertire, dare l'allarme e impartire alla popolazione istruzioni sul comportamento; c - assicurare le attività di condotta; d - coordinare i preparativi e gli interventi delle 
  organizzazioni partner; e - garantire, tempestivamente e in funzione della situazione, la disponibilità operativa e il rinforzo con personale e materiale della protezione della popolazione in vista di un conflitto armato.</t>
         </is>
       </c>
@@ -5919,7 +5919,7 @@
       <c r="AN35" t="inlineStr"/>
       <c r="AO35" t="inlineStr">
         <is>
-          <t>Si ha stato di necessità quando, a seguito di catastrofi, conflitti armati o altre situazioni d’emergenza che comportano un pericolo imminente per lo Stato, le persone o le cose, non sia più possibile garantire con i mezzi ordinari l’attività amministrativa o i servizi d’interesse pubblico e la protezione e l’assistenza delle persone e delle cose a livello cantonale, regionale o locale.</t>
+          <t>Si ha stato di necessità quando, a seguito di catastrofi, conflitti armati o altre situazioni d'emergenza che comportano un pericolo imminente per lo Stato, le persone o le cose, non sia più possibile garantire con i mezzi ordinari l'attività amministrativa o i servizi d'interesse pubblico e la protezione e l'assistenza delle persone e delle cose a livello cantonale, regionale o locale.</t>
         </is>
       </c>
       <c r="AP35" t="inlineStr"/>
@@ -6066,7 +6066,7 @@
       <c r="AN36" t="inlineStr"/>
       <c r="AO36" t="inlineStr">
         <is>
-          <t>Sono impianti di protezione: a - i posti di comando; b. gli impianti d’apprestamento; c - i centri sanitari protetti; d - gli ospedali protetti.</t>
+          <t>Sono impianti di protezione: a - i posti di comando; b. gli impianti d'apprestamento; c - i centri sanitari protetti; d - gli ospedali protetti.</t>
         </is>
       </c>
       <c r="AP36" t="inlineStr"/>
@@ -6793,7 +6793,7 @@
       </c>
       <c r="AO41" t="inlineStr">
         <is>
-          <t>L’Organizzazione degli Stati maggiori di condotta (OSMC) è composta dai rappresentanti della Polizia cantonale, della Federazione cantonale ticinese corpi pompieri, della Federazione cantonale ticinese servizi autoambulanze, del Servizio della protezione civile cantonale, dei servizi tecnici e del Dipartimento delle istituzioni; ogni organizzazione designa il proprio rappresentante. A seconda delle necessità possono essere designati ulteriori responsabili per i servizi tecnici. L’OSMC è diretta dal rappresentante del Dipartimento.</t>
+          <t>L'Organizzazione degli Stati maggiori di condotta (OSMC) è composta dai rappresentanti della Polizia cantonale, della Federazione cantonale ticinese corpi pompieri, della Federazione cantonale ticinese servizi autoambulanze, del Servizio della protezione civile cantonale, dei servizi tecnici e del Dipartimento delle istituzioni; ogni organizzazione designa il proprio rappresentante. A seconda delle necessità possono essere designati ulteriori responsabili per i servizi tecnici. L'OSMC è diretta dal rappresentante del Dipartimento.</t>
         </is>
       </c>
       <c r="AP41" t="inlineStr">
@@ -7094,7 +7094,7 @@
       </c>
       <c r="AO43" t="inlineStr">
         <is>
-          <t>Lo SMCC è l’organo cantonale di condotta del Consiglio di Stato, che ne definisce la composizione, l’organizzazione e il funzionamento. Esso elabora le basi decisionali per il Consiglio di Stato, lo coadiuva nelle funzioni di direzione e coordinamento ed esegue le sue decisioni. Esso è competente quando le circostanze lo esigono, per predisporre e coordinare, in collaborazione con le autorità locali, le necessarie misure d’urgenza e di assistenza e condurne l’attuazione. La sua attivazione è decisa dal Comandante della Polizia cantonale; in caso di impedimento di questo e in successione, dal suo sostituto o dall’ufficiale di picchetto della Polizia cantonale.</t>
+          <t>Lo SMCC è l'organo cantonale di condotta del Consiglio di Stato, che ne definisce la composizione, l'organizzazione e il funzionamento. Esso elabora le basi decisionali per il Consiglio di Stato, lo coadiuva nelle funzioni di direzione e coordinamento ed esegue le sue decisioni. Esso è competente quando le circostanze lo esigono, per predisporre e coordinare, in collaborazione con le autorità locali, le necessarie misure d'urgenza e di assistenza e condurne l'attuazione. La sua attivazione è decisa dal Comandante della Polizia cantonale; in caso di impedimento di questo e in successione, dal suo sostituto o dall'ufficiale di picchetto della Polizia cantonale.</t>
         </is>
       </c>
       <c r="AP43" t="inlineStr">
@@ -7368,7 +7368,7 @@
       <c r="AN45" t="inlineStr"/>
       <c r="AO45" t="inlineStr">
         <is>
-          <t>Il segnale d'allarme acqua viene emesso esclusivamente nelle regioni minacciate a valle di impianti d'accumulazione. Le sirene emettono dodici suoni continui e gravi in sequenze di 20 secondi e a intervalli di 10 secondi. L’allarme acqua esorta la popolazione ad abbandonare immediatamente la regione minacciata.</t>
+          <t>Il segnale d'allarme acqua viene emesso esclusivamente nelle regioni minacciate a valle di impianti d'accumulazione. Le sirene emettono dodici suoni continui e gravi in sequenze di 20 secondi e a intervalli di 10 secondi. L'allarme acqua esorta la popolazione ad abbandonare immediatamente la regione minacciata.</t>
         </is>
       </c>
       <c r="AP45" t="inlineStr"/>
@@ -7662,7 +7662,7 @@
       </c>
       <c r="AO47" t="inlineStr">
         <is>
-          <t>Lo SMEPI coordina l’intervento dei primi enti mobilitati, di regola polizia, pompieri e servizi d’autoambulanza. Esso è condotto, di principio, dalla Polizia cantonale.</t>
+          <t>Lo SMEPI coordina l'intervento dei primi enti mobilitati, di regola polizia, pompieri e servizi d'autoambulanza. Esso è condotto, di principio, dalla Polizia cantonale.</t>
         </is>
       </c>
       <c r="AP47" t="inlineStr"/>
@@ -7798,7 +7798,7 @@
       </c>
       <c r="AD48" t="inlineStr">
         <is>
-          <t>Il Servizio nazionale della protezione civile, di seguito Servizio nazionale, definito di pubblica utilita', e' il sistema che esercita la funzione di protezione civile costituita dall'insieme delle competenze e delle attivita' volte a tutelare la vita, l'integrita' fisica, i beni, gli insediamenti, gli animali e l'ambiente dai danni o dal pericolo di danni derivanti da eventi calamitosi di origine naturale o derivanti dall'attivita' dell'uomo.</t>
+          <t>Il Servizio nazionale della protezione civile, di seguito Servizio nazionale, definito di pubblica utilita', è il sistema che esercita la funzione di protezione civile costituita dall'insieme delle competenze e delle attivita' volte a tutelare la vita, l'integrita' fisica, i beni, gli insediamenti, gli animali e l'ambiente dai danni o dal pericolo di danni derivanti da eventi calamitosi di origine naturale o derivanti dall'attivita' dell'uomo.</t>
         </is>
       </c>
       <c r="AE48" t="inlineStr">
@@ -7846,7 +7846,7 @@
       <c r="AO48" t="inlineStr">
         <is>
           <t>Il servizio della protezione della popolazione si occupa prevalentemente dei preparativi per i casi di emergenza e di catastrofe.
-Assicura la collaborazione con i servizi delle Amministrazioni: federale, cantonale e comunali direttamente collegate con i temi trattati dal servizio e si occupa della coordinazione fra i partner del concetto “protezione della popolazione” (polizia cantonale, Federazione cantonale ticinese dei Corpi Pompieri, Federazione cantonale ticinese dei Servizi autoambulanze, organizzazioni regionali di protezione civile, servizi tecnici cantonali, servizi dello Stato Maggiore cantonale di catastrofe, ecc…).
+Assicura la collaborazione con i servizi delle Amministrazioni: federale, cantonale e comunali direttamente collegate con i temi trattati dal servizio e si occupa della coordinazione fra i partner del concetto "protezione della popolazione" (polizia cantonale, Federazione cantonale ticinese dei Corpi Pompieri, Federazione cantonale ticinese dei Servizi autoambulanze, organizzazioni regionali di protezione civile, servizi tecnici cantonali, servizi dello Stato Maggiore cantonale di catastrofe, ecc…).
 Per il tramite di esercitazioni teoriche e pratiche, approfondisce con le istanze militari, la collaborazione civile-militare.</t>
         </is>
       </c>
@@ -7992,7 +7992,7 @@
       <c r="AC49" t="inlineStr"/>
       <c r="AD49" t="inlineStr">
         <is>
-          <t>Il Dipartimento della protezione civile è una struttura della Presidenza del Consiglio dei Ministri. Il Dipartimento, operando in stretto raccordo con le Regioni e le Province autonome, si occupa di tutte le attività volte alla previsione e alla prevenzione dei rischi, al soccorso e all’assistenza delle popolazioni colpite da calamità, al contrasto e al superamento dell’emergenza.</t>
+          <t>Il Dipartimento della protezione civile è una struttura della Presidenza del Consiglio dei Ministri. Il Dipartimento, operando in stretto raccordo con le Regioni e le Province autonome, si occupa di tutte le attività volte alla previsione e alla prevenzione dei rischi, al soccorso e all'assistenza delle popolazioni colpite da calamità, al contrasto e al superamento dell'emergenza.</t>
         </is>
       </c>
       <c r="AE49" t="inlineStr"/>
@@ -8309,7 +8309,7 @@
       <c r="AN51" t="inlineStr"/>
       <c r="AO51" t="inlineStr">
         <is>
-          <t>La legge LPPC 2002 stabilisce che possono prestare volontariamente servizio di protezione civile: a. gli uomini prosciolti dall’obbligo di prestare servizio nella protezione civile; b. gli uomini soggetti all’obbligo militare prosciolti dall’obbligo di prestare servizio militare o civile; c. gli uomini prosciolti dall’obbligo di prestare servizio militare o civile; d. le cittadine svizzere, a partire dall’anno in cui compiono i 20 anni; e. gli stranieri domiciliati in Svizzera, a partire dall’anno in cui compiono i 20 anni. Bisogna porre attenzione al fatto che secondo la stessa legge, l’unica differenza tra un milite e un volontario (entrambi di protezione civile) è il fatto che i volontari sono prosciolti dall’obbligo di prestare servizio su domanda. Infatti, per il resto, militi e volontari hanno gli stessi diritti e doveri. 
+          <t>La legge LPPC 2002 stabilisce che possono prestare volontariamente servizio di protezione civile: a. gli uomini prosciolti dall'obbligo di prestare servizio nella protezione civile; b. gli uomini soggetti all'obbligo militare prosciolti dall'obbligo di prestare servizio militare o civile; c. gli uomini prosciolti dall'obbligo di prestare servizio militare o civile; d. le cittadine svizzere, a partire dall'anno in cui compiono i 20 anni; e. gli stranieri domiciliati in Svizzera, a partire dall'anno in cui compiono i 20 anni. Bisogna porre attenzione al fatto che secondo la stessa legge, l'unica differenza tra un milite e un volontario (entrambi di protezione civile) è il fatto che i volontari sono prosciolti dall'obbligo di prestare servizio su domanda. Infatti, per il resto, militi e volontari hanno gli stessi diritti e doveri. 
 I diritti dei militi sono essenzialmente quattro: soldo e vitto, alloggio, trasporto gratuiti, cui si aggiungono alcune agevolazioni fiscali e indennità.</t>
         </is>
       </c>
@@ -8449,7 +8449,7 @@
       <c r="AN52" t="inlineStr"/>
       <c r="AO52" t="inlineStr">
         <is>
-          <t>Il Consiglio di Stato è l’autorità competente per: a) assicurare la condotta, l’intervento e il coordinamento delle organizzazioni partner; b) assicurare l’istruzione e la formazione, anche degli organi di condotta locali; c) promuovere l’aiuto intercomunale, così come la cooperazione intercantonale e
+          <t>Il Consiglio di Stato è l'autorità competente per: a) assicurare la condotta, l'intervento e il coordinamento delle organizzazioni partner; b) assicurare l'istruzione e la formazione, anche degli organi di condotta locali; c) promuovere l'aiuto intercomunale, così come la cooperazione intercantonale e
 transfrontaliera; d) esercitare le altre funzioni attribuitegli dalla presente legge.</t>
         </is>
       </c>
@@ -8597,8 +8597,8 @@
       <c r="AN53" t="inlineStr"/>
       <c r="AO53" t="inlineStr">
         <is>
-          <t>I militi svizzeri sono reclutati dall’esercito e dalla protezione civile e di norma vengono assegnati al loro cantone di domicilio, oppure ad altri cantoni, se deciso dal cantone di domicilio, cui comunque spetta la scelta. I militi, oltre ad essere arruolati in maniera ordinaria, possono essere incorporati nel personale di riserva. Se un milite entra a far parte del personale di riserva non deve essere necessariamente formato e non ha diritto a prestare servizio di protezione civile.
-Una volta reclutati e addestrasti, i militi possono essere chiamati a prestare servizio dal consiglio federale o dal cantone cui sono assegnati. Il Consiglio federale e il cantone di assegnamento possono chiamare in servizio i militi di protezione civile in caso di catastrofi e situazioni d’emergenza che colpiscono uno o più Cantoni, oppure le zone limitrofe di Paesi confinanti, oppure in caso di conflitto armato. I militi possono inoltre essere mobilitati anche in assenza di emergenza per svolgere dei lavori di ripristino di pubblica utilità. In quest’ultimo caso però, esistono dei limiti al potere di convocazione esercitato dalle autorità sui militi .</t>
+          <t>I militi svizzeri sono reclutati dall'esercito e dalla protezione civile e di norma vengono assegnati al loro cantone di domicilio, oppure ad altri cantoni, se deciso dal cantone di domicilio, cui comunque spetta la scelta. I militi, oltre ad essere arruolati in maniera ordinaria, possono essere incorporati nel personale di riserva. Se un milite entra a far parte del personale di riserva non deve essere necessariamente formato e non ha diritto a prestare servizio di protezione civile.
+Una volta reclutati e addestrasti, i militi possono essere chiamati a prestare servizio dal consiglio federale o dal cantone cui sono assegnati. Il Consiglio federale e il cantone di assegnamento possono chiamare in servizio i militi di protezione civile in caso di catastrofi e situazioni d'emergenza che colpiscono uno o più Cantoni, oppure le zone limitrofe di Paesi confinanti, oppure in caso di conflitto armato. I militi possono inoltre essere mobilitati anche in assenza di emergenza per svolgere dei lavori di ripristino di pubblica utilità. In quest'ultimo caso però, esistono dei limiti al potere di convocazione esercitato dalle autorità sui militi .</t>
         </is>
       </c>
       <c r="AP53" t="inlineStr"/>
@@ -8874,8 +8874,8 @@
       <c r="AO55" t="inlineStr">
         <is>
           <t>La Sezione è articolata in cinque servizi con distinte aree di competenza: il Servizio amministrativo, il Servizio degli affari militari e del comando di circondario, il Servizio della protezione civile, il Servizio costruzioni di protezione civile e il Servizio della protezione della popolazione. 
-Il servizio amministrativo centralizzato della sezione si occupa di fornire le prime informazioni all’utenza e di smistarle ai vari servizi di competenza. Altri compiti specifici sono la contabilità, la corrispondenza e il supporto logistico per tutta la sezione. 
-Il Servizio degli affari militari e comando di circondario si occupa delle pratiche amministrative legate ai servizi d’istruzione dei militi domiciliati in Ticino come pure degli obblighi fuori servizio (tiro obbligatorio, obbligo di notifica), tiene il controllo dei dati di servizio e di quelli personali dei militi con la collaborazione degli uffici di controllo abitanti dei comuni. 
+Il servizio amministrativo centralizzato della sezione si occupa di fornire le prime informazioni all'utenza e di smistarle ai vari servizi di competenza. Altri compiti specifici sono la contabilità, la corrispondenza e il supporto logistico per tutta la sezione. 
+Il Servizio degli affari militari e comando di circondario si occupa delle pratiche amministrative legate ai servizi d'istruzione dei militi domiciliati in Ticino come pure degli obblighi fuori servizio (tiro obbligatorio, obbligo di notifica), tiene il controllo dei dati di servizio e di quelli personali dei militi con la collaborazione degli uffici di controllo abitanti dei comuni. 
 Il Servizio della protezione civile, unitamente al Centro istruzione della protezione civile di Rivera, assicura l'applicazione delle norme federali e cantonali di protezione civile nelle regioni e nei comuni, cura le diverse pianificazioni (allarmi, approvvigionamenti,...) e l'istruzione dei militi astretti.
 Il Servizio costruzioni si occupa della pianificazione e gestione dei posti protetti, come pure della realizzazione delle costruzioni protette (rifugi, impianti regionali).
 Il servizio della protezione della popolazione si occupa prevalentemente dei preparativi per i casi di emergenza e di catastrofe.</t>
@@ -9431,7 +9431,7 @@
       </c>
       <c r="AD59" t="inlineStr">
         <is>
-          <t>team transfrontaliero di coordinamento costituito congiuntamente da personale qualificato, formato e attrezzato, della protezione civile lombarda e ticinese. Esso ha il compito, durante le emergenze nei territori di confine, di operare insieme sia per la valutazione dell’evento in corso e per i reciproci possibili riflessi sui rispettivi territori, sia quali “ufficiali di collegamento” per collegare le rispettive sale operative di ambo i lati del confine, consentendo una efficiente ed efficace relazione operativa. Il NUVRE viene introdotto dal progetto Gestisco 2018-2021.</t>
+          <t>team transfrontaliero di coordinamento costituito congiuntamente da personale qualificato, formato e attrezzato, della protezione civile lombarda e ticinese. Esso ha il compito, durante le emergenze nei territori di confine, di operare insieme sia per la valutazione dell'evento in corso e per i reciproci possibili riflessi sui rispettivi territori, sia quali "ufficiali di collegamento" per collegare le rispettive sale operative di ambo i lati del confine, consentendo una efficiente ed efficace relazione operativa. Il NUVRE viene introdotto dal progetto Gestisco 2018-2021.</t>
         </is>
       </c>
       <c r="AE59" t="inlineStr"/>
@@ -9563,7 +9563,7 @@
       <c r="AD60" t="inlineStr">
         <is>
           <t>(ex. Centro Situazioni - CESI) La Sala Situazione Italia del Dipartimento della Protezione civile è un centro di coordinamento nazionale che raccoglie, verifica e diffonde le informazioni di protezione civile. Ha il compito di individuare le situazioni emergenziali e allertare immediatamente le diverse componenti e strutture operative del Servizio nazionale della protezione civile che concorrono alla gestione delle emergenze.
-Opera 24 ore su 24, tutti i giorni dell'anno, e vi partecipano il Dipartimento della Protezione civile e le strutture operative del Servizio nazionale della protezione civile. Si mantiene in costante raccordo con le regioni e le prefetture, e con gli operatori delle strutture di comunicazione - es. compagnie di telecomunicazioni, centri di primo soccorso, autostrade, ferrovie - con l’obiettivo di raccogliere e diffondere, in tempo reale, notizie sulle situazioni di emergenza e gli interventi in corso, a livello nazionale e locale.</t>
+Opera 24 ore su 24, tutti i giorni dell'anno, e vi partecipano il Dipartimento della Protezione civile e le strutture operative del Servizio nazionale della protezione civile. Si mantiene in costante raccordo con le regioni e le prefetture, e con gli operatori delle strutture di comunicazione - es. compagnie di telecomunicazioni, centri di primo soccorso, autostrade, ferrovie - con l'obiettivo di raccogliere e diffondere, in tempo reale, notizie sulle situazioni di emergenza e gli interventi in corso, a livello nazionale e locale.</t>
         </is>
       </c>
       <c r="AE60" t="inlineStr"/>
@@ -9857,7 +9857,7 @@
       </c>
       <c r="AD62" t="inlineStr">
         <is>
-          <t>I centri assistenziali di pronto intervento sono delle strutture operative permanenti costituita da magazzini per lo stoccaggio di materiale assistenziale e di pronto intervento da utilizzare in eventi calamitosi in Italia e all’estero Le finalità del centro sono quelle di acquisire, stoccare e mantenere efficienti i mezzi e le attrezzature per fronteggiare le emergenze nel più breve tempo possibile e nel miglior modo possibile.</t>
+          <t>I centri assistenziali di pronto intervento sono delle strutture operative permanenti costituita da magazzini per lo stoccaggio di materiale assistenziale e di pronto intervento da utilizzare in eventi calamitosi in Italia e all'estero Le finalità del centro sono quelle di acquisire, stoccare e mantenere efficienti i mezzi e le attrezzature per fronteggiare le emergenze nel più breve tempo possibile e nel miglior modo possibile.</t>
         </is>
       </c>
       <c r="AE62" t="inlineStr"/>

</xml_diff>